<commit_message>
Enabled XLSX to Tox-To-MDI workflow.
</commit_message>
<xml_diff>
--- a/MDI-To-EDRS-Template.xlsx
+++ b/MDI-To-EDRS-Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mriley7\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mriley7\workspace\raven-import-and-submit-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE67D22F-79E4-4C12-BCDB-447B2AE0AFDD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA7019D1-ED79-4310-9BF2-27319FFB7C4A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{7A50F290-1C75-487E-9806-F93553E4E7CC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8484" xr2:uid="{7A50F290-1C75-487E-9806-F93553E4E7CC}"/>
   </bookViews>
   <sheets>
     <sheet name="MDI RAVEN Input Schema" sheetId="4" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="174">
   <si>
     <t>Manner of Death</t>
   </si>
@@ -148,9 +148,6 @@
     <t>Location of death</t>
   </si>
   <si>
-    <t>Jurisdiction</t>
-  </si>
-  <si>
     <t>Place of death</t>
   </si>
   <si>
@@ -311,9 +308,6 @@
   </si>
   <si>
     <t>End of Cases</t>
-  </si>
-  <si>
-    <t>Certifier</t>
   </si>
   <si>
     <t>Certifier Name</t>
@@ -534,6 +528,9 @@
   </si>
   <si>
     <t>This section describes the autopsy findings, if an autopsy occurred.</t>
+  </si>
+  <si>
+    <t>This section describes the primary Chief Medical Examiner or Coroner associated to the case.</t>
   </si>
   <si>
     <t xml:space="preserve">Name of the Medical Examiner.
@@ -655,30 +652,23 @@
     </r>
   </si>
   <si>
-    <t>GTRI</t>
-  </si>
-  <si>
-    <t>This section describes the primary Medical Examiner or Coroner associated to the case.</t>
-  </si>
-  <si>
-    <t>This section describes the certifier of the case, if the case has been certified. Oftentimes, the Medical Examiner/Coroner and the Certifier can be the same party. If the case is not certified, leave blank</t>
-  </si>
-  <si>
-    <t>Pronouncer of death</t>
-  </si>
-  <si>
-    <t>The person who is pronouncing the place and time of death. 
-Accepted Formats:
-&lt;First Name&gt; &lt;Last Name&gt;
-&lt;First Name&gt; &lt;Middle Initial&gt; &lt;Last Name&gt;
-&lt;First Name&gt; &lt;Middle Name&gt; &lt;Last Name&gt;</t>
+    <t>INVALID</t>
+  </si>
+  <si>
+    <t>Death Pronouncement</t>
+  </si>
+  <si>
+    <t>Death Certifier</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
+  </numFmts>
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -750,15 +740,8 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="23">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -862,30 +845,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFC9C9C9"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF1C67F"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF5D5A1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6E0B4"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFB3"/>
-        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -994,7 +953,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -1024,6 +983,10 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
@@ -1031,6 +994,18 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
@@ -1038,11 +1013,35 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -1060,6 +1059,10 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
@@ -1067,6 +1070,13 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
@@ -1074,6 +1084,10 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
@@ -1081,6 +1095,18 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="14" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
@@ -1088,6 +1114,10 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
@@ -1102,6 +1132,10 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
@@ -1109,18 +1143,8 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
@@ -1133,13 +1157,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
@@ -1152,7 +1173,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1189,8 +1209,65 @@
     <xf numFmtId="0" fontId="7" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="14" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1235,12 +1312,6 @@
     <xf numFmtId="0" fontId="9" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1268,162 +1339,8 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="11" fillId="21" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="11" fillId="21" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="18" fontId="11" fillId="21" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="18" fontId="11" fillId="21" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="20" fontId="11" fillId="21" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="11" fillId="22" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="11" fillId="22" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="18" fontId="11" fillId="22" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="18" fontId="11" fillId="22" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="4" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="4" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1437,9 +1354,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFC9C9C9"/>
       <color rgb="FFF5D5A1"/>
       <color rgb="FFF1C67F"/>
-      <color rgb="FFC9C9C9"/>
       <color rgb="FF9F9F9F"/>
       <color rgb="FFFFB9AB"/>
       <color rgb="FFFF856D"/>
@@ -1761,74 +1678,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54CD1DC7-E143-4CF5-BEA9-4DABBAFFC7B0}">
-  <dimension ref="A1:I65"/>
+  <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" style="37" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" style="52" customWidth="1"/>
-    <col min="3" max="3" width="38.44140625" style="61" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" style="53" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" style="65" customWidth="1"/>
+    <col min="3" max="3" width="38.44140625" style="73" customWidth="1"/>
     <col min="4" max="8" width="32.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="52" t="s">
-        <v>99</v>
-      </c>
-      <c r="C1" s="61" t="s">
+      <c r="B1" s="65" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="73" t="s">
         <v>27</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="F1" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>155</v>
-      </c>
       <c r="I1" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="23.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C2" s="61" t="s">
-        <v>102</v>
+      <c r="C2" s="73" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="109.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="53" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3" s="121" t="s">
+        <v>171</v>
+      </c>
+      <c r="C3" s="122" t="s">
         <v>170</v>
       </c>
-      <c r="B3" s="97" t="s">
-        <v>172</v>
-      </c>
-      <c r="C3" s="98" t="s">
-        <v>171</v>
-      </c>
     </row>
     <row r="4" spans="1:9" s="4" customFormat="1" ht="34.799999999999997" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="74" t="s">
-        <v>103</v>
+      <c r="B4" s="66"/>
+      <c r="C4" s="100" t="s">
+        <v>101</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -1838,899 +1755,869 @@
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" s="6" customFormat="1" ht="29.4" x14ac:dyDescent="0.5">
-      <c r="A5" s="39"/>
-      <c r="B5" s="94" t="s">
+      <c r="A5" s="55"/>
+      <c r="B5" s="118" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="101" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" s="6" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A6" s="55"/>
+      <c r="B6" s="119" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="75" t="s">
+      <c r="C6" s="101" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" s="8" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A7" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="67"/>
+      <c r="C7" s="102" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+    </row>
+    <row r="8" spans="1:9" s="11" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
+      <c r="A8" s="57"/>
+      <c r="B8" s="74" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="103" t="s">
         <v>104</v>
       </c>
-      <c r="D5" s="109"/>
-      <c r="E5" s="109"/>
-      <c r="F5" s="109"/>
-      <c r="G5" s="109"/>
-      <c r="H5" s="109"/>
-      <c r="I5" s="5"/>
-    </row>
-    <row r="6" spans="1:9" s="6" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A6" s="39"/>
-      <c r="B6" s="95" t="s">
+      <c r="D8" s="14"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="10"/>
+    </row>
+    <row r="9" spans="1:9" s="11" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A9" s="57"/>
+      <c r="B9" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="103" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="10"/>
+    </row>
+    <row r="10" spans="1:9" s="11" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A10" s="57"/>
+      <c r="B10" s="74" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="103" t="s">
+        <v>107</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="10"/>
+    </row>
+    <row r="11" spans="1:9" s="11" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A11" s="57"/>
+      <c r="B11" s="75" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="103" t="s">
+        <v>106</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="10"/>
+    </row>
+    <row r="12" spans="1:9" s="11" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A12" s="57"/>
+      <c r="B12" s="74" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="103" t="s">
+        <v>155</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="10"/>
+    </row>
+    <row r="13" spans="1:9" s="11" customFormat="1" ht="57" x14ac:dyDescent="0.5">
+      <c r="A13" s="57"/>
+      <c r="B13" s="74" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="103" t="s">
+        <v>109</v>
+      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="10"/>
+    </row>
+    <row r="14" spans="1:9" s="11" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A14" s="57"/>
+      <c r="B14" s="74" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="103" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" s="85"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="10"/>
+    </row>
+    <row r="15" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="57"/>
+      <c r="B15" s="74" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="103"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="10"/>
+    </row>
+    <row r="16" spans="1:9" s="11" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A16" s="57"/>
+      <c r="B16" s="74" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="103" t="s">
+        <v>111</v>
+      </c>
+      <c r="D16" s="86"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="10"/>
+    </row>
+    <row r="17" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="57"/>
+      <c r="B17" s="74" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="103"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="10"/>
+    </row>
+    <row r="18" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="57"/>
+      <c r="B18" s="74" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="103"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="10"/>
+    </row>
+    <row r="19" spans="1:9" s="11" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
+      <c r="A19" s="57"/>
+      <c r="B19" s="76" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="103"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="10"/>
+    </row>
+    <row r="20" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A20" s="57"/>
+      <c r="B20" s="74" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="103"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="10"/>
+    </row>
+    <row r="21" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A21" s="57"/>
+      <c r="B21" s="74" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="103"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="10"/>
+    </row>
+    <row r="22" spans="1:9" s="16" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
+      <c r="A22" s="114" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="68"/>
+      <c r="C22" s="104" t="s">
+        <v>112</v>
+      </c>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+    </row>
+    <row r="23" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A23" s="58"/>
+      <c r="B23" s="120" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="105" t="s">
+        <v>113</v>
+      </c>
+      <c r="D23" s="87"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="18"/>
+    </row>
+    <row r="24" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A24" s="58"/>
+      <c r="B24" s="120" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="105" t="s">
+        <v>114</v>
+      </c>
+      <c r="D24" s="88"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="18"/>
+    </row>
+    <row r="25" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A25" s="58"/>
+      <c r="B25" s="120" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="105" t="s">
+        <v>115</v>
+      </c>
+      <c r="D25" s="89"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="18"/>
+    </row>
+    <row r="26" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A26" s="58"/>
+      <c r="B26" s="120" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="105" t="s">
+        <v>116</v>
+      </c>
+      <c r="D26" s="89"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="18"/>
+    </row>
+    <row r="27" spans="1:9" s="19" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A27" s="58"/>
+      <c r="B27" s="120" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="105" t="s">
+        <v>117</v>
+      </c>
+      <c r="D27" s="89"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="18"/>
+    </row>
+    <row r="28" spans="1:9" s="19" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A28" s="58"/>
+      <c r="B28" s="120" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="105" t="s">
+        <v>118</v>
+      </c>
+      <c r="D28" s="89"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="18"/>
+    </row>
+    <row r="29" spans="1:9" s="19" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A29" s="58"/>
+      <c r="B29" s="120" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="105" t="s">
+        <v>119</v>
+      </c>
+      <c r="D29" s="89"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="18"/>
+    </row>
+    <row r="30" spans="1:9" s="19" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A30" s="58"/>
+      <c r="B30" s="120" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="105" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30" s="87"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="18"/>
+    </row>
+    <row r="31" spans="1:9" s="19" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A31" s="58"/>
+      <c r="B31" s="120" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="105" t="s">
+        <v>121</v>
+      </c>
+      <c r="D31" s="90"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="18"/>
+    </row>
+    <row r="32" spans="1:9" s="19" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A32" s="58"/>
+      <c r="B32" s="77" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="105" t="s">
+        <v>122</v>
+      </c>
+      <c r="D32" s="90"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="18"/>
+    </row>
+    <row r="33" spans="1:9" s="19" customFormat="1" ht="57" x14ac:dyDescent="0.5">
+      <c r="A33" s="58"/>
+      <c r="B33" s="77" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="105" t="s">
+        <v>123</v>
+      </c>
+      <c r="D33" s="91"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="18"/>
+    </row>
+    <row r="34" spans="1:9" s="19" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
+      <c r="A34" s="58"/>
+      <c r="B34" s="77" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34" s="105" t="s">
+        <v>124</v>
+      </c>
+      <c r="D34" s="90"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="18"/>
+    </row>
+    <row r="35" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A35" s="59"/>
+      <c r="B35" s="77" t="s">
+        <v>82</v>
+      </c>
+      <c r="C35" s="105" t="s">
+        <v>125</v>
+      </c>
+      <c r="D35" s="89"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="25"/>
+    </row>
+    <row r="36" spans="1:9" s="19" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A36" s="58"/>
+      <c r="B36" s="77" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="105" t="s">
+        <v>126</v>
+      </c>
+      <c r="D36" s="90"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="18"/>
+    </row>
+    <row r="37" spans="1:9" s="19" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A37" s="58"/>
+      <c r="B37" s="77" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" s="105" t="s">
+        <v>127</v>
+      </c>
+      <c r="D37" s="90"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="18"/>
+    </row>
+    <row r="38" spans="1:9" s="28" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
+      <c r="A38" s="115" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="69"/>
+      <c r="C38" s="106" t="s">
+        <v>143</v>
+      </c>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="27"/>
+    </row>
+    <row r="39" spans="1:9" s="31" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A39" s="60"/>
+      <c r="B39" s="78" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" s="107" t="s">
+        <v>128</v>
+      </c>
+      <c r="D39" s="92"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="29"/>
+      <c r="G39" s="29"/>
+      <c r="H39" s="29"/>
+      <c r="I39" s="30"/>
+    </row>
+    <row r="40" spans="1:9" s="31" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A40" s="60"/>
+      <c r="B40" s="79" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" s="107" t="s">
+        <v>166</v>
+      </c>
+      <c r="D40" s="92"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="32"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="32"/>
+      <c r="I40" s="30"/>
+    </row>
+    <row r="41" spans="1:9" s="31" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A41" s="60"/>
+      <c r="B41" s="78" t="s">
+        <v>77</v>
+      </c>
+      <c r="C41" s="107" t="s">
+        <v>129</v>
+      </c>
+      <c r="D41" s="92"/>
+      <c r="E41" s="92"/>
+      <c r="F41" s="92"/>
+      <c r="G41" s="92"/>
+      <c r="H41" s="92"/>
+      <c r="I41" s="30"/>
+    </row>
+    <row r="42" spans="1:9" s="31" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A42" s="60"/>
+      <c r="B42" s="117" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="107" t="s">
+        <v>130</v>
+      </c>
+      <c r="D42" s="92"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="29"/>
+      <c r="G42" s="29"/>
+      <c r="H42" s="29"/>
+      <c r="I42" s="30"/>
+    </row>
+    <row r="43" spans="1:9" s="35" customFormat="1" ht="57" x14ac:dyDescent="0.5">
+      <c r="A43" s="123" t="s">
+        <v>172</v>
+      </c>
+      <c r="B43" s="70"/>
+      <c r="C43" s="108" t="s">
+        <v>144</v>
+      </c>
+      <c r="D43" s="93"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="33"/>
+      <c r="G43" s="33"/>
+      <c r="H43" s="33"/>
+      <c r="I43" s="34"/>
+    </row>
+    <row r="44" spans="1:9" s="38" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A44" s="61"/>
+      <c r="B44" s="80" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" s="109" t="s">
+        <v>131</v>
+      </c>
+      <c r="D44" s="94"/>
+      <c r="E44" s="36"/>
+      <c r="F44" s="36"/>
+      <c r="G44" s="36"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="37"/>
+    </row>
+    <row r="45" spans="1:9" s="38" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
+      <c r="A45" s="61"/>
+      <c r="B45" s="80" t="s">
+        <v>22</v>
+      </c>
+      <c r="C45" s="109" t="s">
+        <v>132</v>
+      </c>
+      <c r="D45" s="95"/>
+      <c r="E45" s="39"/>
+      <c r="F45" s="39"/>
+      <c r="G45" s="39"/>
+      <c r="H45" s="39"/>
+      <c r="I45" s="37"/>
+    </row>
+    <row r="46" spans="1:9" s="38" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A46" s="61"/>
+      <c r="B46" s="80" t="s">
+        <v>78</v>
+      </c>
+      <c r="C46" s="109" t="s">
+        <v>137</v>
+      </c>
+      <c r="D46" s="96"/>
+      <c r="E46" s="40"/>
+      <c r="F46" s="40"/>
+      <c r="G46" s="40"/>
+      <c r="H46" s="40"/>
+      <c r="I46" s="37"/>
+    </row>
+    <row r="47" spans="1:9" s="38" customFormat="1" ht="57" x14ac:dyDescent="0.5">
+      <c r="A47" s="61"/>
+      <c r="B47" s="80" t="s">
+        <v>23</v>
+      </c>
+      <c r="C47" s="109" t="s">
+        <v>138</v>
+      </c>
+      <c r="D47" s="97"/>
+      <c r="E47" s="41"/>
+      <c r="F47" s="41"/>
+      <c r="G47" s="41"/>
+      <c r="H47" s="41"/>
+      <c r="I47" s="37"/>
+    </row>
+    <row r="48" spans="1:9" s="38" customFormat="1" ht="91.2" x14ac:dyDescent="0.5">
+      <c r="A48" s="61"/>
+      <c r="B48" s="80" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48" s="109" t="s">
+        <v>139</v>
+      </c>
+      <c r="D48" s="95"/>
+      <c r="E48" s="39"/>
+      <c r="F48" s="39"/>
+      <c r="G48" s="39"/>
+      <c r="H48" s="39"/>
+      <c r="I48" s="37"/>
+    </row>
+    <row r="49" spans="1:9" s="38" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A49" s="61"/>
+      <c r="B49" s="80" t="s">
+        <v>40</v>
+      </c>
+      <c r="C49" s="109" t="s">
+        <v>140</v>
+      </c>
+      <c r="D49" s="96"/>
+      <c r="E49" s="40"/>
+      <c r="F49" s="40"/>
+      <c r="G49" s="40"/>
+      <c r="H49" s="40"/>
+      <c r="I49" s="37"/>
+    </row>
+    <row r="50" spans="1:9" s="43" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A50" s="62" t="s">
+        <v>44</v>
+      </c>
+      <c r="B50" s="71"/>
+      <c r="C50" s="110" t="s">
+        <v>145</v>
+      </c>
+      <c r="D50" s="42"/>
+      <c r="E50" s="42"/>
+      <c r="F50" s="42"/>
+      <c r="G50" s="42"/>
+      <c r="H50" s="42"/>
+      <c r="I50" s="42"/>
+    </row>
+    <row r="51" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A51" s="63"/>
+      <c r="B51" s="81" t="s">
+        <v>45</v>
+      </c>
+      <c r="C51" s="111" t="s">
+        <v>141</v>
+      </c>
+      <c r="D51" s="98"/>
+      <c r="E51" s="44"/>
+      <c r="F51" s="44"/>
+      <c r="G51" s="44"/>
+      <c r="H51" s="44"/>
+      <c r="I51" s="45"/>
+    </row>
+    <row r="52" spans="1:9" s="46" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A52" s="63"/>
+      <c r="B52" s="81" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="75" t="s">
-        <v>105</v>
-      </c>
-      <c r="D6" s="109"/>
-      <c r="E6" s="109"/>
-      <c r="F6" s="109"/>
-      <c r="G6" s="109"/>
-      <c r="H6" s="109"/>
-      <c r="I6" s="5"/>
-    </row>
-    <row r="7" spans="1:9" s="8" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A7" s="40" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="54"/>
-      <c r="C7" s="76" t="s">
-        <v>107</v>
-      </c>
-      <c r="D7" s="110"/>
-      <c r="E7" s="110"/>
-      <c r="F7" s="110"/>
-      <c r="G7" s="110"/>
-      <c r="H7" s="110"/>
-      <c r="I7" s="7"/>
-    </row>
-    <row r="8" spans="1:9" s="10" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
-      <c r="A8" s="41"/>
-      <c r="B8" s="62" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="77" t="s">
-        <v>106</v>
-      </c>
-      <c r="D8" s="111"/>
-      <c r="E8" s="112"/>
-      <c r="F8" s="112"/>
-      <c r="G8" s="112"/>
-      <c r="H8" s="112"/>
-      <c r="I8" s="9"/>
-    </row>
-    <row r="9" spans="1:9" s="10" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A9" s="41"/>
-      <c r="B9" s="62" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="77" t="s">
-        <v>110</v>
-      </c>
-      <c r="D9" s="111"/>
-      <c r="E9" s="112"/>
-      <c r="F9" s="112"/>
-      <c r="G9" s="112"/>
-      <c r="H9" s="112"/>
-      <c r="I9" s="9"/>
-    </row>
-    <row r="10" spans="1:9" s="10" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A10" s="41"/>
-      <c r="B10" s="62" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="77" t="s">
-        <v>109</v>
-      </c>
-      <c r="D10" s="111"/>
-      <c r="E10" s="112"/>
-      <c r="F10" s="112"/>
-      <c r="G10" s="112"/>
-      <c r="H10" s="112"/>
-      <c r="I10" s="9"/>
-    </row>
-    <row r="11" spans="1:9" s="10" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A11" s="41"/>
-      <c r="B11" s="63" t="s">
-        <v>77</v>
-      </c>
-      <c r="C11" s="77" t="s">
-        <v>108</v>
-      </c>
-      <c r="D11" s="111"/>
-      <c r="E11" s="112"/>
-      <c r="F11" s="112"/>
-      <c r="G11" s="112"/>
-      <c r="H11" s="112"/>
-      <c r="I11" s="9"/>
-    </row>
-    <row r="12" spans="1:9" s="10" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A12" s="41"/>
-      <c r="B12" s="62" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="77" t="s">
-        <v>156</v>
-      </c>
-      <c r="D12" s="111"/>
-      <c r="E12" s="112"/>
-      <c r="F12" s="112"/>
-      <c r="G12" s="112"/>
-      <c r="H12" s="112"/>
-      <c r="I12" s="9"/>
-    </row>
-    <row r="13" spans="1:9" s="10" customFormat="1" ht="57" x14ac:dyDescent="0.5">
-      <c r="A13" s="41"/>
-      <c r="B13" s="62" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="77" t="s">
-        <v>111</v>
-      </c>
-      <c r="D13" s="111"/>
-      <c r="E13" s="112"/>
-      <c r="F13" s="112"/>
-      <c r="G13" s="112"/>
-      <c r="H13" s="112"/>
-      <c r="I13" s="9"/>
-    </row>
-    <row r="14" spans="1:9" s="10" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A14" s="41"/>
-      <c r="B14" s="62" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="77" t="s">
-        <v>112</v>
-      </c>
-      <c r="D14" s="111"/>
-      <c r="E14" s="112"/>
-      <c r="F14" s="112"/>
-      <c r="G14" s="112"/>
-      <c r="H14" s="112"/>
-      <c r="I14" s="9"/>
-    </row>
-    <row r="15" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="41"/>
-      <c r="B15" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="77"/>
-      <c r="D15" s="111"/>
-      <c r="E15" s="112"/>
-      <c r="F15" s="112"/>
-      <c r="G15" s="112"/>
-      <c r="H15" s="112"/>
-      <c r="I15" s="9"/>
-    </row>
-    <row r="16" spans="1:9" s="10" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A16" s="41"/>
-      <c r="B16" s="62" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="77" t="s">
-        <v>113</v>
-      </c>
-      <c r="D16" s="113"/>
-      <c r="E16" s="114"/>
-      <c r="F16" s="114"/>
-      <c r="G16" s="114"/>
-      <c r="H16" s="112"/>
-      <c r="I16" s="9"/>
-    </row>
-    <row r="17" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="41"/>
-      <c r="B17" s="62" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="77"/>
-      <c r="D17" s="111"/>
-      <c r="E17" s="112"/>
-      <c r="F17" s="112"/>
-      <c r="G17" s="112"/>
-      <c r="H17" s="112"/>
-      <c r="I17" s="9"/>
-    </row>
-    <row r="18" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="41"/>
-      <c r="B18" s="62" t="s">
-        <v>101</v>
-      </c>
-      <c r="C18" s="77"/>
-      <c r="D18" s="111"/>
-      <c r="E18" s="112"/>
-      <c r="F18" s="112"/>
-      <c r="G18" s="112"/>
-      <c r="H18" s="112"/>
-      <c r="I18" s="9"/>
-    </row>
-    <row r="19" spans="1:9" s="10" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
-      <c r="A19" s="41"/>
-      <c r="B19" s="64" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="77"/>
-      <c r="D19" s="111"/>
-      <c r="E19" s="112"/>
-      <c r="F19" s="112"/>
-      <c r="G19" s="112"/>
-      <c r="H19" s="112"/>
-      <c r="I19" s="9"/>
-    </row>
-    <row r="20" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="41"/>
-      <c r="B20" s="62" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="77"/>
-      <c r="D20" s="111"/>
-      <c r="E20" s="112"/>
-      <c r="F20" s="112"/>
-      <c r="G20" s="112"/>
-      <c r="H20" s="112"/>
-      <c r="I20" s="9"/>
-    </row>
-    <row r="21" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="41"/>
-      <c r="B21" s="62" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="77"/>
-      <c r="D21" s="111"/>
-      <c r="E21" s="112"/>
-      <c r="F21" s="112"/>
-      <c r="G21" s="112"/>
-      <c r="H21" s="112"/>
-      <c r="I21" s="9"/>
-    </row>
-    <row r="22" spans="1:9" s="12" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
-      <c r="A22" s="90" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="55"/>
-      <c r="C22" s="78" t="s">
-        <v>114</v>
-      </c>
-      <c r="D22" s="115"/>
-      <c r="E22" s="115"/>
-      <c r="F22" s="115"/>
-      <c r="G22" s="115"/>
-      <c r="H22" s="115"/>
-      <c r="I22" s="11"/>
-    </row>
-    <row r="23" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A23" s="42"/>
-      <c r="B23" s="96" t="s">
-        <v>2</v>
-      </c>
-      <c r="C23" s="79" t="s">
-        <v>115</v>
-      </c>
-      <c r="D23" s="116"/>
-      <c r="E23" s="117"/>
-      <c r="F23" s="117"/>
-      <c r="G23" s="117"/>
-      <c r="H23" s="117"/>
-      <c r="I23" s="13"/>
-    </row>
-    <row r="24" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A24" s="42"/>
-      <c r="B24" s="96" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="79" t="s">
-        <v>116</v>
-      </c>
-      <c r="D24" s="118"/>
-      <c r="E24" s="119"/>
-      <c r="F24" s="119"/>
-      <c r="G24" s="119"/>
-      <c r="H24" s="119"/>
-      <c r="I24" s="13"/>
-    </row>
-    <row r="25" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A25" s="42"/>
-      <c r="B25" s="96" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="79" t="s">
-        <v>117</v>
-      </c>
-      <c r="D25" s="120"/>
-      <c r="E25" s="121"/>
-      <c r="F25" s="121"/>
-      <c r="G25" s="121"/>
-      <c r="H25" s="121"/>
-      <c r="I25" s="13"/>
-    </row>
-    <row r="26" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A26" s="42"/>
-      <c r="B26" s="96" t="s">
-        <v>100</v>
-      </c>
-      <c r="C26" s="79" t="s">
-        <v>118</v>
-      </c>
-      <c r="D26" s="120"/>
-      <c r="E26" s="121"/>
-      <c r="F26" s="121"/>
-      <c r="G26" s="121"/>
-      <c r="H26" s="121"/>
-      <c r="I26" s="13"/>
-    </row>
-    <row r="27" spans="1:9" s="14" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A27" s="42"/>
-      <c r="B27" s="96" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="79" t="s">
-        <v>119</v>
-      </c>
-      <c r="D27" s="120"/>
-      <c r="E27" s="121"/>
-      <c r="F27" s="121"/>
-      <c r="G27" s="121"/>
-      <c r="H27" s="121"/>
-      <c r="I27" s="13"/>
-    </row>
-    <row r="28" spans="1:9" s="14" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A28" s="42"/>
-      <c r="B28" s="96" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="79" t="s">
-        <v>120</v>
-      </c>
-      <c r="D28" s="120"/>
-      <c r="E28" s="121"/>
-      <c r="F28" s="121"/>
-      <c r="G28" s="121"/>
-      <c r="H28" s="121"/>
-      <c r="I28" s="13"/>
-    </row>
-    <row r="29" spans="1:9" s="14" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A29" s="42"/>
-      <c r="B29" s="96" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="79" t="s">
-        <v>121</v>
-      </c>
-      <c r="D29" s="120"/>
-      <c r="E29" s="121"/>
-      <c r="F29" s="121"/>
-      <c r="G29" s="121"/>
-      <c r="H29" s="121"/>
-      <c r="I29" s="13"/>
-    </row>
-    <row r="30" spans="1:9" s="14" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A30" s="42"/>
-      <c r="B30" s="96" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="79" t="s">
-        <v>122</v>
-      </c>
-      <c r="D30" s="116"/>
-      <c r="E30" s="117"/>
-      <c r="F30" s="117"/>
-      <c r="G30" s="117"/>
-      <c r="H30" s="117"/>
-      <c r="I30" s="13"/>
-    </row>
-    <row r="31" spans="1:9" s="14" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A31" s="42"/>
-      <c r="B31" s="96" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" s="79" t="s">
-        <v>123</v>
-      </c>
-      <c r="D31" s="122"/>
-      <c r="E31" s="123"/>
-      <c r="F31" s="123"/>
-      <c r="G31" s="123"/>
-      <c r="H31" s="123"/>
-      <c r="I31" s="13"/>
-    </row>
-    <row r="32" spans="1:9" s="14" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A32" s="42"/>
-      <c r="B32" s="65" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" s="79" t="s">
-        <v>124</v>
-      </c>
-      <c r="D32" s="122"/>
-      <c r="E32" s="123"/>
-      <c r="F32" s="123"/>
-      <c r="G32" s="123"/>
-      <c r="H32" s="123"/>
-      <c r="I32" s="13"/>
-    </row>
-    <row r="33" spans="1:9" s="14" customFormat="1" ht="57" x14ac:dyDescent="0.5">
-      <c r="A33" s="42"/>
-      <c r="B33" s="65" t="s">
-        <v>42</v>
-      </c>
-      <c r="C33" s="79" t="s">
-        <v>125</v>
-      </c>
-      <c r="D33" s="100"/>
-      <c r="E33" s="101"/>
-      <c r="F33" s="101"/>
-      <c r="G33" s="99"/>
-      <c r="H33" s="101"/>
-      <c r="I33" s="13"/>
-    </row>
-    <row r="34" spans="1:9" s="14" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
-      <c r="A34" s="42"/>
-      <c r="B34" s="65" t="s">
-        <v>84</v>
-      </c>
-      <c r="C34" s="79" t="s">
-        <v>126</v>
-      </c>
-      <c r="D34" s="102"/>
-      <c r="E34" s="103"/>
-      <c r="F34" s="104"/>
-      <c r="G34" s="99"/>
-      <c r="H34" s="104"/>
-      <c r="I34" s="13"/>
-    </row>
-    <row r="35" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A35" s="43"/>
-      <c r="B35" s="65" t="s">
-        <v>83</v>
-      </c>
-      <c r="C35" s="79" t="s">
-        <v>127</v>
-      </c>
-      <c r="D35" s="120"/>
-      <c r="E35" s="121"/>
-      <c r="F35" s="121"/>
-      <c r="G35" s="121"/>
-      <c r="H35" s="121"/>
-      <c r="I35" s="15"/>
-    </row>
-    <row r="36" spans="1:9" s="14" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A36" s="42"/>
-      <c r="B36" s="65" t="s">
-        <v>43</v>
-      </c>
-      <c r="C36" s="79" t="s">
-        <v>128</v>
-      </c>
-      <c r="D36" s="122"/>
-      <c r="E36" s="123"/>
-      <c r="F36" s="123"/>
-      <c r="G36" s="123"/>
-      <c r="H36" s="123"/>
-      <c r="I36" s="13"/>
-    </row>
-    <row r="37" spans="1:9" s="14" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A37" s="42"/>
-      <c r="B37" s="65" t="s">
-        <v>44</v>
-      </c>
-      <c r="C37" s="79" t="s">
-        <v>129</v>
-      </c>
-      <c r="D37" s="122"/>
-      <c r="E37" s="123"/>
-      <c r="F37" s="123"/>
-      <c r="G37" s="123"/>
-      <c r="H37" s="123"/>
-      <c r="I37" s="13"/>
-    </row>
-    <row r="38" spans="1:9" s="18" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
-      <c r="A38" s="91" t="s">
-        <v>30</v>
-      </c>
-      <c r="B38" s="56"/>
-      <c r="C38" s="80" t="s">
-        <v>145</v>
-      </c>
-      <c r="D38" s="124"/>
-      <c r="E38" s="124"/>
-      <c r="F38" s="124"/>
-      <c r="G38" s="124"/>
-      <c r="H38" s="124"/>
-      <c r="I38" s="17"/>
-    </row>
-    <row r="39" spans="1:9" s="20" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A39" s="44"/>
-      <c r="B39" s="66" t="s">
-        <v>39</v>
-      </c>
-      <c r="C39" s="81" t="s">
-        <v>130</v>
-      </c>
-      <c r="D39" s="125"/>
-      <c r="E39" s="126"/>
-      <c r="F39" s="126"/>
-      <c r="G39" s="126"/>
-      <c r="H39" s="126"/>
-      <c r="I39" s="19"/>
-    </row>
-    <row r="40" spans="1:9" s="20" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A40" s="44"/>
-      <c r="B40" s="67" t="s">
-        <v>98</v>
-      </c>
-      <c r="C40" s="81" t="s">
-        <v>167</v>
-      </c>
-      <c r="D40" s="125"/>
-      <c r="E40" s="126"/>
-      <c r="F40" s="127"/>
-      <c r="G40" s="126"/>
-      <c r="H40" s="127"/>
-      <c r="I40" s="19"/>
-    </row>
-    <row r="41" spans="1:9" s="20" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A41" s="44"/>
-      <c r="B41" s="66" t="s">
-        <v>78</v>
-      </c>
-      <c r="C41" s="81" t="s">
-        <v>131</v>
-      </c>
-      <c r="D41" s="125"/>
-      <c r="E41" s="125"/>
-      <c r="F41" s="125"/>
-      <c r="G41" s="125"/>
-      <c r="H41" s="125"/>
-      <c r="I41" s="19"/>
-    </row>
-    <row r="42" spans="1:9" s="20" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A42" s="44"/>
-      <c r="B42" s="93" t="s">
-        <v>1</v>
-      </c>
-      <c r="C42" s="81" t="s">
-        <v>132</v>
-      </c>
-      <c r="D42" s="125"/>
-      <c r="E42" s="126"/>
-      <c r="F42" s="126"/>
-      <c r="G42" s="126"/>
-      <c r="H42" s="126"/>
-      <c r="I42" s="19"/>
-    </row>
-    <row r="43" spans="1:9" s="22" customFormat="1" ht="57" x14ac:dyDescent="0.5">
-      <c r="A43" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="B43" s="57"/>
-      <c r="C43" s="82" t="s">
+      <c r="C52" s="111" t="s">
+        <v>142</v>
+      </c>
+      <c r="D52" s="98"/>
+      <c r="E52" s="44"/>
+      <c r="F52" s="44"/>
+      <c r="G52" s="44"/>
+      <c r="H52" s="44"/>
+      <c r="I52" s="45"/>
+    </row>
+    <row r="53" spans="1:9" s="48" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A53" s="116" t="s">
+        <v>173</v>
+      </c>
+      <c r="B53" s="72"/>
+      <c r="C53" s="112" t="s">
         <v>146</v>
       </c>
-      <c r="D43" s="128"/>
-      <c r="E43" s="129"/>
-      <c r="F43" s="129"/>
-      <c r="G43" s="129"/>
-      <c r="H43" s="129"/>
-      <c r="I43" s="21"/>
-    </row>
-    <row r="44" spans="1:9" s="24" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A44" s="46"/>
-      <c r="B44" s="68" t="s">
-        <v>21</v>
-      </c>
-      <c r="C44" s="83" t="s">
-        <v>133</v>
-      </c>
-      <c r="D44" s="105"/>
-      <c r="E44" s="106"/>
-      <c r="F44" s="106"/>
-      <c r="G44" s="106"/>
-      <c r="H44" s="106"/>
-      <c r="I44" s="23"/>
-    </row>
-    <row r="45" spans="1:9" s="24" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
-      <c r="A45" s="46"/>
-      <c r="B45" s="68" t="s">
-        <v>22</v>
-      </c>
-      <c r="C45" s="83" t="s">
-        <v>134</v>
-      </c>
-      <c r="D45" s="107"/>
-      <c r="E45" s="108"/>
-      <c r="F45" s="108"/>
-      <c r="G45" s="108"/>
-      <c r="H45" s="108"/>
-      <c r="I45" s="23"/>
-    </row>
-    <row r="46" spans="1:9" s="24" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A46" s="46"/>
-      <c r="B46" s="68" t="s">
-        <v>79</v>
-      </c>
-      <c r="C46" s="83" t="s">
-        <v>139</v>
-      </c>
-      <c r="D46" s="130"/>
-      <c r="E46" s="131"/>
-      <c r="F46" s="131"/>
-      <c r="G46" s="131"/>
-      <c r="H46" s="131"/>
-      <c r="I46" s="23"/>
-    </row>
-    <row r="47" spans="1:9" s="24" customFormat="1" ht="57" x14ac:dyDescent="0.5">
-      <c r="A47" s="46"/>
-      <c r="B47" s="68" t="s">
-        <v>23</v>
-      </c>
-      <c r="C47" s="83" t="s">
-        <v>140</v>
-      </c>
-      <c r="D47" s="105"/>
-      <c r="E47" s="106"/>
-      <c r="F47" s="106"/>
-      <c r="G47" s="106"/>
-      <c r="H47" s="106"/>
-      <c r="I47" s="23"/>
-    </row>
-    <row r="48" spans="1:9" s="24" customFormat="1" ht="91.2" x14ac:dyDescent="0.5">
-      <c r="A48" s="46"/>
-      <c r="B48" s="68" t="s">
-        <v>24</v>
-      </c>
-      <c r="C48" s="83" t="s">
-        <v>141</v>
-      </c>
-      <c r="D48" s="107"/>
-      <c r="E48" s="108"/>
-      <c r="F48" s="108"/>
-      <c r="G48" s="108"/>
-      <c r="H48" s="108"/>
-      <c r="I48" s="23"/>
-    </row>
-    <row r="49" spans="1:9" s="24" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
-      <c r="A49" s="46"/>
-      <c r="B49" s="68" t="s">
-        <v>175</v>
-      </c>
-      <c r="C49" s="83" t="s">
-        <v>176</v>
-      </c>
-      <c r="D49" s="130"/>
-      <c r="E49" s="131"/>
-      <c r="F49" s="131"/>
-      <c r="G49" s="131"/>
-      <c r="H49" s="131"/>
-      <c r="I49" s="23"/>
-    </row>
-    <row r="50" spans="1:9" s="24" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A50" s="46"/>
-      <c r="B50" s="68" t="s">
-        <v>41</v>
-      </c>
-      <c r="C50" s="83" t="s">
-        <v>142</v>
-      </c>
-      <c r="D50" s="130"/>
-      <c r="E50" s="131"/>
-      <c r="F50" s="131"/>
-      <c r="G50" s="131"/>
-      <c r="H50" s="131"/>
-      <c r="I50" s="23"/>
-    </row>
-    <row r="51" spans="1:9" s="26" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A51" s="47" t="s">
-        <v>45</v>
-      </c>
-      <c r="B51" s="58"/>
-      <c r="C51" s="84" t="s">
+      <c r="D53" s="47"/>
+      <c r="E53" s="47"/>
+      <c r="F53" s="47"/>
+      <c r="G53" s="47"/>
+      <c r="H53" s="47"/>
+      <c r="I53" s="47"/>
+    </row>
+    <row r="54" spans="1:9" s="51" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
+      <c r="A54" s="64"/>
+      <c r="B54" s="82" t="s">
+        <v>32</v>
+      </c>
+      <c r="C54" s="113" t="s">
         <v>147</v>
       </c>
-      <c r="D51" s="132"/>
-      <c r="E51" s="132"/>
-      <c r="F51" s="132"/>
-      <c r="G51" s="132"/>
-      <c r="H51" s="132"/>
-      <c r="I51" s="25"/>
-    </row>
-    <row r="52" spans="1:9" s="28" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A52" s="48"/>
-      <c r="B52" s="69" t="s">
-        <v>46</v>
-      </c>
-      <c r="C52" s="85" t="s">
-        <v>143</v>
-      </c>
-      <c r="D52" s="133"/>
-      <c r="E52" s="134"/>
-      <c r="F52" s="134"/>
-      <c r="G52" s="134"/>
-      <c r="H52" s="134"/>
-      <c r="I52" s="27"/>
-    </row>
-    <row r="53" spans="1:9" s="28" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A53" s="48"/>
-      <c r="B53" s="69" t="s">
-        <v>82</v>
-      </c>
-      <c r="C53" s="85" t="s">
-        <v>144</v>
-      </c>
-      <c r="D53" s="133"/>
-      <c r="E53" s="134"/>
-      <c r="F53" s="134"/>
-      <c r="G53" s="134"/>
-      <c r="H53" s="134"/>
-      <c r="I53" s="27"/>
-    </row>
-    <row r="54" spans="1:9" s="30" customFormat="1" ht="42" x14ac:dyDescent="0.5">
-      <c r="A54" s="92" t="s">
-        <v>164</v>
-      </c>
-      <c r="B54" s="59"/>
-      <c r="C54" s="86" t="s">
-        <v>173</v>
-      </c>
-      <c r="D54" s="135"/>
-      <c r="E54" s="135"/>
-      <c r="F54" s="135"/>
-      <c r="G54" s="135"/>
-      <c r="H54" s="135"/>
-      <c r="I54" s="29"/>
-    </row>
-    <row r="55" spans="1:9" s="32" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
-      <c r="A55" s="49"/>
-      <c r="B55" s="70" t="s">
-        <v>32</v>
-      </c>
-      <c r="C55" s="87" t="s">
+      <c r="D54" s="99"/>
+      <c r="E54" s="49"/>
+      <c r="F54" s="49"/>
+      <c r="G54" s="49"/>
+      <c r="H54" s="49"/>
+      <c r="I54" s="50"/>
+    </row>
+    <row r="55" spans="1:9" s="51" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A55" s="64"/>
+      <c r="B55" s="83" t="s">
+        <v>91</v>
+      </c>
+      <c r="C55" s="113" t="s">
         <v>148</v>
       </c>
-      <c r="D55" s="136"/>
-      <c r="E55" s="137"/>
-      <c r="F55" s="137"/>
-      <c r="G55" s="137"/>
-      <c r="H55" s="137"/>
-      <c r="I55" s="31"/>
-    </row>
-    <row r="56" spans="1:9" s="32" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A56" s="49"/>
-      <c r="B56" s="71" t="s">
+      <c r="D55" s="99"/>
+      <c r="E55" s="49"/>
+      <c r="F55" s="49"/>
+      <c r="G55" s="49"/>
+      <c r="H55" s="49"/>
+      <c r="I55" s="50"/>
+    </row>
+    <row r="56" spans="1:9" s="51" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A56" s="64"/>
+      <c r="B56" s="82" t="s">
         <v>92</v>
       </c>
-      <c r="C56" s="87" t="s">
+      <c r="C56" s="113" t="s">
         <v>149</v>
       </c>
-      <c r="D56" s="136"/>
-      <c r="E56" s="137"/>
-      <c r="F56" s="137"/>
-      <c r="G56" s="137"/>
-      <c r="H56" s="137"/>
-      <c r="I56" s="31"/>
-    </row>
-    <row r="57" spans="1:9" s="32" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A57" s="49"/>
-      <c r="B57" s="70" t="s">
-        <v>93</v>
-      </c>
-      <c r="C57" s="87" t="s">
+      <c r="D56" s="99"/>
+      <c r="E56" s="49"/>
+      <c r="F56" s="49"/>
+      <c r="G56" s="49"/>
+      <c r="H56" s="49"/>
+      <c r="I56" s="50"/>
+    </row>
+    <row r="57" spans="1:9" s="51" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A57" s="64"/>
+      <c r="B57" s="82" t="s">
+        <v>33</v>
+      </c>
+      <c r="C57" s="113" t="s">
         <v>150</v>
       </c>
-      <c r="D57" s="136"/>
-      <c r="E57" s="137"/>
-      <c r="F57" s="137"/>
-      <c r="G57" s="137"/>
-      <c r="H57" s="137"/>
-      <c r="I57" s="31"/>
-    </row>
-    <row r="58" spans="1:9" s="32" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A58" s="49"/>
-      <c r="B58" s="70" t="s">
-        <v>33</v>
-      </c>
-      <c r="C58" s="87" t="s">
+      <c r="D57" s="99"/>
+      <c r="E57" s="49"/>
+      <c r="F57" s="49"/>
+      <c r="G57" s="49"/>
+      <c r="H57" s="49"/>
+      <c r="I57" s="50"/>
+    </row>
+    <row r="58" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A58" s="64"/>
+      <c r="B58" s="82" t="s">
+        <v>34</v>
+      </c>
+      <c r="C58" s="113"/>
+      <c r="D58" s="99"/>
+      <c r="E58" s="49"/>
+      <c r="F58" s="49"/>
+      <c r="G58" s="49"/>
+      <c r="H58" s="49"/>
+      <c r="I58" s="50"/>
+    </row>
+    <row r="59" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A59" s="64"/>
+      <c r="B59" s="82" t="s">
+        <v>35</v>
+      </c>
+      <c r="C59" s="113"/>
+      <c r="D59" s="99"/>
+      <c r="E59" s="49"/>
+      <c r="F59" s="49"/>
+      <c r="G59" s="49"/>
+      <c r="H59" s="49"/>
+      <c r="I59" s="50"/>
+    </row>
+    <row r="60" spans="1:9" s="51" customFormat="1" ht="39.6" x14ac:dyDescent="0.5">
+      <c r="A60" s="64"/>
+      <c r="B60" s="84" t="s">
+        <v>36</v>
+      </c>
+      <c r="C60" s="113"/>
+      <c r="D60" s="99"/>
+      <c r="E60" s="49"/>
+      <c r="F60" s="49"/>
+      <c r="G60" s="49"/>
+      <c r="H60" s="49"/>
+      <c r="I60" s="50"/>
+    </row>
+    <row r="61" spans="1:9" s="51" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
+      <c r="A61" s="64"/>
+      <c r="B61" s="84" t="s">
+        <v>37</v>
+      </c>
+      <c r="C61" s="113"/>
+      <c r="D61" s="99"/>
+      <c r="E61" s="49"/>
+      <c r="F61" s="49"/>
+      <c r="G61" s="49"/>
+      <c r="H61" s="49"/>
+      <c r="I61" s="50"/>
+    </row>
+    <row r="62" spans="1:9" s="51" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
+      <c r="A62" s="64"/>
+      <c r="B62" s="82" t="s">
+        <v>94</v>
+      </c>
+      <c r="C62" s="113" t="s">
         <v>151</v>
       </c>
-      <c r="D58" s="136"/>
-      <c r="E58" s="137"/>
-      <c r="F58" s="137"/>
-      <c r="G58" s="137"/>
-      <c r="H58" s="137"/>
-      <c r="I58" s="31"/>
-    </row>
-    <row r="59" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A59" s="49"/>
-      <c r="B59" s="70" t="s">
-        <v>34</v>
-      </c>
-      <c r="C59" s="87"/>
-      <c r="D59" s="136"/>
-      <c r="E59" s="137"/>
-      <c r="F59" s="137"/>
-      <c r="G59" s="137"/>
-      <c r="H59" s="137"/>
-      <c r="I59" s="31"/>
-    </row>
-    <row r="60" spans="1:9" s="32" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A60" s="49"/>
-      <c r="B60" s="70" t="s">
-        <v>35</v>
-      </c>
-      <c r="C60" s="87"/>
-      <c r="D60" s="136"/>
-      <c r="E60" s="137"/>
-      <c r="F60" s="137"/>
-      <c r="G60" s="137"/>
-      <c r="H60" s="137"/>
-      <c r="I60" s="31"/>
-    </row>
-    <row r="61" spans="1:9" s="32" customFormat="1" ht="39.6" x14ac:dyDescent="0.5">
-      <c r="A61" s="49"/>
-      <c r="B61" s="72" t="s">
-        <v>36</v>
-      </c>
-      <c r="C61" s="87"/>
-      <c r="D61" s="136"/>
-      <c r="E61" s="137"/>
-      <c r="F61" s="137"/>
-      <c r="G61" s="137"/>
-      <c r="H61" s="137"/>
-      <c r="I61" s="31"/>
-    </row>
-    <row r="62" spans="1:9" s="32" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
-      <c r="A62" s="49"/>
-      <c r="B62" s="72" t="s">
-        <v>37</v>
-      </c>
-      <c r="C62" s="87"/>
-      <c r="D62" s="136"/>
-      <c r="E62" s="137"/>
-      <c r="F62" s="137"/>
-      <c r="G62" s="137"/>
-      <c r="H62" s="137"/>
-      <c r="I62" s="31"/>
-    </row>
-    <row r="63" spans="1:9" s="34" customFormat="1" ht="57" x14ac:dyDescent="0.5">
-      <c r="A63" s="50" t="s">
+      <c r="D62" s="99"/>
+      <c r="E62" s="49"/>
+      <c r="F62" s="49"/>
+      <c r="G62" s="49"/>
+      <c r="H62" s="49"/>
+      <c r="I62" s="50"/>
+    </row>
+    <row r="63" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A63" s="64"/>
+      <c r="B63" s="82" t="s">
         <v>95</v>
       </c>
-      <c r="B63" s="60"/>
-      <c r="C63" s="88" t="s">
-        <v>174</v>
-      </c>
-      <c r="D63" s="138"/>
-      <c r="E63" s="138"/>
-      <c r="F63" s="138"/>
-      <c r="G63" s="138"/>
-      <c r="H63" s="138"/>
-      <c r="I63" s="33"/>
-    </row>
-    <row r="64" spans="1:9" s="36" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
-      <c r="A64" s="51"/>
-      <c r="B64" s="73" t="s">
-        <v>96</v>
-      </c>
-      <c r="C64" s="89" t="s">
-        <v>152</v>
-      </c>
-      <c r="D64" s="139"/>
-      <c r="E64" s="140"/>
-      <c r="F64" s="140"/>
-      <c r="G64" s="140"/>
-      <c r="H64" s="140"/>
-      <c r="I64" s="35"/>
-    </row>
-    <row r="65" spans="1:9" s="36" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A65" s="51"/>
-      <c r="B65" s="73" t="s">
-        <v>97</v>
-      </c>
-      <c r="C65" s="89" t="s">
-        <v>163</v>
-      </c>
-      <c r="D65" s="139"/>
-      <c r="E65" s="140"/>
-      <c r="F65" s="140"/>
-      <c r="G65" s="140"/>
-      <c r="H65" s="140"/>
-      <c r="I65" s="35"/>
+      <c r="C63" s="113" t="s">
+        <v>162</v>
+      </c>
+      <c r="D63" s="99"/>
+      <c r="E63" s="49"/>
+      <c r="F63" s="49"/>
+      <c r="G63" s="49"/>
+      <c r="H63" s="49"/>
+      <c r="I63" s="50"/>
     </row>
   </sheetData>
   <sheetProtection deleteColumns="0" selectLockedCells="1"/>
@@ -2785,13 +2672,13 @@
           <x14:formula1>
             <xm:f>'Drop Down List Values'!$J$2:$J$7</xm:f>
           </x14:formula1>
-          <xm:sqref>D50:H50</xm:sqref>
+          <xm:sqref>D49:H49</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{093E1169-867D-4A32-AC3C-DC58C26E3C39}">
           <x14:formula1>
             <xm:f>'Drop Down List Values'!$M$2:$M$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D65:H65</xm:sqref>
+          <xm:sqref>D63:H63</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{33A578CF-33CA-4B41-B2C5-7541E5042FC9}">
           <x14:formula1>
@@ -2821,7 +2708,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F8BFBD-18C1-4ED5-A02E-9841686C259E}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -2850,19 +2737,19 @@
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H1" t="s">
         <v>25</v>
@@ -2871,205 +2758,205 @@
         <v>1</v>
       </c>
       <c r="J1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="L1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="L2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" t="s">
         <v>74</v>
       </c>
-      <c r="H4" t="s">
-        <v>53</v>
-      </c>
-      <c r="I4" t="s">
-        <v>75</v>
-      </c>
       <c r="J4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="L4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s">
         <v>52</v>
       </c>
-      <c r="D6" t="s">
-        <v>53</v>
-      </c>
       <c r="E6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -3079,6 +2966,65 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D4902BA52C7D94A994657A564808B2B" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e4455a60d2ff5f5fcd8815d6d89b5b66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b541edd5-2552-480e-ada6-0e2c8d317108" xmlns:ns3="780ae317-08c5-4e10-af93-dd385a8384a9" xmlns:ns4="3146657c-56f4-4c0a-bb9c-a675121ac670" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d1d01ecd782f081d5d944fa263943fc4" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="b541edd5-2552-480e-ada6-0e2c8d317108"/>
@@ -3277,7 +3223,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_dlc_DocId xmlns="b541edd5-2552-480e-ada6-0e2c8d317108">YVWEJ5DVYS2U-421999773-68</_dlc_DocId>
@@ -3291,66 +3237,23 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{448710E8-BE9E-4C9E-A40A-0AC1DAE48E99}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF0D7A6D-D78F-4048-9348-0B4289842B11}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0980278E-2A79-4F44-8623-FE545C304BE1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3370,36 +3273,20 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69E3EF86-6C9E-4C22-A476-13DA012C68C5}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="780ae317-08c5-4e10-af93-dd385a8384a9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="780ae317-08c5-4e10-af93-dd385a8384a9"/>
+    <ds:schemaRef ds:uri="3146657c-56f4-4c0a-bb9c-a675121ac670"/>
+    <ds:schemaRef ds:uri="b541edd5-2552-480e-ada6-0e2c8d317108"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="b541edd5-2552-480e-ada6-0e2c8d317108"/>
-    <ds:schemaRef ds:uri="3146657c-56f4-4c0a-bb9c-a675121ac670"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{448710E8-BE9E-4C9E-A40A-0AC1DAE48E99}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF0D7A6D-D78F-4048-9348-0B4289842B11}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated xlsx file with autopsy location information.
</commit_message>
<xml_diff>
--- a/MDI-To-EDRS-Template.xlsx
+++ b/MDI-To-EDRS-Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20396"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20403"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mriley7\workspace\raven-import-and-submit-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA7019D1-ED79-4310-9BF2-27319FFB7C4A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80EE54F1-0FE6-469C-A3F2-C71DCB09E89B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8484" xr2:uid="{7A50F290-1C75-487E-9806-F93553E4E7CC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8490" xr2:uid="{7A50F290-1C75-487E-9806-F93553E4E7CC}"/>
   </bookViews>
   <sheets>
     <sheet name="MDI RAVEN Input Schema" sheetId="4" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="180">
   <si>
     <t>Manner of Death</t>
   </si>
@@ -659,6 +659,24 @@
   </si>
   <si>
     <t>Death Certifier</t>
+  </si>
+  <si>
+    <t>Autopsy Performed Location: Street</t>
+  </si>
+  <si>
+    <t>Autopsy Performed Location: City</t>
+  </si>
+  <si>
+    <t>Autopsy Performed Location: County</t>
+  </si>
+  <si>
+    <t>Primary Address of the autopsy location. Multiple lines are supported.</t>
+  </si>
+  <si>
+    <t>Autopsy Performed Location: State, U.S. Territory or Canadian Province</t>
+  </si>
+  <si>
+    <t>Autopsy Performed Location: Postal Code</t>
   </si>
 </sst>
 </file>
@@ -1678,23 +1696,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54CD1DC7-E143-4CF5-BEA9-4DABBAFFC7B0}">
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="22.5" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" style="53" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" style="65" customWidth="1"/>
-    <col min="3" max="3" width="38.44140625" style="73" customWidth="1"/>
-    <col min="4" max="8" width="32.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="27.28515625" style="53" customWidth="1"/>
+    <col min="2" max="2" width="64.42578125" style="65" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" style="73" customWidth="1"/>
+    <col min="4" max="8" width="32.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="53" t="s">
         <v>26</v>
       </c>
@@ -1723,12 +1741,12 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="23.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" ht="36.75" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C2" s="73" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="109.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9" ht="120" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="53" t="s">
         <v>169</v>
       </c>
@@ -1739,7 +1757,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="4" customFormat="1" ht="34.799999999999997" thickTop="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:9" s="4" customFormat="1" ht="36.75" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A4" s="54" t="s">
         <v>28</v>
       </c>
@@ -1754,7 +1772,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" s="6" customFormat="1" ht="29.4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:9" s="6" customFormat="1" ht="29.25" x14ac:dyDescent="0.45">
       <c r="A5" s="55"/>
       <c r="B5" s="118" t="s">
         <v>79</v>
@@ -1769,7 +1787,7 @@
       <c r="H5" s="52"/>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="1:9" s="6" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:9" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.45">
       <c r="A6" s="55"/>
       <c r="B6" s="119" t="s">
         <v>80</v>
@@ -1784,7 +1802,7 @@
       <c r="H6" s="52"/>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="1:9" s="8" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:9" s="8" customFormat="1" ht="36" x14ac:dyDescent="0.45">
       <c r="A7" s="56" t="s">
         <v>29</v>
       </c>
@@ -1799,7 +1817,7 @@
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:9" s="11" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:9" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.45">
       <c r="A8" s="57"/>
       <c r="B8" s="74" t="s">
         <v>10</v>
@@ -1814,7 +1832,7 @@
       <c r="H8" s="9"/>
       <c r="I8" s="10"/>
     </row>
-    <row r="9" spans="1:9" s="11" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:9" s="11" customFormat="1" ht="60" x14ac:dyDescent="0.45">
       <c r="A9" s="57"/>
       <c r="B9" s="74" t="s">
         <v>11</v>
@@ -1829,7 +1847,7 @@
       <c r="H9" s="9"/>
       <c r="I9" s="10"/>
     </row>
-    <row r="10" spans="1:9" s="11" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:9" s="11" customFormat="1" ht="24" x14ac:dyDescent="0.45">
       <c r="A10" s="57"/>
       <c r="B10" s="74" t="s">
         <v>12</v>
@@ -1844,7 +1862,7 @@
       <c r="H10" s="9"/>
       <c r="I10" s="10"/>
     </row>
-    <row r="11" spans="1:9" s="11" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:9" s="11" customFormat="1" ht="36" x14ac:dyDescent="0.45">
       <c r="A11" s="57"/>
       <c r="B11" s="75" t="s">
         <v>76</v>
@@ -1859,7 +1877,7 @@
       <c r="H11" s="9"/>
       <c r="I11" s="10"/>
     </row>
-    <row r="12" spans="1:9" s="11" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:9" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.45">
       <c r="A12" s="57"/>
       <c r="B12" s="74" t="s">
         <v>13</v>
@@ -1874,7 +1892,7 @@
       <c r="H12" s="9"/>
       <c r="I12" s="10"/>
     </row>
-    <row r="13" spans="1:9" s="11" customFormat="1" ht="57" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:9" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.45">
       <c r="A13" s="57"/>
       <c r="B13" s="74" t="s">
         <v>14</v>
@@ -1889,7 +1907,7 @@
       <c r="H13" s="9"/>
       <c r="I13" s="10"/>
     </row>
-    <row r="14" spans="1:9" s="11" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:9" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.45">
       <c r="A14" s="57"/>
       <c r="B14" s="74" t="s">
         <v>15</v>
@@ -1904,7 +1922,7 @@
       <c r="H14" s="12"/>
       <c r="I14" s="10"/>
     </row>
-    <row r="15" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A15" s="57"/>
       <c r="B15" s="74" t="s">
         <v>16</v>
@@ -1917,7 +1935,7 @@
       <c r="H15" s="9"/>
       <c r="I15" s="10"/>
     </row>
-    <row r="16" spans="1:9" s="11" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:9" s="11" customFormat="1" ht="24" x14ac:dyDescent="0.45">
       <c r="A16" s="57"/>
       <c r="B16" s="74" t="s">
         <v>17</v>
@@ -1932,7 +1950,7 @@
       <c r="H16" s="9"/>
       <c r="I16" s="10"/>
     </row>
-    <row r="17" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A17" s="57"/>
       <c r="B17" s="74" t="s">
         <v>18</v>
@@ -1945,7 +1963,7 @@
       <c r="H17" s="9"/>
       <c r="I17" s="10"/>
     </row>
-    <row r="18" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A18" s="57"/>
       <c r="B18" s="74" t="s">
         <v>99</v>
@@ -1958,7 +1976,7 @@
       <c r="H18" s="9"/>
       <c r="I18" s="10"/>
     </row>
-    <row r="19" spans="1:9" s="11" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:9" s="11" customFormat="1" ht="38.25" x14ac:dyDescent="0.45">
       <c r="A19" s="57"/>
       <c r="B19" s="76" t="s">
         <v>19</v>
@@ -1971,7 +1989,7 @@
       <c r="H19" s="9"/>
       <c r="I19" s="10"/>
     </row>
-    <row r="20" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A20" s="57"/>
       <c r="B20" s="74" t="s">
         <v>38</v>
@@ -1984,7 +2002,7 @@
       <c r="H20" s="9"/>
       <c r="I20" s="10"/>
     </row>
-    <row r="21" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A21" s="57"/>
       <c r="B21" s="74" t="s">
         <v>20</v>
@@ -1997,7 +2015,7 @@
       <c r="H21" s="9"/>
       <c r="I21" s="10"/>
     </row>
-    <row r="22" spans="1:9" s="16" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:9" s="16" customFormat="1" ht="84" x14ac:dyDescent="0.45">
       <c r="A22" s="114" t="s">
         <v>31</v>
       </c>
@@ -2012,7 +2030,7 @@
       <c r="H22" s="15"/>
       <c r="I22" s="15"/>
     </row>
-    <row r="23" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A23" s="58"/>
       <c r="B23" s="120" t="s">
         <v>2</v>
@@ -2027,7 +2045,7 @@
       <c r="H23" s="17"/>
       <c r="I23" s="18"/>
     </row>
-    <row r="24" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A24" s="58"/>
       <c r="B24" s="120" t="s">
         <v>4</v>
@@ -2042,7 +2060,7 @@
       <c r="H24" s="20"/>
       <c r="I24" s="18"/>
     </row>
-    <row r="25" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A25" s="58"/>
       <c r="B25" s="120" t="s">
         <v>6</v>
@@ -2057,7 +2075,7 @@
       <c r="H25" s="21"/>
       <c r="I25" s="18"/>
     </row>
-    <row r="26" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A26" s="58"/>
       <c r="B26" s="120" t="s">
         <v>98</v>
@@ -2072,7 +2090,7 @@
       <c r="H26" s="21"/>
       <c r="I26" s="18"/>
     </row>
-    <row r="27" spans="1:9" s="19" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:9" s="19" customFormat="1" ht="48" x14ac:dyDescent="0.45">
       <c r="A27" s="58"/>
       <c r="B27" s="120" t="s">
         <v>3</v>
@@ -2087,7 +2105,7 @@
       <c r="H27" s="21"/>
       <c r="I27" s="18"/>
     </row>
-    <row r="28" spans="1:9" s="19" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:9" s="19" customFormat="1" ht="48" x14ac:dyDescent="0.45">
       <c r="A28" s="58"/>
       <c r="B28" s="120" t="s">
         <v>5</v>
@@ -2102,7 +2120,7 @@
       <c r="H28" s="21"/>
       <c r="I28" s="18"/>
     </row>
-    <row r="29" spans="1:9" s="19" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:9" s="19" customFormat="1" ht="48" x14ac:dyDescent="0.45">
       <c r="A29" s="58"/>
       <c r="B29" s="120" t="s">
         <v>7</v>
@@ -2117,7 +2135,7 @@
       <c r="H29" s="21"/>
       <c r="I29" s="18"/>
     </row>
-    <row r="30" spans="1:9" s="19" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:9" s="19" customFormat="1" ht="48" x14ac:dyDescent="0.45">
       <c r="A30" s="58"/>
       <c r="B30" s="120" t="s">
         <v>8</v>
@@ -2132,7 +2150,7 @@
       <c r="H30" s="17"/>
       <c r="I30" s="18"/>
     </row>
-    <row r="31" spans="1:9" s="19" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:9" s="19" customFormat="1" ht="48" x14ac:dyDescent="0.45">
       <c r="A31" s="58"/>
       <c r="B31" s="120" t="s">
         <v>9</v>
@@ -2147,7 +2165,7 @@
       <c r="H31" s="22"/>
       <c r="I31" s="18"/>
     </row>
-    <row r="32" spans="1:9" s="19" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:9" s="19" customFormat="1" ht="24" x14ac:dyDescent="0.45">
       <c r="A32" s="58"/>
       <c r="B32" s="77" t="s">
         <v>0</v>
@@ -2162,7 +2180,7 @@
       <c r="H32" s="22"/>
       <c r="I32" s="18"/>
     </row>
-    <row r="33" spans="1:9" s="19" customFormat="1" ht="57" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:9" s="19" customFormat="1" ht="60" x14ac:dyDescent="0.45">
       <c r="A33" s="58"/>
       <c r="B33" s="77" t="s">
         <v>41</v>
@@ -2177,7 +2195,7 @@
       <c r="H33" s="23"/>
       <c r="I33" s="18"/>
     </row>
-    <row r="34" spans="1:9" s="19" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:9" s="19" customFormat="1" ht="84" x14ac:dyDescent="0.45">
       <c r="A34" s="58"/>
       <c r="B34" s="77" t="s">
         <v>83</v>
@@ -2192,7 +2210,7 @@
       <c r="H34" s="24"/>
       <c r="I34" s="18"/>
     </row>
-    <row r="35" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A35" s="59"/>
       <c r="B35" s="77" t="s">
         <v>82</v>
@@ -2207,7 +2225,7 @@
       <c r="H35" s="21"/>
       <c r="I35" s="25"/>
     </row>
-    <row r="36" spans="1:9" s="19" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:9" s="19" customFormat="1" ht="36" x14ac:dyDescent="0.45">
       <c r="A36" s="58"/>
       <c r="B36" s="77" t="s">
         <v>42</v>
@@ -2222,7 +2240,7 @@
       <c r="H36" s="22"/>
       <c r="I36" s="18"/>
     </row>
-    <row r="37" spans="1:9" s="19" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:9" s="19" customFormat="1" ht="36" x14ac:dyDescent="0.45">
       <c r="A37" s="58"/>
       <c r="B37" s="77" t="s">
         <v>43</v>
@@ -2237,7 +2255,7 @@
       <c r="H37" s="22"/>
       <c r="I37" s="18"/>
     </row>
-    <row r="38" spans="1:9" s="28" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:9" s="28" customFormat="1" ht="84" x14ac:dyDescent="0.45">
       <c r="A38" s="115" t="s">
         <v>30</v>
       </c>
@@ -2252,7 +2270,7 @@
       <c r="H38" s="27"/>
       <c r="I38" s="27"/>
     </row>
-    <row r="39" spans="1:9" s="31" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:9" s="31" customFormat="1" ht="24" x14ac:dyDescent="0.45">
       <c r="A39" s="60"/>
       <c r="B39" s="78" t="s">
         <v>39</v>
@@ -2267,7 +2285,7 @@
       <c r="H39" s="29"/>
       <c r="I39" s="30"/>
     </row>
-    <row r="40" spans="1:9" s="31" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:9" s="31" customFormat="1" ht="24" x14ac:dyDescent="0.45">
       <c r="A40" s="60"/>
       <c r="B40" s="79" t="s">
         <v>96</v>
@@ -2282,7 +2300,7 @@
       <c r="H40" s="32"/>
       <c r="I40" s="30"/>
     </row>
-    <row r="41" spans="1:9" s="31" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:9" s="31" customFormat="1" ht="36" x14ac:dyDescent="0.45">
       <c r="A41" s="60"/>
       <c r="B41" s="78" t="s">
         <v>77</v>
@@ -2297,7 +2315,7 @@
       <c r="H41" s="92"/>
       <c r="I41" s="30"/>
     </row>
-    <row r="42" spans="1:9" s="31" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:9" s="31" customFormat="1" ht="36" x14ac:dyDescent="0.45">
       <c r="A42" s="60"/>
       <c r="B42" s="117" t="s">
         <v>1</v>
@@ -2312,7 +2330,7 @@
       <c r="H42" s="29"/>
       <c r="I42" s="30"/>
     </row>
-    <row r="43" spans="1:9" s="35" customFormat="1" ht="57" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:9" s="35" customFormat="1" ht="60" x14ac:dyDescent="0.45">
       <c r="A43" s="123" t="s">
         <v>172</v>
       </c>
@@ -2327,7 +2345,7 @@
       <c r="H43" s="33"/>
       <c r="I43" s="34"/>
     </row>
-    <row r="44" spans="1:9" s="38" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:9" s="38" customFormat="1" ht="48" x14ac:dyDescent="0.45">
       <c r="A44" s="61"/>
       <c r="B44" s="80" t="s">
         <v>21</v>
@@ -2342,7 +2360,7 @@
       <c r="H44" s="36"/>
       <c r="I44" s="37"/>
     </row>
-    <row r="45" spans="1:9" s="38" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:9" s="38" customFormat="1" ht="84" x14ac:dyDescent="0.45">
       <c r="A45" s="61"/>
       <c r="B45" s="80" t="s">
         <v>22</v>
@@ -2357,7 +2375,7 @@
       <c r="H45" s="39"/>
       <c r="I45" s="37"/>
     </row>
-    <row r="46" spans="1:9" s="38" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:9" s="38" customFormat="1" ht="36" x14ac:dyDescent="0.45">
       <c r="A46" s="61"/>
       <c r="B46" s="80" t="s">
         <v>78</v>
@@ -2372,7 +2390,7 @@
       <c r="H46" s="40"/>
       <c r="I46" s="37"/>
     </row>
-    <row r="47" spans="1:9" s="38" customFormat="1" ht="57" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:9" s="38" customFormat="1" ht="60" x14ac:dyDescent="0.45">
       <c r="A47" s="61"/>
       <c r="B47" s="80" t="s">
         <v>23</v>
@@ -2387,7 +2405,7 @@
       <c r="H47" s="41"/>
       <c r="I47" s="37"/>
     </row>
-    <row r="48" spans="1:9" s="38" customFormat="1" ht="91.2" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:9" s="38" customFormat="1" ht="96" x14ac:dyDescent="0.45">
       <c r="A48" s="61"/>
       <c r="B48" s="80" t="s">
         <v>24</v>
@@ -2402,7 +2420,7 @@
       <c r="H48" s="39"/>
       <c r="I48" s="37"/>
     </row>
-    <row r="49" spans="1:9" s="38" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:9" s="38" customFormat="1" ht="36" x14ac:dyDescent="0.45">
       <c r="A49" s="61"/>
       <c r="B49" s="80" t="s">
         <v>40</v>
@@ -2417,7 +2435,7 @@
       <c r="H49" s="40"/>
       <c r="I49" s="37"/>
     </row>
-    <row r="50" spans="1:9" s="43" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:9" s="43" customFormat="1" ht="24" x14ac:dyDescent="0.45">
       <c r="A50" s="62" t="s">
         <v>44</v>
       </c>
@@ -2432,7 +2450,7 @@
       <c r="H50" s="42"/>
       <c r="I50" s="42"/>
     </row>
-    <row r="51" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A51" s="63"/>
       <c r="B51" s="81" t="s">
         <v>45</v>
@@ -2447,115 +2465,69 @@
       <c r="H51" s="44"/>
       <c r="I51" s="45"/>
     </row>
-    <row r="52" spans="1:9" s="46" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A52" s="63"/>
+    <row r="52" spans="1:9" s="63" customFormat="1" ht="36" x14ac:dyDescent="0.45">
       <c r="B52" s="81" t="s">
         <v>81</v>
       </c>
       <c r="C52" s="111" t="s">
         <v>142</v>
       </c>
-      <c r="D52" s="98"/>
-      <c r="E52" s="44"/>
-      <c r="F52" s="44"/>
-      <c r="G52" s="44"/>
-      <c r="H52" s="44"/>
-      <c r="I52" s="45"/>
-    </row>
-    <row r="53" spans="1:9" s="48" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A53" s="116" t="s">
+    </row>
+    <row r="53" spans="1:9" s="63" customFormat="1" ht="24" x14ac:dyDescent="0.45">
+      <c r="B53" s="81" t="s">
+        <v>174</v>
+      </c>
+      <c r="C53" s="111" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" s="63" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B54" s="81" t="s">
+        <v>175</v>
+      </c>
+      <c r="C54" s="111"/>
+    </row>
+    <row r="55" spans="1:9" s="63" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B55" s="81" t="s">
+        <v>176</v>
+      </c>
+      <c r="C55" s="111"/>
+    </row>
+    <row r="56" spans="1:9" s="63" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B56" s="81" t="s">
+        <v>178</v>
+      </c>
+      <c r="C56" s="111"/>
+    </row>
+    <row r="57" spans="1:9" s="63" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B57" s="81" t="s">
+        <v>179</v>
+      </c>
+      <c r="C57" s="111"/>
+    </row>
+    <row r="58" spans="1:9" s="48" customFormat="1" ht="36" x14ac:dyDescent="0.45">
+      <c r="A58" s="116" t="s">
         <v>173</v>
       </c>
-      <c r="B53" s="72"/>
-      <c r="C53" s="112" t="s">
+      <c r="B58" s="72"/>
+      <c r="C58" s="112" t="s">
         <v>146</v>
       </c>
-      <c r="D53" s="47"/>
-      <c r="E53" s="47"/>
-      <c r="F53" s="47"/>
-      <c r="G53" s="47"/>
-      <c r="H53" s="47"/>
-      <c r="I53" s="47"/>
-    </row>
-    <row r="54" spans="1:9" s="51" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
-      <c r="A54" s="64"/>
-      <c r="B54" s="82" t="s">
-        <v>32</v>
-      </c>
-      <c r="C54" s="113" t="s">
-        <v>147</v>
-      </c>
-      <c r="D54" s="99"/>
-      <c r="E54" s="49"/>
-      <c r="F54" s="49"/>
-      <c r="G54" s="49"/>
-      <c r="H54" s="49"/>
-      <c r="I54" s="50"/>
-    </row>
-    <row r="55" spans="1:9" s="51" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A55" s="64"/>
-      <c r="B55" s="83" t="s">
-        <v>91</v>
-      </c>
-      <c r="C55" s="113" t="s">
-        <v>148</v>
-      </c>
-      <c r="D55" s="99"/>
-      <c r="E55" s="49"/>
-      <c r="F55" s="49"/>
-      <c r="G55" s="49"/>
-      <c r="H55" s="49"/>
-      <c r="I55" s="50"/>
-    </row>
-    <row r="56" spans="1:9" s="51" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A56" s="64"/>
-      <c r="B56" s="82" t="s">
-        <v>92</v>
-      </c>
-      <c r="C56" s="113" t="s">
-        <v>149</v>
-      </c>
-      <c r="D56" s="99"/>
-      <c r="E56" s="49"/>
-      <c r="F56" s="49"/>
-      <c r="G56" s="49"/>
-      <c r="H56" s="49"/>
-      <c r="I56" s="50"/>
-    </row>
-    <row r="57" spans="1:9" s="51" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A57" s="64"/>
-      <c r="B57" s="82" t="s">
-        <v>33</v>
-      </c>
-      <c r="C57" s="113" t="s">
-        <v>150</v>
-      </c>
-      <c r="D57" s="99"/>
-      <c r="E57" s="49"/>
-      <c r="F57" s="49"/>
-      <c r="G57" s="49"/>
-      <c r="H57" s="49"/>
-      <c r="I57" s="50"/>
-    </row>
-    <row r="58" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A58" s="64"/>
-      <c r="B58" s="82" t="s">
-        <v>34</v>
-      </c>
-      <c r="C58" s="113"/>
-      <c r="D58" s="99"/>
-      <c r="E58" s="49"/>
-      <c r="F58" s="49"/>
-      <c r="G58" s="49"/>
-      <c r="H58" s="49"/>
-      <c r="I58" s="50"/>
-    </row>
-    <row r="59" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="D58" s="47"/>
+      <c r="E58" s="47"/>
+      <c r="F58" s="47"/>
+      <c r="G58" s="47"/>
+      <c r="H58" s="47"/>
+      <c r="I58" s="47"/>
+    </row>
+    <row r="59" spans="1:9" s="51" customFormat="1" ht="72" x14ac:dyDescent="0.45">
       <c r="A59" s="64"/>
       <c r="B59" s="82" t="s">
-        <v>35</v>
-      </c>
-      <c r="C59" s="113"/>
+        <v>32</v>
+      </c>
+      <c r="C59" s="113" t="s">
+        <v>147</v>
+      </c>
       <c r="D59" s="99"/>
       <c r="E59" s="49"/>
       <c r="F59" s="49"/>
@@ -2563,12 +2535,14 @@
       <c r="H59" s="49"/>
       <c r="I59" s="50"/>
     </row>
-    <row r="60" spans="1:9" s="51" customFormat="1" ht="39.6" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:9" s="51" customFormat="1" ht="48" x14ac:dyDescent="0.45">
       <c r="A60" s="64"/>
-      <c r="B60" s="84" t="s">
-        <v>36</v>
-      </c>
-      <c r="C60" s="113"/>
+      <c r="B60" s="83" t="s">
+        <v>91</v>
+      </c>
+      <c r="C60" s="113" t="s">
+        <v>148</v>
+      </c>
       <c r="D60" s="99"/>
       <c r="E60" s="49"/>
       <c r="F60" s="49"/>
@@ -2576,12 +2550,14 @@
       <c r="H60" s="49"/>
       <c r="I60" s="50"/>
     </row>
-    <row r="61" spans="1:9" s="51" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:9" s="51" customFormat="1" ht="36" x14ac:dyDescent="0.45">
       <c r="A61" s="64"/>
-      <c r="B61" s="84" t="s">
-        <v>37</v>
-      </c>
-      <c r="C61" s="113"/>
+      <c r="B61" s="82" t="s">
+        <v>92</v>
+      </c>
+      <c r="C61" s="113" t="s">
+        <v>149</v>
+      </c>
       <c r="D61" s="99"/>
       <c r="E61" s="49"/>
       <c r="F61" s="49"/>
@@ -2589,13 +2565,13 @@
       <c r="H61" s="49"/>
       <c r="I61" s="50"/>
     </row>
-    <row r="62" spans="1:9" s="51" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:9" s="51" customFormat="1" ht="36" x14ac:dyDescent="0.45">
       <c r="A62" s="64"/>
       <c r="B62" s="82" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="C62" s="113" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D62" s="99"/>
       <c r="E62" s="49"/>
@@ -2604,20 +2580,87 @@
       <c r="H62" s="49"/>
       <c r="I62" s="50"/>
     </row>
-    <row r="63" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A63" s="64"/>
       <c r="B63" s="82" t="s">
-        <v>95</v>
-      </c>
-      <c r="C63" s="113" t="s">
-        <v>162</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="C63" s="113"/>
       <c r="D63" s="99"/>
       <c r="E63" s="49"/>
       <c r="F63" s="49"/>
       <c r="G63" s="49"/>
       <c r="H63" s="49"/>
       <c r="I63" s="50"/>
+    </row>
+    <row r="64" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A64" s="64"/>
+      <c r="B64" s="82" t="s">
+        <v>35</v>
+      </c>
+      <c r="C64" s="113"/>
+      <c r="D64" s="99"/>
+      <c r="E64" s="49"/>
+      <c r="F64" s="49"/>
+      <c r="G64" s="49"/>
+      <c r="H64" s="49"/>
+      <c r="I64" s="50"/>
+    </row>
+    <row r="65" spans="1:9" s="51" customFormat="1" ht="38.25" x14ac:dyDescent="0.45">
+      <c r="A65" s="64"/>
+      <c r="B65" s="84" t="s">
+        <v>36</v>
+      </c>
+      <c r="C65" s="113"/>
+      <c r="D65" s="99"/>
+      <c r="E65" s="49"/>
+      <c r="F65" s="49"/>
+      <c r="G65" s="49"/>
+      <c r="H65" s="49"/>
+      <c r="I65" s="50"/>
+    </row>
+    <row r="66" spans="1:9" s="51" customFormat="1" ht="25.5" x14ac:dyDescent="0.45">
+      <c r="A66" s="64"/>
+      <c r="B66" s="84" t="s">
+        <v>37</v>
+      </c>
+      <c r="C66" s="113"/>
+      <c r="D66" s="99"/>
+      <c r="E66" s="49"/>
+      <c r="F66" s="49"/>
+      <c r="G66" s="49"/>
+      <c r="H66" s="49"/>
+      <c r="I66" s="50"/>
+    </row>
+    <row r="67" spans="1:9" s="51" customFormat="1" ht="72" x14ac:dyDescent="0.45">
+      <c r="A67" s="64"/>
+      <c r="B67" s="82" t="s">
+        <v>94</v>
+      </c>
+      <c r="C67" s="113" t="s">
+        <v>151</v>
+      </c>
+      <c r="D67" s="99"/>
+      <c r="E67" s="49"/>
+      <c r="F67" s="49"/>
+      <c r="G67" s="49"/>
+      <c r="H67" s="49"/>
+      <c r="I67" s="50"/>
+    </row>
+    <row r="68" spans="1:9" s="51" customFormat="1" ht="24" x14ac:dyDescent="0.45">
+      <c r="A68" s="64"/>
+      <c r="B68" s="82" t="s">
+        <v>95</v>
+      </c>
+      <c r="C68" s="113" t="s">
+        <v>162</v>
+      </c>
+      <c r="D68" s="99"/>
+      <c r="E68" s="49"/>
+      <c r="F68" s="49"/>
+      <c r="G68" s="49"/>
+      <c r="H68" s="49"/>
+      <c r="I68" s="50"/>
     </row>
   </sheetData>
   <sheetProtection deleteColumns="0" selectLockedCells="1"/>
@@ -2678,7 +2721,7 @@
           <x14:formula1>
             <xm:f>'Drop Down List Values'!$M$2:$M$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D63:H63</xm:sqref>
+          <xm:sqref>D68:H68</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{33A578CF-33CA-4B41-B2C5-7541E5042FC9}">
           <x14:formula1>
@@ -2712,24 +2755,24 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="62" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="49.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="49.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -2770,7 +2813,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -2811,7 +2854,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -2852,7 +2895,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>168</v>
       </c>
@@ -2893,7 +2936,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -2925,7 +2968,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -2945,7 +2988,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -2966,65 +3009,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="b541edd5-2552-480e-ada6-0e2c8d317108">YVWEJ5DVYS2U-421999773-68</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="b541edd5-2552-480e-ada6-0e2c8d317108">
+      <Url>https://cdcpartners.sharepoint.com/sites/NCHS/nvssmodcop/_layouts/15/DocIdRedir.aspx?ID=YVWEJ5DVYS2U-421999773-68</Url>
+      <Description>YVWEJ5DVYS2U-421999773-68</Description>
+    </_dlc_DocIdUrl>
+    <ShareFileCreator xmlns="780ae317-08c5-4e10-af93-dd385a8384a9" xsi:nil="true"/>
+    <ShareFileCreated xmlns="780ae317-08c5-4e10-af93-dd385a8384a9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D4902BA52C7D94A994657A564808B2B" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e4455a60d2ff5f5fcd8815d6d89b5b66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b541edd5-2552-480e-ada6-0e2c8d317108" xmlns:ns3="780ae317-08c5-4e10-af93-dd385a8384a9" xmlns:ns4="3146657c-56f4-4c0a-bb9c-a675121ac670" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d1d01ecd782f081d5d944fa263943fc4" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="b541edd5-2552-480e-ada6-0e2c8d317108"/>
@@ -3223,37 +3221,84 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="b541edd5-2552-480e-ada6-0e2c8d317108">YVWEJ5DVYS2U-421999773-68</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="b541edd5-2552-480e-ada6-0e2c8d317108">
-      <Url>https://cdcpartners.sharepoint.com/sites/NCHS/nvssmodcop/_layouts/15/DocIdRedir.aspx?ID=YVWEJ5DVYS2U-421999773-68</Url>
-      <Description>YVWEJ5DVYS2U-421999773-68</Description>
-    </_dlc_DocIdUrl>
-    <ShareFileCreator xmlns="780ae317-08c5-4e10-af93-dd385a8384a9" xsi:nil="true"/>
-    <ShareFileCreated xmlns="780ae317-08c5-4e10-af93-dd385a8384a9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{448710E8-BE9E-4C9E-A40A-0AC1DAE48E99}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69E3EF86-6C9E-4C22-A476-13DA012C68C5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="780ae317-08c5-4e10-af93-dd385a8384a9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="3146657c-56f4-4c0a-bb9c-a675121ac670"/>
+    <ds:schemaRef ds:uri="b541edd5-2552-480e-ada6-0e2c8d317108"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF0D7A6D-D78F-4048-9348-0B4289842B11}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0980278E-2A79-4F44-8623-FE545C304BE1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3273,20 +3318,18 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF0D7A6D-D78F-4048-9348-0B4289842B11}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69E3EF86-6C9E-4C22-A476-13DA012C68C5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{448710E8-BE9E-4C9E-A40A-0AC1DAE48E99}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="780ae317-08c5-4e10-af93-dd385a8384a9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="3146657c-56f4-4c0a-bb9c-a675121ac670"/>
-    <ds:schemaRef ds:uri="b541edd5-2552-480e-ada6-0e2c8d317108"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added lines to excel file to autopsy location name.
</commit_message>
<xml_diff>
--- a/MDI-To-EDRS-Template.xlsx
+++ b/MDI-To-EDRS-Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mriley7\workspace\raven-import-and-submit-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80EE54F1-0FE6-469C-A3F2-C71DCB09E89B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F43D857-94EB-472C-B98C-8C7156000CAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8490" xr2:uid="{7A50F290-1C75-487E-9806-F93553E4E7CC}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="182">
   <si>
     <t>Manner of Death</t>
   </si>
@@ -677,6 +677,12 @@
   </si>
   <si>
     <t>Autopsy Performed Location: Postal Code</t>
+  </si>
+  <si>
+    <t>Autopsy Performed Office Name</t>
+  </si>
+  <si>
+    <t>Name of the office in which the autopsy took place</t>
   </si>
 </sst>
 </file>
@@ -971,7 +977,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -1130,10 +1136,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -1696,30 +1698,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54CD1DC7-E143-4CF5-BEA9-4DABBAFFC7B0}">
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="22.5" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" style="53" customWidth="1"/>
-    <col min="2" max="2" width="64.42578125" style="65" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" style="73" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" style="52" customWidth="1"/>
+    <col min="2" max="2" width="64.42578125" style="64" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" style="72" customWidth="1"/>
     <col min="4" max="8" width="32.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="64" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="73" t="s">
+      <c r="C1" s="72" t="s">
         <v>27</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -1742,27 +1744,27 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="36.75" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C2" s="73" t="s">
+      <c r="C2" s="72" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="120" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="52" t="s">
         <v>169</v>
       </c>
-      <c r="B3" s="121" t="s">
+      <c r="B3" s="120" t="s">
         <v>171</v>
       </c>
-      <c r="C3" s="122" t="s">
+      <c r="C3" s="121" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="4" customFormat="1" ht="36.75" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="100" t="s">
+      <c r="B4" s="65"/>
+      <c r="C4" s="99" t="s">
         <v>101</v>
       </c>
       <c r="D4" s="3"/>
@@ -1772,42 +1774,42 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" s="6" customFormat="1" ht="29.25" x14ac:dyDescent="0.45">
-      <c r="A5" s="55"/>
-      <c r="B5" s="118" t="s">
+    <row r="5" spans="1:9" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.45">
+      <c r="A5" s="54"/>
+      <c r="B5" s="117" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="101" t="s">
+      <c r="C5" s="100" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
       <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:9" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.45">
-      <c r="A6" s="55"/>
-      <c r="B6" s="119" t="s">
+      <c r="A6" s="54"/>
+      <c r="B6" s="118" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="101" t="s">
+      <c r="C6" s="100" t="s">
         <v>103</v>
       </c>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
       <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:9" s="8" customFormat="1" ht="36" x14ac:dyDescent="0.45">
-      <c r="A7" s="56" t="s">
+      <c r="A7" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="67"/>
-      <c r="C7" s="102" t="s">
+      <c r="B7" s="66"/>
+      <c r="C7" s="101" t="s">
         <v>105</v>
       </c>
       <c r="D7" s="7"/>
@@ -1818,11 +1820,11 @@
       <c r="I7" s="7"/>
     </row>
     <row r="8" spans="1:9" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.45">
-      <c r="A8" s="57"/>
-      <c r="B8" s="74" t="s">
+      <c r="A8" s="56"/>
+      <c r="B8" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="103" t="s">
+      <c r="C8" s="102" t="s">
         <v>104</v>
       </c>
       <c r="D8" s="14"/>
@@ -1833,11 +1835,11 @@
       <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:9" s="11" customFormat="1" ht="60" x14ac:dyDescent="0.45">
-      <c r="A9" s="57"/>
-      <c r="B9" s="74" t="s">
+      <c r="A9" s="56"/>
+      <c r="B9" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="103" t="s">
+      <c r="C9" s="102" t="s">
         <v>108</v>
       </c>
       <c r="D9" s="14"/>
@@ -1848,11 +1850,11 @@
       <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:9" s="11" customFormat="1" ht="24" x14ac:dyDescent="0.45">
-      <c r="A10" s="57"/>
-      <c r="B10" s="74" t="s">
+      <c r="A10" s="56"/>
+      <c r="B10" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="103" t="s">
+      <c r="C10" s="102" t="s">
         <v>107</v>
       </c>
       <c r="D10" s="14"/>
@@ -1863,11 +1865,11 @@
       <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9" s="11" customFormat="1" ht="36" x14ac:dyDescent="0.45">
-      <c r="A11" s="57"/>
-      <c r="B11" s="75" t="s">
+      <c r="A11" s="56"/>
+      <c r="B11" s="74" t="s">
         <v>76</v>
       </c>
-      <c r="C11" s="103" t="s">
+      <c r="C11" s="102" t="s">
         <v>106</v>
       </c>
       <c r="D11" s="14"/>
@@ -1878,11 +1880,11 @@
       <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:9" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.45">
-      <c r="A12" s="57"/>
-      <c r="B12" s="74" t="s">
+      <c r="A12" s="56"/>
+      <c r="B12" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="103" t="s">
+      <c r="C12" s="102" t="s">
         <v>155</v>
       </c>
       <c r="D12" s="14"/>
@@ -1893,11 +1895,11 @@
       <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.45">
-      <c r="A13" s="57"/>
-      <c r="B13" s="74" t="s">
+      <c r="A13" s="56"/>
+      <c r="B13" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="103" t="s">
+      <c r="C13" s="102" t="s">
         <v>109</v>
       </c>
       <c r="D13" s="14"/>
@@ -1908,14 +1910,14 @@
       <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.45">
-      <c r="A14" s="57"/>
-      <c r="B14" s="74" t="s">
+      <c r="A14" s="56"/>
+      <c r="B14" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="103" t="s">
+      <c r="C14" s="102" t="s">
         <v>110</v>
       </c>
-      <c r="D14" s="85"/>
+      <c r="D14" s="84"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
@@ -1923,11 +1925,11 @@
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="57"/>
-      <c r="B15" s="74" t="s">
+      <c r="A15" s="56"/>
+      <c r="B15" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="103"/>
+      <c r="C15" s="102"/>
       <c r="D15" s="14"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
@@ -1936,14 +1938,14 @@
       <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:9" s="11" customFormat="1" ht="24" x14ac:dyDescent="0.45">
-      <c r="A16" s="57"/>
-      <c r="B16" s="74" t="s">
+      <c r="A16" s="56"/>
+      <c r="B16" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="103" t="s">
+      <c r="C16" s="102" t="s">
         <v>111</v>
       </c>
-      <c r="D16" s="86"/>
+      <c r="D16" s="85"/>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
@@ -1951,11 +1953,11 @@
       <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="57"/>
-      <c r="B17" s="74" t="s">
+      <c r="A17" s="56"/>
+      <c r="B17" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="103"/>
+      <c r="C17" s="102"/>
       <c r="D17" s="14"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
@@ -1964,11 +1966,11 @@
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="57"/>
-      <c r="B18" s="74" t="s">
+      <c r="A18" s="56"/>
+      <c r="B18" s="73" t="s">
         <v>99</v>
       </c>
-      <c r="C18" s="103"/>
+      <c r="C18" s="102"/>
       <c r="D18" s="14"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
@@ -1976,12 +1978,12 @@
       <c r="H18" s="9"/>
       <c r="I18" s="10"/>
     </row>
-    <row r="19" spans="1:9" s="11" customFormat="1" ht="38.25" x14ac:dyDescent="0.45">
-      <c r="A19" s="57"/>
-      <c r="B19" s="76" t="s">
+    <row r="19" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="56"/>
+      <c r="B19" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="103"/>
+      <c r="C19" s="102"/>
       <c r="D19" s="14"/>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
@@ -1990,11 +1992,11 @@
       <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="57"/>
-      <c r="B20" s="74" t="s">
+      <c r="A20" s="56"/>
+      <c r="B20" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="103"/>
+      <c r="C20" s="102"/>
       <c r="D20" s="14"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
@@ -2003,11 +2005,11 @@
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="57"/>
-      <c r="B21" s="74" t="s">
+      <c r="A21" s="56"/>
+      <c r="B21" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="103"/>
+      <c r="C21" s="102"/>
       <c r="D21" s="14"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
@@ -2016,11 +2018,11 @@
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" s="16" customFormat="1" ht="84" x14ac:dyDescent="0.45">
-      <c r="A22" s="114" t="s">
+      <c r="A22" s="113" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="68"/>
-      <c r="C22" s="104" t="s">
+      <c r="B22" s="67"/>
+      <c r="C22" s="103" t="s">
         <v>112</v>
       </c>
       <c r="D22" s="15"/>
@@ -2031,14 +2033,14 @@
       <c r="I22" s="15"/>
     </row>
     <row r="23" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="58"/>
-      <c r="B23" s="120" t="s">
+      <c r="A23" s="57"/>
+      <c r="B23" s="119" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="105" t="s">
+      <c r="C23" s="104" t="s">
         <v>113</v>
       </c>
-      <c r="D23" s="87"/>
+      <c r="D23" s="86"/>
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
@@ -2046,14 +2048,14 @@
       <c r="I23" s="18"/>
     </row>
     <row r="24" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="58"/>
-      <c r="B24" s="120" t="s">
+      <c r="A24" s="57"/>
+      <c r="B24" s="119" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="105" t="s">
+      <c r="C24" s="104" t="s">
         <v>114</v>
       </c>
-      <c r="D24" s="88"/>
+      <c r="D24" s="87"/>
       <c r="E24" s="20"/>
       <c r="F24" s="20"/>
       <c r="G24" s="20"/>
@@ -2061,14 +2063,14 @@
       <c r="I24" s="18"/>
     </row>
     <row r="25" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="58"/>
-      <c r="B25" s="120" t="s">
+      <c r="A25" s="57"/>
+      <c r="B25" s="119" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="105" t="s">
+      <c r="C25" s="104" t="s">
         <v>115</v>
       </c>
-      <c r="D25" s="89"/>
+      <c r="D25" s="88"/>
       <c r="E25" s="21"/>
       <c r="F25" s="21"/>
       <c r="G25" s="21"/>
@@ -2076,14 +2078,14 @@
       <c r="I25" s="18"/>
     </row>
     <row r="26" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="58"/>
-      <c r="B26" s="120" t="s">
+      <c r="A26" s="57"/>
+      <c r="B26" s="119" t="s">
         <v>98</v>
       </c>
-      <c r="C26" s="105" t="s">
+      <c r="C26" s="104" t="s">
         <v>116</v>
       </c>
-      <c r="D26" s="89"/>
+      <c r="D26" s="88"/>
       <c r="E26" s="21"/>
       <c r="F26" s="21"/>
       <c r="G26" s="21"/>
@@ -2091,14 +2093,14 @@
       <c r="I26" s="18"/>
     </row>
     <row r="27" spans="1:9" s="19" customFormat="1" ht="48" x14ac:dyDescent="0.45">
-      <c r="A27" s="58"/>
-      <c r="B27" s="120" t="s">
+      <c r="A27" s="57"/>
+      <c r="B27" s="119" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="105" t="s">
+      <c r="C27" s="104" t="s">
         <v>117</v>
       </c>
-      <c r="D27" s="89"/>
+      <c r="D27" s="88"/>
       <c r="E27" s="21"/>
       <c r="F27" s="21"/>
       <c r="G27" s="21"/>
@@ -2106,14 +2108,14 @@
       <c r="I27" s="18"/>
     </row>
     <row r="28" spans="1:9" s="19" customFormat="1" ht="48" x14ac:dyDescent="0.45">
-      <c r="A28" s="58"/>
-      <c r="B28" s="120" t="s">
+      <c r="A28" s="57"/>
+      <c r="B28" s="119" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="105" t="s">
+      <c r="C28" s="104" t="s">
         <v>118</v>
       </c>
-      <c r="D28" s="89"/>
+      <c r="D28" s="88"/>
       <c r="E28" s="21"/>
       <c r="F28" s="21"/>
       <c r="G28" s="21"/>
@@ -2121,14 +2123,14 @@
       <c r="I28" s="18"/>
     </row>
     <row r="29" spans="1:9" s="19" customFormat="1" ht="48" x14ac:dyDescent="0.45">
-      <c r="A29" s="58"/>
-      <c r="B29" s="120" t="s">
+      <c r="A29" s="57"/>
+      <c r="B29" s="119" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="105" t="s">
+      <c r="C29" s="104" t="s">
         <v>119</v>
       </c>
-      <c r="D29" s="89"/>
+      <c r="D29" s="88"/>
       <c r="E29" s="21"/>
       <c r="F29" s="21"/>
       <c r="G29" s="21"/>
@@ -2136,14 +2138,14 @@
       <c r="I29" s="18"/>
     </row>
     <row r="30" spans="1:9" s="19" customFormat="1" ht="48" x14ac:dyDescent="0.45">
-      <c r="A30" s="58"/>
-      <c r="B30" s="120" t="s">
+      <c r="A30" s="57"/>
+      <c r="B30" s="119" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="105" t="s">
+      <c r="C30" s="104" t="s">
         <v>120</v>
       </c>
-      <c r="D30" s="87"/>
+      <c r="D30" s="86"/>
       <c r="E30" s="17"/>
       <c r="F30" s="17"/>
       <c r="G30" s="17"/>
@@ -2151,14 +2153,14 @@
       <c r="I30" s="18"/>
     </row>
     <row r="31" spans="1:9" s="19" customFormat="1" ht="48" x14ac:dyDescent="0.45">
-      <c r="A31" s="58"/>
-      <c r="B31" s="120" t="s">
+      <c r="A31" s="57"/>
+      <c r="B31" s="119" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="105" t="s">
+      <c r="C31" s="104" t="s">
         <v>121</v>
       </c>
-      <c r="D31" s="90"/>
+      <c r="D31" s="89"/>
       <c r="E31" s="22"/>
       <c r="F31" s="22"/>
       <c r="G31" s="22"/>
@@ -2166,14 +2168,14 @@
       <c r="I31" s="18"/>
     </row>
     <row r="32" spans="1:9" s="19" customFormat="1" ht="24" x14ac:dyDescent="0.45">
-      <c r="A32" s="58"/>
-      <c r="B32" s="77" t="s">
+      <c r="A32" s="57"/>
+      <c r="B32" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="105" t="s">
+      <c r="C32" s="104" t="s">
         <v>122</v>
       </c>
-      <c r="D32" s="90"/>
+      <c r="D32" s="89"/>
       <c r="E32" s="22"/>
       <c r="F32" s="22"/>
       <c r="G32" s="22"/>
@@ -2181,14 +2183,14 @@
       <c r="I32" s="18"/>
     </row>
     <row r="33" spans="1:9" s="19" customFormat="1" ht="60" x14ac:dyDescent="0.45">
-      <c r="A33" s="58"/>
-      <c r="B33" s="77" t="s">
+      <c r="A33" s="57"/>
+      <c r="B33" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="105" t="s">
+      <c r="C33" s="104" t="s">
         <v>123</v>
       </c>
-      <c r="D33" s="91"/>
+      <c r="D33" s="90"/>
       <c r="E33" s="23"/>
       <c r="F33" s="23"/>
       <c r="G33" s="23"/>
@@ -2196,14 +2198,14 @@
       <c r="I33" s="18"/>
     </row>
     <row r="34" spans="1:9" s="19" customFormat="1" ht="84" x14ac:dyDescent="0.45">
-      <c r="A34" s="58"/>
-      <c r="B34" s="77" t="s">
+      <c r="A34" s="57"/>
+      <c r="B34" s="76" t="s">
         <v>83</v>
       </c>
-      <c r="C34" s="105" t="s">
+      <c r="C34" s="104" t="s">
         <v>124</v>
       </c>
-      <c r="D34" s="90"/>
+      <c r="D34" s="89"/>
       <c r="E34" s="22"/>
       <c r="F34" s="24"/>
       <c r="G34" s="22"/>
@@ -2211,14 +2213,14 @@
       <c r="I34" s="18"/>
     </row>
     <row r="35" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="59"/>
-      <c r="B35" s="77" t="s">
+      <c r="A35" s="58"/>
+      <c r="B35" s="76" t="s">
         <v>82</v>
       </c>
-      <c r="C35" s="105" t="s">
+      <c r="C35" s="104" t="s">
         <v>125</v>
       </c>
-      <c r="D35" s="89"/>
+      <c r="D35" s="88"/>
       <c r="E35" s="21"/>
       <c r="F35" s="21"/>
       <c r="G35" s="21"/>
@@ -2226,14 +2228,14 @@
       <c r="I35" s="25"/>
     </row>
     <row r="36" spans="1:9" s="19" customFormat="1" ht="36" x14ac:dyDescent="0.45">
-      <c r="A36" s="58"/>
-      <c r="B36" s="77" t="s">
+      <c r="A36" s="57"/>
+      <c r="B36" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="C36" s="105" t="s">
+      <c r="C36" s="104" t="s">
         <v>126</v>
       </c>
-      <c r="D36" s="90"/>
+      <c r="D36" s="89"/>
       <c r="E36" s="22"/>
       <c r="F36" s="22"/>
       <c r="G36" s="22"/>
@@ -2241,14 +2243,14 @@
       <c r="I36" s="18"/>
     </row>
     <row r="37" spans="1:9" s="19" customFormat="1" ht="36" x14ac:dyDescent="0.45">
-      <c r="A37" s="58"/>
-      <c r="B37" s="77" t="s">
+      <c r="A37" s="57"/>
+      <c r="B37" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="C37" s="105" t="s">
+      <c r="C37" s="104" t="s">
         <v>127</v>
       </c>
-      <c r="D37" s="90"/>
+      <c r="D37" s="89"/>
       <c r="E37" s="22"/>
       <c r="F37" s="22"/>
       <c r="G37" s="22"/>
@@ -2256,11 +2258,11 @@
       <c r="I37" s="18"/>
     </row>
     <row r="38" spans="1:9" s="28" customFormat="1" ht="84" x14ac:dyDescent="0.45">
-      <c r="A38" s="115" t="s">
+      <c r="A38" s="114" t="s">
         <v>30</v>
       </c>
-      <c r="B38" s="69"/>
-      <c r="C38" s="106" t="s">
+      <c r="B38" s="68"/>
+      <c r="C38" s="105" t="s">
         <v>143</v>
       </c>
       <c r="D38" s="27"/>
@@ -2271,14 +2273,14 @@
       <c r="I38" s="27"/>
     </row>
     <row r="39" spans="1:9" s="31" customFormat="1" ht="24" x14ac:dyDescent="0.45">
-      <c r="A39" s="60"/>
-      <c r="B39" s="78" t="s">
+      <c r="A39" s="59"/>
+      <c r="B39" s="77" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="107" t="s">
+      <c r="C39" s="106" t="s">
         <v>128</v>
       </c>
-      <c r="D39" s="92"/>
+      <c r="D39" s="91"/>
       <c r="E39" s="29"/>
       <c r="F39" s="29"/>
       <c r="G39" s="29"/>
@@ -2286,14 +2288,14 @@
       <c r="I39" s="30"/>
     </row>
     <row r="40" spans="1:9" s="31" customFormat="1" ht="24" x14ac:dyDescent="0.45">
-      <c r="A40" s="60"/>
-      <c r="B40" s="79" t="s">
+      <c r="A40" s="59"/>
+      <c r="B40" s="78" t="s">
         <v>96</v>
       </c>
-      <c r="C40" s="107" t="s">
+      <c r="C40" s="106" t="s">
         <v>166</v>
       </c>
-      <c r="D40" s="92"/>
+      <c r="D40" s="91"/>
       <c r="E40" s="29"/>
       <c r="F40" s="32"/>
       <c r="G40" s="29"/>
@@ -2301,29 +2303,29 @@
       <c r="I40" s="30"/>
     </row>
     <row r="41" spans="1:9" s="31" customFormat="1" ht="36" x14ac:dyDescent="0.45">
-      <c r="A41" s="60"/>
-      <c r="B41" s="78" t="s">
+      <c r="A41" s="59"/>
+      <c r="B41" s="77" t="s">
         <v>77</v>
       </c>
-      <c r="C41" s="107" t="s">
+      <c r="C41" s="106" t="s">
         <v>129</v>
       </c>
-      <c r="D41" s="92"/>
-      <c r="E41" s="92"/>
-      <c r="F41" s="92"/>
-      <c r="G41" s="92"/>
-      <c r="H41" s="92"/>
+      <c r="D41" s="91"/>
+      <c r="E41" s="91"/>
+      <c r="F41" s="91"/>
+      <c r="G41" s="91"/>
+      <c r="H41" s="91"/>
       <c r="I41" s="30"/>
     </row>
     <row r="42" spans="1:9" s="31" customFormat="1" ht="36" x14ac:dyDescent="0.45">
-      <c r="A42" s="60"/>
-      <c r="B42" s="117" t="s">
+      <c r="A42" s="59"/>
+      <c r="B42" s="116" t="s">
         <v>1</v>
       </c>
-      <c r="C42" s="107" t="s">
+      <c r="C42" s="106" t="s">
         <v>130</v>
       </c>
-      <c r="D42" s="92"/>
+      <c r="D42" s="91"/>
       <c r="E42" s="29"/>
       <c r="F42" s="29"/>
       <c r="G42" s="29"/>
@@ -2331,14 +2333,14 @@
       <c r="I42" s="30"/>
     </row>
     <row r="43" spans="1:9" s="35" customFormat="1" ht="60" x14ac:dyDescent="0.45">
-      <c r="A43" s="123" t="s">
+      <c r="A43" s="122" t="s">
         <v>172</v>
       </c>
-      <c r="B43" s="70"/>
-      <c r="C43" s="108" t="s">
+      <c r="B43" s="69"/>
+      <c r="C43" s="107" t="s">
         <v>144</v>
       </c>
-      <c r="D43" s="93"/>
+      <c r="D43" s="92"/>
       <c r="E43" s="33"/>
       <c r="F43" s="33"/>
       <c r="G43" s="33"/>
@@ -2346,14 +2348,14 @@
       <c r="I43" s="34"/>
     </row>
     <row r="44" spans="1:9" s="38" customFormat="1" ht="48" x14ac:dyDescent="0.45">
-      <c r="A44" s="61"/>
-      <c r="B44" s="80" t="s">
+      <c r="A44" s="60"/>
+      <c r="B44" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="C44" s="109" t="s">
+      <c r="C44" s="108" t="s">
         <v>131</v>
       </c>
-      <c r="D44" s="94"/>
+      <c r="D44" s="93"/>
       <c r="E44" s="36"/>
       <c r="F44" s="36"/>
       <c r="G44" s="36"/>
@@ -2361,14 +2363,14 @@
       <c r="I44" s="37"/>
     </row>
     <row r="45" spans="1:9" s="38" customFormat="1" ht="84" x14ac:dyDescent="0.45">
-      <c r="A45" s="61"/>
-      <c r="B45" s="80" t="s">
+      <c r="A45" s="60"/>
+      <c r="B45" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="C45" s="109" t="s">
+      <c r="C45" s="108" t="s">
         <v>132</v>
       </c>
-      <c r="D45" s="95"/>
+      <c r="D45" s="94"/>
       <c r="E45" s="39"/>
       <c r="F45" s="39"/>
       <c r="G45" s="39"/>
@@ -2376,14 +2378,14 @@
       <c r="I45" s="37"/>
     </row>
     <row r="46" spans="1:9" s="38" customFormat="1" ht="36" x14ac:dyDescent="0.45">
-      <c r="A46" s="61"/>
-      <c r="B46" s="80" t="s">
+      <c r="A46" s="60"/>
+      <c r="B46" s="79" t="s">
         <v>78</v>
       </c>
-      <c r="C46" s="109" t="s">
+      <c r="C46" s="108" t="s">
         <v>137</v>
       </c>
-      <c r="D46" s="96"/>
+      <c r="D46" s="95"/>
       <c r="E46" s="40"/>
       <c r="F46" s="40"/>
       <c r="G46" s="40"/>
@@ -2391,14 +2393,14 @@
       <c r="I46" s="37"/>
     </row>
     <row r="47" spans="1:9" s="38" customFormat="1" ht="60" x14ac:dyDescent="0.45">
-      <c r="A47" s="61"/>
-      <c r="B47" s="80" t="s">
+      <c r="A47" s="60"/>
+      <c r="B47" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="C47" s="109" t="s">
+      <c r="C47" s="108" t="s">
         <v>138</v>
       </c>
-      <c r="D47" s="97"/>
+      <c r="D47" s="96"/>
       <c r="E47" s="41"/>
       <c r="F47" s="41"/>
       <c r="G47" s="41"/>
@@ -2406,14 +2408,14 @@
       <c r="I47" s="37"/>
     </row>
     <row r="48" spans="1:9" s="38" customFormat="1" ht="96" x14ac:dyDescent="0.45">
-      <c r="A48" s="61"/>
-      <c r="B48" s="80" t="s">
+      <c r="A48" s="60"/>
+      <c r="B48" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="C48" s="109" t="s">
+      <c r="C48" s="108" t="s">
         <v>139</v>
       </c>
-      <c r="D48" s="95"/>
+      <c r="D48" s="94"/>
       <c r="E48" s="39"/>
       <c r="F48" s="39"/>
       <c r="G48" s="39"/>
@@ -2421,14 +2423,14 @@
       <c r="I48" s="37"/>
     </row>
     <row r="49" spans="1:9" s="38" customFormat="1" ht="36" x14ac:dyDescent="0.45">
-      <c r="A49" s="61"/>
-      <c r="B49" s="80" t="s">
+      <c r="A49" s="60"/>
+      <c r="B49" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="C49" s="109" t="s">
+      <c r="C49" s="108" t="s">
         <v>140</v>
       </c>
-      <c r="D49" s="96"/>
+      <c r="D49" s="95"/>
       <c r="E49" s="40"/>
       <c r="F49" s="40"/>
       <c r="G49" s="40"/>
@@ -2436,11 +2438,11 @@
       <c r="I49" s="37"/>
     </row>
     <row r="50" spans="1:9" s="43" customFormat="1" ht="24" x14ac:dyDescent="0.45">
-      <c r="A50" s="62" t="s">
+      <c r="A50" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="B50" s="71"/>
-      <c r="C50" s="110" t="s">
+      <c r="B50" s="70"/>
+      <c r="C50" s="109" t="s">
         <v>145</v>
       </c>
       <c r="D50" s="42"/>
@@ -2450,217 +2452,260 @@
       <c r="H50" s="42"/>
       <c r="I50" s="42"/>
     </row>
-    <row r="51" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="63"/>
-      <c r="B51" s="81" t="s">
+    <row r="51" spans="1:9" s="45" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A51" s="62"/>
+      <c r="B51" s="80" t="s">
         <v>45</v>
       </c>
-      <c r="C51" s="111" t="s">
+      <c r="C51" s="110" t="s">
         <v>141</v>
       </c>
-      <c r="D51" s="98"/>
-      <c r="E51" s="44"/>
-      <c r="F51" s="44"/>
-      <c r="G51" s="44"/>
-      <c r="H51" s="44"/>
-      <c r="I51" s="45"/>
-    </row>
-    <row r="52" spans="1:9" s="63" customFormat="1" ht="36" x14ac:dyDescent="0.45">
-      <c r="B52" s="81" t="s">
+      <c r="D51" s="97"/>
+      <c r="E51" s="97"/>
+      <c r="F51" s="97"/>
+      <c r="G51" s="97"/>
+      <c r="H51" s="97"/>
+      <c r="I51" s="44"/>
+    </row>
+    <row r="52" spans="1:9" s="62" customFormat="1" ht="36" x14ac:dyDescent="0.45">
+      <c r="B52" s="80" t="s">
         <v>81</v>
       </c>
-      <c r="C52" s="111" t="s">
+      <c r="C52" s="110" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" s="63" customFormat="1" ht="24" x14ac:dyDescent="0.45">
-      <c r="B53" s="81" t="s">
+      <c r="D52" s="97"/>
+      <c r="E52" s="97"/>
+      <c r="F52" s="97"/>
+      <c r="G52" s="97"/>
+      <c r="H52" s="97"/>
+    </row>
+    <row r="53" spans="1:9" s="62" customFormat="1" ht="24" x14ac:dyDescent="0.45">
+      <c r="B53" s="80" t="s">
+        <v>180</v>
+      </c>
+      <c r="C53" s="110" t="s">
+        <v>181</v>
+      </c>
+      <c r="D53" s="97"/>
+      <c r="E53" s="97"/>
+      <c r="F53" s="97"/>
+      <c r="G53" s="97"/>
+      <c r="H53" s="97"/>
+    </row>
+    <row r="54" spans="1:9" s="62" customFormat="1" ht="24" x14ac:dyDescent="0.45">
+      <c r="B54" s="80" t="s">
         <v>174</v>
       </c>
-      <c r="C53" s="111" t="s">
+      <c r="C54" s="110" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" s="63" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B54" s="81" t="s">
+      <c r="D54" s="97"/>
+      <c r="E54" s="97"/>
+      <c r="F54" s="97"/>
+      <c r="G54" s="97"/>
+      <c r="H54" s="97"/>
+    </row>
+    <row r="55" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B55" s="80" t="s">
         <v>175</v>
       </c>
-      <c r="C54" s="111"/>
-    </row>
-    <row r="55" spans="1:9" s="63" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B55" s="81" t="s">
+      <c r="C55" s="110"/>
+      <c r="D55" s="97"/>
+      <c r="E55" s="97"/>
+      <c r="F55" s="97"/>
+      <c r="G55" s="97"/>
+      <c r="H55" s="97"/>
+    </row>
+    <row r="56" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B56" s="80" t="s">
         <v>176</v>
       </c>
-      <c r="C55" s="111"/>
-    </row>
-    <row r="56" spans="1:9" s="63" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B56" s="81" t="s">
+      <c r="C56" s="110"/>
+      <c r="D56" s="97"/>
+      <c r="E56" s="97"/>
+      <c r="F56" s="97"/>
+      <c r="G56" s="97"/>
+      <c r="H56" s="97"/>
+    </row>
+    <row r="57" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B57" s="80" t="s">
         <v>178</v>
       </c>
-      <c r="C56" s="111"/>
-    </row>
-    <row r="57" spans="1:9" s="63" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B57" s="81" t="s">
+      <c r="C57" s="110"/>
+      <c r="D57" s="97"/>
+      <c r="E57" s="97"/>
+      <c r="F57" s="97"/>
+      <c r="G57" s="97"/>
+      <c r="H57" s="97"/>
+    </row>
+    <row r="58" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B58" s="80" t="s">
         <v>179</v>
       </c>
-      <c r="C57" s="111"/>
-    </row>
-    <row r="58" spans="1:9" s="48" customFormat="1" ht="36" x14ac:dyDescent="0.45">
-      <c r="A58" s="116" t="s">
+      <c r="C58" s="110"/>
+      <c r="D58" s="97"/>
+      <c r="E58" s="97"/>
+      <c r="F58" s="97"/>
+      <c r="G58" s="97"/>
+      <c r="H58" s="97"/>
+    </row>
+    <row r="59" spans="1:9" s="47" customFormat="1" ht="36" x14ac:dyDescent="0.45">
+      <c r="A59" s="115" t="s">
         <v>173</v>
       </c>
-      <c r="B58" s="72"/>
-      <c r="C58" s="112" t="s">
+      <c r="B59" s="71"/>
+      <c r="C59" s="111" t="s">
         <v>146</v>
       </c>
-      <c r="D58" s="47"/>
-      <c r="E58" s="47"/>
-      <c r="F58" s="47"/>
-      <c r="G58" s="47"/>
-      <c r="H58" s="47"/>
-      <c r="I58" s="47"/>
-    </row>
-    <row r="59" spans="1:9" s="51" customFormat="1" ht="72" x14ac:dyDescent="0.45">
-      <c r="A59" s="64"/>
-      <c r="B59" s="82" t="s">
+      <c r="D59" s="46"/>
+      <c r="E59" s="46"/>
+      <c r="F59" s="46"/>
+      <c r="G59" s="46"/>
+      <c r="H59" s="46"/>
+      <c r="I59" s="46"/>
+    </row>
+    <row r="60" spans="1:9" s="50" customFormat="1" ht="72" x14ac:dyDescent="0.45">
+      <c r="A60" s="63"/>
+      <c r="B60" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="C59" s="113" t="s">
+      <c r="C60" s="112" t="s">
         <v>147</v>
       </c>
-      <c r="D59" s="99"/>
-      <c r="E59" s="49"/>
-      <c r="F59" s="49"/>
-      <c r="G59" s="49"/>
-      <c r="H59" s="49"/>
-      <c r="I59" s="50"/>
-    </row>
-    <row r="60" spans="1:9" s="51" customFormat="1" ht="48" x14ac:dyDescent="0.45">
-      <c r="A60" s="64"/>
-      <c r="B60" s="83" t="s">
+      <c r="D60" s="98"/>
+      <c r="E60" s="48"/>
+      <c r="F60" s="48"/>
+      <c r="G60" s="48"/>
+      <c r="H60" s="48"/>
+      <c r="I60" s="49"/>
+    </row>
+    <row r="61" spans="1:9" s="50" customFormat="1" ht="48" x14ac:dyDescent="0.45">
+      <c r="A61" s="63"/>
+      <c r="B61" s="82" t="s">
         <v>91</v>
       </c>
-      <c r="C60" s="113" t="s">
+      <c r="C61" s="112" t="s">
         <v>148</v>
       </c>
-      <c r="D60" s="99"/>
-      <c r="E60" s="49"/>
-      <c r="F60" s="49"/>
-      <c r="G60" s="49"/>
-      <c r="H60" s="49"/>
-      <c r="I60" s="50"/>
-    </row>
-    <row r="61" spans="1:9" s="51" customFormat="1" ht="36" x14ac:dyDescent="0.45">
-      <c r="A61" s="64"/>
-      <c r="B61" s="82" t="s">
+      <c r="D61" s="98"/>
+      <c r="E61" s="48"/>
+      <c r="F61" s="48"/>
+      <c r="G61" s="48"/>
+      <c r="H61" s="48"/>
+      <c r="I61" s="49"/>
+    </row>
+    <row r="62" spans="1:9" s="50" customFormat="1" ht="36" x14ac:dyDescent="0.45">
+      <c r="A62" s="63"/>
+      <c r="B62" s="81" t="s">
         <v>92</v>
       </c>
-      <c r="C61" s="113" t="s">
+      <c r="C62" s="112" t="s">
         <v>149</v>
       </c>
-      <c r="D61" s="99"/>
-      <c r="E61" s="49"/>
-      <c r="F61" s="49"/>
-      <c r="G61" s="49"/>
-      <c r="H61" s="49"/>
-      <c r="I61" s="50"/>
-    </row>
-    <row r="62" spans="1:9" s="51" customFormat="1" ht="36" x14ac:dyDescent="0.45">
-      <c r="A62" s="64"/>
-      <c r="B62" s="82" t="s">
+      <c r="D62" s="98"/>
+      <c r="E62" s="48"/>
+      <c r="F62" s="48"/>
+      <c r="G62" s="48"/>
+      <c r="H62" s="48"/>
+      <c r="I62" s="49"/>
+    </row>
+    <row r="63" spans="1:9" s="50" customFormat="1" ht="36" x14ac:dyDescent="0.45">
+      <c r="A63" s="63"/>
+      <c r="B63" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="C62" s="113" t="s">
+      <c r="C63" s="112" t="s">
         <v>150</v>
       </c>
-      <c r="D62" s="99"/>
-      <c r="E62" s="49"/>
-      <c r="F62" s="49"/>
-      <c r="G62" s="49"/>
-      <c r="H62" s="49"/>
-      <c r="I62" s="50"/>
-    </row>
-    <row r="63" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A63" s="64"/>
-      <c r="B63" s="82" t="s">
+      <c r="D63" s="98"/>
+      <c r="E63" s="48"/>
+      <c r="F63" s="48"/>
+      <c r="G63" s="48"/>
+      <c r="H63" s="48"/>
+      <c r="I63" s="49"/>
+    </row>
+    <row r="64" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A64" s="63"/>
+      <c r="B64" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="C63" s="113"/>
-      <c r="D63" s="99"/>
-      <c r="E63" s="49"/>
-      <c r="F63" s="49"/>
-      <c r="G63" s="49"/>
-      <c r="H63" s="49"/>
-      <c r="I63" s="50"/>
-    </row>
-    <row r="64" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A64" s="64"/>
-      <c r="B64" s="82" t="s">
+      <c r="C64" s="112"/>
+      <c r="D64" s="98"/>
+      <c r="E64" s="48"/>
+      <c r="F64" s="48"/>
+      <c r="G64" s="48"/>
+      <c r="H64" s="48"/>
+      <c r="I64" s="49"/>
+    </row>
+    <row r="65" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A65" s="63"/>
+      <c r="B65" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="C64" s="113"/>
-      <c r="D64" s="99"/>
-      <c r="E64" s="49"/>
-      <c r="F64" s="49"/>
-      <c r="G64" s="49"/>
-      <c r="H64" s="49"/>
-      <c r="I64" s="50"/>
-    </row>
-    <row r="65" spans="1:9" s="51" customFormat="1" ht="38.25" x14ac:dyDescent="0.45">
-      <c r="A65" s="64"/>
-      <c r="B65" s="84" t="s">
+      <c r="C65" s="112"/>
+      <c r="D65" s="98"/>
+      <c r="E65" s="48"/>
+      <c r="F65" s="48"/>
+      <c r="G65" s="48"/>
+      <c r="H65" s="48"/>
+      <c r="I65" s="49"/>
+    </row>
+    <row r="66" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A66" s="63"/>
+      <c r="B66" s="83" t="s">
         <v>36</v>
       </c>
-      <c r="C65" s="113"/>
-      <c r="D65" s="99"/>
-      <c r="E65" s="49"/>
-      <c r="F65" s="49"/>
-      <c r="G65" s="49"/>
-      <c r="H65" s="49"/>
-      <c r="I65" s="50"/>
-    </row>
-    <row r="66" spans="1:9" s="51" customFormat="1" ht="25.5" x14ac:dyDescent="0.45">
-      <c r="A66" s="64"/>
-      <c r="B66" s="84" t="s">
+      <c r="C66" s="112"/>
+      <c r="D66" s="98"/>
+      <c r="E66" s="48"/>
+      <c r="F66" s="48"/>
+      <c r="G66" s="48"/>
+      <c r="H66" s="48"/>
+      <c r="I66" s="49"/>
+    </row>
+    <row r="67" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A67" s="63"/>
+      <c r="B67" s="83" t="s">
         <v>37</v>
       </c>
-      <c r="C66" s="113"/>
-      <c r="D66" s="99"/>
-      <c r="E66" s="49"/>
-      <c r="F66" s="49"/>
-      <c r="G66" s="49"/>
-      <c r="H66" s="49"/>
-      <c r="I66" s="50"/>
-    </row>
-    <row r="67" spans="1:9" s="51" customFormat="1" ht="72" x14ac:dyDescent="0.45">
-      <c r="A67" s="64"/>
-      <c r="B67" s="82" t="s">
+      <c r="C67" s="112"/>
+      <c r="D67" s="98"/>
+      <c r="E67" s="48"/>
+      <c r="F67" s="48"/>
+      <c r="G67" s="48"/>
+      <c r="H67" s="48"/>
+      <c r="I67" s="49"/>
+    </row>
+    <row r="68" spans="1:9" s="50" customFormat="1" ht="72" x14ac:dyDescent="0.45">
+      <c r="A68" s="63"/>
+      <c r="B68" s="81" t="s">
         <v>94</v>
       </c>
-      <c r="C67" s="113" t="s">
+      <c r="C68" s="112" t="s">
         <v>151</v>
       </c>
-      <c r="D67" s="99"/>
-      <c r="E67" s="49"/>
-      <c r="F67" s="49"/>
-      <c r="G67" s="49"/>
-      <c r="H67" s="49"/>
-      <c r="I67" s="50"/>
-    </row>
-    <row r="68" spans="1:9" s="51" customFormat="1" ht="24" x14ac:dyDescent="0.45">
-      <c r="A68" s="64"/>
-      <c r="B68" s="82" t="s">
+      <c r="D68" s="98"/>
+      <c r="E68" s="48"/>
+      <c r="F68" s="48"/>
+      <c r="G68" s="48"/>
+      <c r="H68" s="48"/>
+      <c r="I68" s="49"/>
+    </row>
+    <row r="69" spans="1:9" s="50" customFormat="1" ht="24" x14ac:dyDescent="0.45">
+      <c r="A69" s="63"/>
+      <c r="B69" s="81" t="s">
         <v>95</v>
       </c>
-      <c r="C68" s="113" t="s">
+      <c r="C69" s="112" t="s">
         <v>162</v>
       </c>
-      <c r="D68" s="99"/>
-      <c r="E68" s="49"/>
-      <c r="F68" s="49"/>
-      <c r="G68" s="49"/>
-      <c r="H68" s="49"/>
-      <c r="I68" s="50"/>
+      <c r="D69" s="98"/>
+      <c r="E69" s="48"/>
+      <c r="F69" s="48"/>
+      <c r="G69" s="48"/>
+      <c r="H69" s="48"/>
+      <c r="I69" s="49"/>
     </row>
   </sheetData>
   <sheetProtection deleteColumns="0" selectLockedCells="1"/>
@@ -2721,7 +2766,7 @@
           <x14:formula1>
             <xm:f>'Drop Down List Values'!$M$2:$M$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D68:H68</xm:sqref>
+          <xm:sqref>D69:H69</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{33A578CF-33CA-4B41-B2C5-7541E5042FC9}">
           <x14:formula1>
@@ -3009,20 +3054,65 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="b541edd5-2552-480e-ada6-0e2c8d317108">YVWEJ5DVYS2U-421999773-68</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="b541edd5-2552-480e-ada6-0e2c8d317108">
-      <Url>https://cdcpartners.sharepoint.com/sites/NCHS/nvssmodcop/_layouts/15/DocIdRedir.aspx?ID=YVWEJ5DVYS2U-421999773-68</Url>
-      <Description>YVWEJ5DVYS2U-421999773-68</Description>
-    </_dlc_DocIdUrl>
-    <ShareFileCreator xmlns="780ae317-08c5-4e10-af93-dd385a8384a9" xsi:nil="true"/>
-    <ShareFileCreated xmlns="780ae317-08c5-4e10-af93-dd385a8384a9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D4902BA52C7D94A994657A564808B2B" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e4455a60d2ff5f5fcd8815d6d89b5b66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b541edd5-2552-480e-ada6-0e2c8d317108" xmlns:ns3="780ae317-08c5-4e10-af93-dd385a8384a9" xmlns:ns4="3146657c-56f4-4c0a-bb9c-a675121ac670" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d1d01ecd782f081d5d944fa263943fc4" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="b541edd5-2552-480e-ada6-0e2c8d317108"/>
@@ -3221,84 +3311,37 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="b541edd5-2552-480e-ada6-0e2c8d317108">YVWEJ5DVYS2U-421999773-68</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="b541edd5-2552-480e-ada6-0e2c8d317108">
+      <Url>https://cdcpartners.sharepoint.com/sites/NCHS/nvssmodcop/_layouts/15/DocIdRedir.aspx?ID=YVWEJ5DVYS2U-421999773-68</Url>
+      <Description>YVWEJ5DVYS2U-421999773-68</Description>
+    </_dlc_DocIdUrl>
+    <ShareFileCreator xmlns="780ae317-08c5-4e10-af93-dd385a8384a9" xsi:nil="true"/>
+    <ShareFileCreated xmlns="780ae317-08c5-4e10-af93-dd385a8384a9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69E3EF86-6C9E-4C22-A476-13DA012C68C5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{448710E8-BE9E-4C9E-A40A-0AC1DAE48E99}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="780ae317-08c5-4e10-af93-dd385a8384a9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="3146657c-56f4-4c0a-bb9c-a675121ac670"/>
-    <ds:schemaRef ds:uri="b541edd5-2552-480e-ada6-0e2c8d317108"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF0D7A6D-D78F-4048-9348-0B4289842B11}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0980278E-2A79-4F44-8623-FE545C304BE1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3318,18 +3361,20 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF0D7A6D-D78F-4048-9348-0B4289842B11}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69E3EF86-6C9E-4C22-A476-13DA012C68C5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{448710E8-BE9E-4C9E-A40A-0AC1DAE48E99}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b541edd5-2552-480e-ada6-0e2c8d317108"/>
+    <ds:schemaRef ds:uri="3146657c-56f4-4c0a-bb9c-a675121ac670"/>
+    <ds:schemaRef ds:uri="780ae317-08c5-4e10-af93-dd385a8384a9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Pushed MDI-To-EDRS-Template to correct main branch
</commit_message>
<xml_diff>
--- a/MDI-To-EDRS-Template.xlsx
+++ b/MDI-To-EDRS-Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20396"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20403"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mriley7\workspace\raven-import-and-submit-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA7019D1-ED79-4310-9BF2-27319FFB7C4A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F43D857-94EB-472C-B98C-8C7156000CAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8484" xr2:uid="{7A50F290-1C75-487E-9806-F93553E4E7CC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8490" xr2:uid="{7A50F290-1C75-487E-9806-F93553E4E7CC}"/>
   </bookViews>
   <sheets>
     <sheet name="MDI RAVEN Input Schema" sheetId="4" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="182">
   <si>
     <t>Manner of Death</t>
   </si>
@@ -659,6 +659,30 @@
   </si>
   <si>
     <t>Death Certifier</t>
+  </si>
+  <si>
+    <t>Autopsy Performed Location: Street</t>
+  </si>
+  <si>
+    <t>Autopsy Performed Location: City</t>
+  </si>
+  <si>
+    <t>Autopsy Performed Location: County</t>
+  </si>
+  <si>
+    <t>Primary Address of the autopsy location. Multiple lines are supported.</t>
+  </si>
+  <si>
+    <t>Autopsy Performed Location: State, U.S. Territory or Canadian Province</t>
+  </si>
+  <si>
+    <t>Autopsy Performed Location: Postal Code</t>
+  </si>
+  <si>
+    <t>Autopsy Performed Office Name</t>
+  </si>
+  <si>
+    <t>Name of the office in which the autopsy took place</t>
   </si>
 </sst>
 </file>
@@ -953,7 +977,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -1112,10 +1136,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -1678,30 +1698,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54CD1DC7-E143-4CF5-BEA9-4DABBAFFC7B0}">
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="22.5" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" style="53" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" style="65" customWidth="1"/>
-    <col min="3" max="3" width="38.44140625" style="73" customWidth="1"/>
-    <col min="4" max="8" width="32.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="27.28515625" style="52" customWidth="1"/>
+    <col min="2" max="2" width="64.42578125" style="64" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" style="72" customWidth="1"/>
+    <col min="4" max="8" width="32.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A1" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="64" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="73" t="s">
+      <c r="C1" s="72" t="s">
         <v>27</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -1723,28 +1743,28 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="23.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C2" s="73" t="s">
+    <row r="2" spans="1:9" ht="36.75" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C2" s="72" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="109.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="53" t="s">
+    <row r="3" spans="1:9" ht="120" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="52" t="s">
         <v>169</v>
       </c>
-      <c r="B3" s="121" t="s">
+      <c r="B3" s="120" t="s">
         <v>171</v>
       </c>
-      <c r="C3" s="122" t="s">
+      <c r="C3" s="121" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="4" customFormat="1" ht="34.799999999999997" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="54" t="s">
+    <row r="4" spans="1:9" s="4" customFormat="1" ht="36.75" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="100" t="s">
+      <c r="B4" s="65"/>
+      <c r="C4" s="99" t="s">
         <v>101</v>
       </c>
       <c r="D4" s="3"/>
@@ -1754,42 +1774,42 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" s="6" customFormat="1" ht="29.4" x14ac:dyDescent="0.5">
-      <c r="A5" s="55"/>
-      <c r="B5" s="118" t="s">
+    <row r="5" spans="1:9" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.45">
+      <c r="A5" s="54"/>
+      <c r="B5" s="117" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="101" t="s">
+      <c r="C5" s="100" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="1:9" s="6" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A6" s="55"/>
-      <c r="B6" s="119" t="s">
+    <row r="6" spans="1:9" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.45">
+      <c r="A6" s="54"/>
+      <c r="B6" s="118" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="101" t="s">
+      <c r="C6" s="100" t="s">
         <v>103</v>
       </c>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="1:9" s="8" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A7" s="56" t="s">
+    <row r="7" spans="1:9" s="8" customFormat="1" ht="36" x14ac:dyDescent="0.45">
+      <c r="A7" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="67"/>
-      <c r="C7" s="102" t="s">
+      <c r="B7" s="66"/>
+      <c r="C7" s="101" t="s">
         <v>105</v>
       </c>
       <c r="D7" s="7"/>
@@ -1799,12 +1819,12 @@
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:9" s="11" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
-      <c r="A8" s="57"/>
-      <c r="B8" s="74" t="s">
+    <row r="8" spans="1:9" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.45">
+      <c r="A8" s="56"/>
+      <c r="B8" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="103" t="s">
+      <c r="C8" s="102" t="s">
         <v>104</v>
       </c>
       <c r="D8" s="14"/>
@@ -1814,12 +1834,12 @@
       <c r="H8" s="9"/>
       <c r="I8" s="10"/>
     </row>
-    <row r="9" spans="1:9" s="11" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A9" s="57"/>
-      <c r="B9" s="74" t="s">
+    <row r="9" spans="1:9" s="11" customFormat="1" ht="60" x14ac:dyDescent="0.45">
+      <c r="A9" s="56"/>
+      <c r="B9" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="103" t="s">
+      <c r="C9" s="102" t="s">
         <v>108</v>
       </c>
       <c r="D9" s="14"/>
@@ -1829,12 +1849,12 @@
       <c r="H9" s="9"/>
       <c r="I9" s="10"/>
     </row>
-    <row r="10" spans="1:9" s="11" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A10" s="57"/>
-      <c r="B10" s="74" t="s">
+    <row r="10" spans="1:9" s="11" customFormat="1" ht="24" x14ac:dyDescent="0.45">
+      <c r="A10" s="56"/>
+      <c r="B10" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="103" t="s">
+      <c r="C10" s="102" t="s">
         <v>107</v>
       </c>
       <c r="D10" s="14"/>
@@ -1844,12 +1864,12 @@
       <c r="H10" s="9"/>
       <c r="I10" s="10"/>
     </row>
-    <row r="11" spans="1:9" s="11" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A11" s="57"/>
-      <c r="B11" s="75" t="s">
+    <row r="11" spans="1:9" s="11" customFormat="1" ht="36" x14ac:dyDescent="0.45">
+      <c r="A11" s="56"/>
+      <c r="B11" s="74" t="s">
         <v>76</v>
       </c>
-      <c r="C11" s="103" t="s">
+      <c r="C11" s="102" t="s">
         <v>106</v>
       </c>
       <c r="D11" s="14"/>
@@ -1859,12 +1879,12 @@
       <c r="H11" s="9"/>
       <c r="I11" s="10"/>
     </row>
-    <row r="12" spans="1:9" s="11" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A12" s="57"/>
-      <c r="B12" s="74" t="s">
+    <row r="12" spans="1:9" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.45">
+      <c r="A12" s="56"/>
+      <c r="B12" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="103" t="s">
+      <c r="C12" s="102" t="s">
         <v>155</v>
       </c>
       <c r="D12" s="14"/>
@@ -1874,12 +1894,12 @@
       <c r="H12" s="9"/>
       <c r="I12" s="10"/>
     </row>
-    <row r="13" spans="1:9" s="11" customFormat="1" ht="57" x14ac:dyDescent="0.5">
-      <c r="A13" s="57"/>
-      <c r="B13" s="74" t="s">
+    <row r="13" spans="1:9" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.45">
+      <c r="A13" s="56"/>
+      <c r="B13" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="103" t="s">
+      <c r="C13" s="102" t="s">
         <v>109</v>
       </c>
       <c r="D13" s="14"/>
@@ -1889,27 +1909,27 @@
       <c r="H13" s="9"/>
       <c r="I13" s="10"/>
     </row>
-    <row r="14" spans="1:9" s="11" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A14" s="57"/>
-      <c r="B14" s="74" t="s">
+    <row r="14" spans="1:9" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.45">
+      <c r="A14" s="56"/>
+      <c r="B14" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="103" t="s">
+      <c r="C14" s="102" t="s">
         <v>110</v>
       </c>
-      <c r="D14" s="85"/>
+      <c r="D14" s="84"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
       <c r="I14" s="10"/>
     </row>
-    <row r="15" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="57"/>
-      <c r="B15" s="74" t="s">
+    <row r="15" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="56"/>
+      <c r="B15" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="103"/>
+      <c r="C15" s="102"/>
       <c r="D15" s="14"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
@@ -1917,27 +1937,27 @@
       <c r="H15" s="9"/>
       <c r="I15" s="10"/>
     </row>
-    <row r="16" spans="1:9" s="11" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A16" s="57"/>
-      <c r="B16" s="74" t="s">
+    <row r="16" spans="1:9" s="11" customFormat="1" ht="24" x14ac:dyDescent="0.45">
+      <c r="A16" s="56"/>
+      <c r="B16" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="103" t="s">
+      <c r="C16" s="102" t="s">
         <v>111</v>
       </c>
-      <c r="D16" s="86"/>
+      <c r="D16" s="85"/>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
       <c r="H16" s="9"/>
       <c r="I16" s="10"/>
     </row>
-    <row r="17" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="57"/>
-      <c r="B17" s="74" t="s">
+    <row r="17" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="56"/>
+      <c r="B17" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="103"/>
+      <c r="C17" s="102"/>
       <c r="D17" s="14"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
@@ -1945,12 +1965,12 @@
       <c r="H17" s="9"/>
       <c r="I17" s="10"/>
     </row>
-    <row r="18" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="57"/>
-      <c r="B18" s="74" t="s">
+    <row r="18" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="56"/>
+      <c r="B18" s="73" t="s">
         <v>99</v>
       </c>
-      <c r="C18" s="103"/>
+      <c r="C18" s="102"/>
       <c r="D18" s="14"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
@@ -1958,12 +1978,12 @@
       <c r="H18" s="9"/>
       <c r="I18" s="10"/>
     </row>
-    <row r="19" spans="1:9" s="11" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
-      <c r="A19" s="57"/>
-      <c r="B19" s="76" t="s">
+    <row r="19" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A19" s="56"/>
+      <c r="B19" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="103"/>
+      <c r="C19" s="102"/>
       <c r="D19" s="14"/>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
@@ -1971,12 +1991,12 @@
       <c r="H19" s="9"/>
       <c r="I19" s="10"/>
     </row>
-    <row r="20" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="57"/>
-      <c r="B20" s="74" t="s">
+    <row r="20" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="56"/>
+      <c r="B20" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="103"/>
+      <c r="C20" s="102"/>
       <c r="D20" s="14"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
@@ -1984,12 +2004,12 @@
       <c r="H20" s="9"/>
       <c r="I20" s="10"/>
     </row>
-    <row r="21" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="57"/>
-      <c r="B21" s="74" t="s">
+    <row r="21" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="56"/>
+      <c r="B21" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="103"/>
+      <c r="C21" s="102"/>
       <c r="D21" s="14"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
@@ -1997,12 +2017,12 @@
       <c r="H21" s="9"/>
       <c r="I21" s="10"/>
     </row>
-    <row r="22" spans="1:9" s="16" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
-      <c r="A22" s="114" t="s">
+    <row r="22" spans="1:9" s="16" customFormat="1" ht="84" x14ac:dyDescent="0.45">
+      <c r="A22" s="113" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="68"/>
-      <c r="C22" s="104" t="s">
+      <c r="B22" s="67"/>
+      <c r="C22" s="103" t="s">
         <v>112</v>
       </c>
       <c r="D22" s="15"/>
@@ -2012,237 +2032,237 @@
       <c r="H22" s="15"/>
       <c r="I22" s="15"/>
     </row>
-    <row r="23" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A23" s="58"/>
-      <c r="B23" s="120" t="s">
+    <row r="23" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="57"/>
+      <c r="B23" s="119" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="105" t="s">
+      <c r="C23" s="104" t="s">
         <v>113</v>
       </c>
-      <c r="D23" s="87"/>
+      <c r="D23" s="86"/>
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
       <c r="H23" s="17"/>
       <c r="I23" s="18"/>
     </row>
-    <row r="24" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A24" s="58"/>
-      <c r="B24" s="120" t="s">
+    <row r="24" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="57"/>
+      <c r="B24" s="119" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="105" t="s">
+      <c r="C24" s="104" t="s">
         <v>114</v>
       </c>
-      <c r="D24" s="88"/>
+      <c r="D24" s="87"/>
       <c r="E24" s="20"/>
       <c r="F24" s="20"/>
       <c r="G24" s="20"/>
       <c r="H24" s="20"/>
       <c r="I24" s="18"/>
     </row>
-    <row r="25" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A25" s="58"/>
-      <c r="B25" s="120" t="s">
+    <row r="25" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="57"/>
+      <c r="B25" s="119" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="105" t="s">
+      <c r="C25" s="104" t="s">
         <v>115</v>
       </c>
-      <c r="D25" s="89"/>
+      <c r="D25" s="88"/>
       <c r="E25" s="21"/>
       <c r="F25" s="21"/>
       <c r="G25" s="21"/>
       <c r="H25" s="21"/>
       <c r="I25" s="18"/>
     </row>
-    <row r="26" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A26" s="58"/>
-      <c r="B26" s="120" t="s">
+    <row r="26" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="57"/>
+      <c r="B26" s="119" t="s">
         <v>98</v>
       </c>
-      <c r="C26" s="105" t="s">
+      <c r="C26" s="104" t="s">
         <v>116</v>
       </c>
-      <c r="D26" s="89"/>
+      <c r="D26" s="88"/>
       <c r="E26" s="21"/>
       <c r="F26" s="21"/>
       <c r="G26" s="21"/>
       <c r="H26" s="21"/>
       <c r="I26" s="18"/>
     </row>
-    <row r="27" spans="1:9" s="19" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A27" s="58"/>
-      <c r="B27" s="120" t="s">
+    <row r="27" spans="1:9" s="19" customFormat="1" ht="48" x14ac:dyDescent="0.45">
+      <c r="A27" s="57"/>
+      <c r="B27" s="119" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="105" t="s">
+      <c r="C27" s="104" t="s">
         <v>117</v>
       </c>
-      <c r="D27" s="89"/>
+      <c r="D27" s="88"/>
       <c r="E27" s="21"/>
       <c r="F27" s="21"/>
       <c r="G27" s="21"/>
       <c r="H27" s="21"/>
       <c r="I27" s="18"/>
     </row>
-    <row r="28" spans="1:9" s="19" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A28" s="58"/>
-      <c r="B28" s="120" t="s">
+    <row r="28" spans="1:9" s="19" customFormat="1" ht="48" x14ac:dyDescent="0.45">
+      <c r="A28" s="57"/>
+      <c r="B28" s="119" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="105" t="s">
+      <c r="C28" s="104" t="s">
         <v>118</v>
       </c>
-      <c r="D28" s="89"/>
+      <c r="D28" s="88"/>
       <c r="E28" s="21"/>
       <c r="F28" s="21"/>
       <c r="G28" s="21"/>
       <c r="H28" s="21"/>
       <c r="I28" s="18"/>
     </row>
-    <row r="29" spans="1:9" s="19" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A29" s="58"/>
-      <c r="B29" s="120" t="s">
+    <row r="29" spans="1:9" s="19" customFormat="1" ht="48" x14ac:dyDescent="0.45">
+      <c r="A29" s="57"/>
+      <c r="B29" s="119" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="105" t="s">
+      <c r="C29" s="104" t="s">
         <v>119</v>
       </c>
-      <c r="D29" s="89"/>
+      <c r="D29" s="88"/>
       <c r="E29" s="21"/>
       <c r="F29" s="21"/>
       <c r="G29" s="21"/>
       <c r="H29" s="21"/>
       <c r="I29" s="18"/>
     </row>
-    <row r="30" spans="1:9" s="19" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A30" s="58"/>
-      <c r="B30" s="120" t="s">
+    <row r="30" spans="1:9" s="19" customFormat="1" ht="48" x14ac:dyDescent="0.45">
+      <c r="A30" s="57"/>
+      <c r="B30" s="119" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="105" t="s">
+      <c r="C30" s="104" t="s">
         <v>120</v>
       </c>
-      <c r="D30" s="87"/>
+      <c r="D30" s="86"/>
       <c r="E30" s="17"/>
       <c r="F30" s="17"/>
       <c r="G30" s="17"/>
       <c r="H30" s="17"/>
       <c r="I30" s="18"/>
     </row>
-    <row r="31" spans="1:9" s="19" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A31" s="58"/>
-      <c r="B31" s="120" t="s">
+    <row r="31" spans="1:9" s="19" customFormat="1" ht="48" x14ac:dyDescent="0.45">
+      <c r="A31" s="57"/>
+      <c r="B31" s="119" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="105" t="s">
+      <c r="C31" s="104" t="s">
         <v>121</v>
       </c>
-      <c r="D31" s="90"/>
+      <c r="D31" s="89"/>
       <c r="E31" s="22"/>
       <c r="F31" s="22"/>
       <c r="G31" s="22"/>
       <c r="H31" s="22"/>
       <c r="I31" s="18"/>
     </row>
-    <row r="32" spans="1:9" s="19" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A32" s="58"/>
-      <c r="B32" s="77" t="s">
+    <row r="32" spans="1:9" s="19" customFormat="1" ht="24" x14ac:dyDescent="0.45">
+      <c r="A32" s="57"/>
+      <c r="B32" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="105" t="s">
+      <c r="C32" s="104" t="s">
         <v>122</v>
       </c>
-      <c r="D32" s="90"/>
+      <c r="D32" s="89"/>
       <c r="E32" s="22"/>
       <c r="F32" s="22"/>
       <c r="G32" s="22"/>
       <c r="H32" s="22"/>
       <c r="I32" s="18"/>
     </row>
-    <row r="33" spans="1:9" s="19" customFormat="1" ht="57" x14ac:dyDescent="0.5">
-      <c r="A33" s="58"/>
-      <c r="B33" s="77" t="s">
+    <row r="33" spans="1:9" s="19" customFormat="1" ht="60" x14ac:dyDescent="0.45">
+      <c r="A33" s="57"/>
+      <c r="B33" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="105" t="s">
+      <c r="C33" s="104" t="s">
         <v>123</v>
       </c>
-      <c r="D33" s="91"/>
+      <c r="D33" s="90"/>
       <c r="E33" s="23"/>
       <c r="F33" s="23"/>
       <c r="G33" s="23"/>
       <c r="H33" s="23"/>
       <c r="I33" s="18"/>
     </row>
-    <row r="34" spans="1:9" s="19" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
-      <c r="A34" s="58"/>
-      <c r="B34" s="77" t="s">
+    <row r="34" spans="1:9" s="19" customFormat="1" ht="84" x14ac:dyDescent="0.45">
+      <c r="A34" s="57"/>
+      <c r="B34" s="76" t="s">
         <v>83</v>
       </c>
-      <c r="C34" s="105" t="s">
+      <c r="C34" s="104" t="s">
         <v>124</v>
       </c>
-      <c r="D34" s="90"/>
+      <c r="D34" s="89"/>
       <c r="E34" s="22"/>
       <c r="F34" s="24"/>
       <c r="G34" s="22"/>
       <c r="H34" s="24"/>
       <c r="I34" s="18"/>
     </row>
-    <row r="35" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A35" s="59"/>
-      <c r="B35" s="77" t="s">
+    <row r="35" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="58"/>
+      <c r="B35" s="76" t="s">
         <v>82</v>
       </c>
-      <c r="C35" s="105" t="s">
+      <c r="C35" s="104" t="s">
         <v>125</v>
       </c>
-      <c r="D35" s="89"/>
+      <c r="D35" s="88"/>
       <c r="E35" s="21"/>
       <c r="F35" s="21"/>
       <c r="G35" s="21"/>
       <c r="H35" s="21"/>
       <c r="I35" s="25"/>
     </row>
-    <row r="36" spans="1:9" s="19" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A36" s="58"/>
-      <c r="B36" s="77" t="s">
+    <row r="36" spans="1:9" s="19" customFormat="1" ht="36" x14ac:dyDescent="0.45">
+      <c r="A36" s="57"/>
+      <c r="B36" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="C36" s="105" t="s">
+      <c r="C36" s="104" t="s">
         <v>126</v>
       </c>
-      <c r="D36" s="90"/>
+      <c r="D36" s="89"/>
       <c r="E36" s="22"/>
       <c r="F36" s="22"/>
       <c r="G36" s="22"/>
       <c r="H36" s="22"/>
       <c r="I36" s="18"/>
     </row>
-    <row r="37" spans="1:9" s="19" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A37" s="58"/>
-      <c r="B37" s="77" t="s">
+    <row r="37" spans="1:9" s="19" customFormat="1" ht="36" x14ac:dyDescent="0.45">
+      <c r="A37" s="57"/>
+      <c r="B37" s="76" t="s">
         <v>43</v>
       </c>
-      <c r="C37" s="105" t="s">
+      <c r="C37" s="104" t="s">
         <v>127</v>
       </c>
-      <c r="D37" s="90"/>
+      <c r="D37" s="89"/>
       <c r="E37" s="22"/>
       <c r="F37" s="22"/>
       <c r="G37" s="22"/>
       <c r="H37" s="22"/>
       <c r="I37" s="18"/>
     </row>
-    <row r="38" spans="1:9" s="28" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
-      <c r="A38" s="115" t="s">
+    <row r="38" spans="1:9" s="28" customFormat="1" ht="84" x14ac:dyDescent="0.45">
+      <c r="A38" s="114" t="s">
         <v>30</v>
       </c>
-      <c r="B38" s="69"/>
-      <c r="C38" s="106" t="s">
+      <c r="B38" s="68"/>
+      <c r="C38" s="105" t="s">
         <v>143</v>
       </c>
       <c r="D38" s="27"/>
@@ -2252,177 +2272,177 @@
       <c r="H38" s="27"/>
       <c r="I38" s="27"/>
     </row>
-    <row r="39" spans="1:9" s="31" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A39" s="60"/>
-      <c r="B39" s="78" t="s">
+    <row r="39" spans="1:9" s="31" customFormat="1" ht="24" x14ac:dyDescent="0.45">
+      <c r="A39" s="59"/>
+      <c r="B39" s="77" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="107" t="s">
+      <c r="C39" s="106" t="s">
         <v>128</v>
       </c>
-      <c r="D39" s="92"/>
+      <c r="D39" s="91"/>
       <c r="E39" s="29"/>
       <c r="F39" s="29"/>
       <c r="G39" s="29"/>
       <c r="H39" s="29"/>
       <c r="I39" s="30"/>
     </row>
-    <row r="40" spans="1:9" s="31" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A40" s="60"/>
-      <c r="B40" s="79" t="s">
+    <row r="40" spans="1:9" s="31" customFormat="1" ht="24" x14ac:dyDescent="0.45">
+      <c r="A40" s="59"/>
+      <c r="B40" s="78" t="s">
         <v>96</v>
       </c>
-      <c r="C40" s="107" t="s">
+      <c r="C40" s="106" t="s">
         <v>166</v>
       </c>
-      <c r="D40" s="92"/>
+      <c r="D40" s="91"/>
       <c r="E40" s="29"/>
       <c r="F40" s="32"/>
       <c r="G40" s="29"/>
       <c r="H40" s="32"/>
       <c r="I40" s="30"/>
     </row>
-    <row r="41" spans="1:9" s="31" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A41" s="60"/>
-      <c r="B41" s="78" t="s">
+    <row r="41" spans="1:9" s="31" customFormat="1" ht="36" x14ac:dyDescent="0.45">
+      <c r="A41" s="59"/>
+      <c r="B41" s="77" t="s">
         <v>77</v>
       </c>
-      <c r="C41" s="107" t="s">
+      <c r="C41" s="106" t="s">
         <v>129</v>
       </c>
-      <c r="D41" s="92"/>
-      <c r="E41" s="92"/>
-      <c r="F41" s="92"/>
-      <c r="G41" s="92"/>
-      <c r="H41" s="92"/>
+      <c r="D41" s="91"/>
+      <c r="E41" s="91"/>
+      <c r="F41" s="91"/>
+      <c r="G41" s="91"/>
+      <c r="H41" s="91"/>
       <c r="I41" s="30"/>
     </row>
-    <row r="42" spans="1:9" s="31" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A42" s="60"/>
-      <c r="B42" s="117" t="s">
+    <row r="42" spans="1:9" s="31" customFormat="1" ht="36" x14ac:dyDescent="0.45">
+      <c r="A42" s="59"/>
+      <c r="B42" s="116" t="s">
         <v>1</v>
       </c>
-      <c r="C42" s="107" t="s">
+      <c r="C42" s="106" t="s">
         <v>130</v>
       </c>
-      <c r="D42" s="92"/>
+      <c r="D42" s="91"/>
       <c r="E42" s="29"/>
       <c r="F42" s="29"/>
       <c r="G42" s="29"/>
       <c r="H42" s="29"/>
       <c r="I42" s="30"/>
     </row>
-    <row r="43" spans="1:9" s="35" customFormat="1" ht="57" x14ac:dyDescent="0.5">
-      <c r="A43" s="123" t="s">
+    <row r="43" spans="1:9" s="35" customFormat="1" ht="60" x14ac:dyDescent="0.45">
+      <c r="A43" s="122" t="s">
         <v>172</v>
       </c>
-      <c r="B43" s="70"/>
-      <c r="C43" s="108" t="s">
+      <c r="B43" s="69"/>
+      <c r="C43" s="107" t="s">
         <v>144</v>
       </c>
-      <c r="D43" s="93"/>
+      <c r="D43" s="92"/>
       <c r="E43" s="33"/>
       <c r="F43" s="33"/>
       <c r="G43" s="33"/>
       <c r="H43" s="33"/>
       <c r="I43" s="34"/>
     </row>
-    <row r="44" spans="1:9" s="38" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A44" s="61"/>
-      <c r="B44" s="80" t="s">
+    <row r="44" spans="1:9" s="38" customFormat="1" ht="48" x14ac:dyDescent="0.45">
+      <c r="A44" s="60"/>
+      <c r="B44" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="C44" s="109" t="s">
+      <c r="C44" s="108" t="s">
         <v>131</v>
       </c>
-      <c r="D44" s="94"/>
+      <c r="D44" s="93"/>
       <c r="E44" s="36"/>
       <c r="F44" s="36"/>
       <c r="G44" s="36"/>
       <c r="H44" s="36"/>
       <c r="I44" s="37"/>
     </row>
-    <row r="45" spans="1:9" s="38" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
-      <c r="A45" s="61"/>
-      <c r="B45" s="80" t="s">
+    <row r="45" spans="1:9" s="38" customFormat="1" ht="84" x14ac:dyDescent="0.45">
+      <c r="A45" s="60"/>
+      <c r="B45" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="C45" s="109" t="s">
+      <c r="C45" s="108" t="s">
         <v>132</v>
       </c>
-      <c r="D45" s="95"/>
+      <c r="D45" s="94"/>
       <c r="E45" s="39"/>
       <c r="F45" s="39"/>
       <c r="G45" s="39"/>
       <c r="H45" s="39"/>
       <c r="I45" s="37"/>
     </row>
-    <row r="46" spans="1:9" s="38" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A46" s="61"/>
-      <c r="B46" s="80" t="s">
+    <row r="46" spans="1:9" s="38" customFormat="1" ht="36" x14ac:dyDescent="0.45">
+      <c r="A46" s="60"/>
+      <c r="B46" s="79" t="s">
         <v>78</v>
       </c>
-      <c r="C46" s="109" t="s">
+      <c r="C46" s="108" t="s">
         <v>137</v>
       </c>
-      <c r="D46" s="96"/>
+      <c r="D46" s="95"/>
       <c r="E46" s="40"/>
       <c r="F46" s="40"/>
       <c r="G46" s="40"/>
       <c r="H46" s="40"/>
       <c r="I46" s="37"/>
     </row>
-    <row r="47" spans="1:9" s="38" customFormat="1" ht="57" x14ac:dyDescent="0.5">
-      <c r="A47" s="61"/>
-      <c r="B47" s="80" t="s">
+    <row r="47" spans="1:9" s="38" customFormat="1" ht="60" x14ac:dyDescent="0.45">
+      <c r="A47" s="60"/>
+      <c r="B47" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="C47" s="109" t="s">
+      <c r="C47" s="108" t="s">
         <v>138</v>
       </c>
-      <c r="D47" s="97"/>
+      <c r="D47" s="96"/>
       <c r="E47" s="41"/>
       <c r="F47" s="41"/>
       <c r="G47" s="41"/>
       <c r="H47" s="41"/>
       <c r="I47" s="37"/>
     </row>
-    <row r="48" spans="1:9" s="38" customFormat="1" ht="91.2" x14ac:dyDescent="0.5">
-      <c r="A48" s="61"/>
-      <c r="B48" s="80" t="s">
+    <row r="48" spans="1:9" s="38" customFormat="1" ht="96" x14ac:dyDescent="0.45">
+      <c r="A48" s="60"/>
+      <c r="B48" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="C48" s="109" t="s">
+      <c r="C48" s="108" t="s">
         <v>139</v>
       </c>
-      <c r="D48" s="95"/>
+      <c r="D48" s="94"/>
       <c r="E48" s="39"/>
       <c r="F48" s="39"/>
       <c r="G48" s="39"/>
       <c r="H48" s="39"/>
       <c r="I48" s="37"/>
     </row>
-    <row r="49" spans="1:9" s="38" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A49" s="61"/>
-      <c r="B49" s="80" t="s">
+    <row r="49" spans="1:9" s="38" customFormat="1" ht="36" x14ac:dyDescent="0.45">
+      <c r="A49" s="60"/>
+      <c r="B49" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="C49" s="109" t="s">
+      <c r="C49" s="108" t="s">
         <v>140</v>
       </c>
-      <c r="D49" s="96"/>
+      <c r="D49" s="95"/>
       <c r="E49" s="40"/>
       <c r="F49" s="40"/>
       <c r="G49" s="40"/>
       <c r="H49" s="40"/>
       <c r="I49" s="37"/>
     </row>
-    <row r="50" spans="1:9" s="43" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A50" s="62" t="s">
+    <row r="50" spans="1:9" s="43" customFormat="1" ht="24" x14ac:dyDescent="0.45">
+      <c r="A50" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="B50" s="71"/>
-      <c r="C50" s="110" t="s">
+      <c r="B50" s="70"/>
+      <c r="C50" s="109" t="s">
         <v>145</v>
       </c>
       <c r="D50" s="42"/>
@@ -2432,192 +2452,260 @@
       <c r="H50" s="42"/>
       <c r="I50" s="42"/>
     </row>
-    <row r="51" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A51" s="63"/>
-      <c r="B51" s="81" t="s">
+    <row r="51" spans="1:9" s="45" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A51" s="62"/>
+      <c r="B51" s="80" t="s">
         <v>45</v>
       </c>
-      <c r="C51" s="111" t="s">
+      <c r="C51" s="110" t="s">
         <v>141</v>
       </c>
-      <c r="D51" s="98"/>
-      <c r="E51" s="44"/>
-      <c r="F51" s="44"/>
-      <c r="G51" s="44"/>
-      <c r="H51" s="44"/>
-      <c r="I51" s="45"/>
-    </row>
-    <row r="52" spans="1:9" s="46" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A52" s="63"/>
-      <c r="B52" s="81" t="s">
+      <c r="D51" s="97"/>
+      <c r="E51" s="97"/>
+      <c r="F51" s="97"/>
+      <c r="G51" s="97"/>
+      <c r="H51" s="97"/>
+      <c r="I51" s="44"/>
+    </row>
+    <row r="52" spans="1:9" s="62" customFormat="1" ht="36" x14ac:dyDescent="0.45">
+      <c r="B52" s="80" t="s">
         <v>81</v>
       </c>
-      <c r="C52" s="111" t="s">
+      <c r="C52" s="110" t="s">
         <v>142</v>
       </c>
-      <c r="D52" s="98"/>
-      <c r="E52" s="44"/>
-      <c r="F52" s="44"/>
-      <c r="G52" s="44"/>
-      <c r="H52" s="44"/>
-      <c r="I52" s="45"/>
-    </row>
-    <row r="53" spans="1:9" s="48" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A53" s="116" t="s">
+      <c r="D52" s="97"/>
+      <c r="E52" s="97"/>
+      <c r="F52" s="97"/>
+      <c r="G52" s="97"/>
+      <c r="H52" s="97"/>
+    </row>
+    <row r="53" spans="1:9" s="62" customFormat="1" ht="24" x14ac:dyDescent="0.45">
+      <c r="B53" s="80" t="s">
+        <v>180</v>
+      </c>
+      <c r="C53" s="110" t="s">
+        <v>181</v>
+      </c>
+      <c r="D53" s="97"/>
+      <c r="E53" s="97"/>
+      <c r="F53" s="97"/>
+      <c r="G53" s="97"/>
+      <c r="H53" s="97"/>
+    </row>
+    <row r="54" spans="1:9" s="62" customFormat="1" ht="24" x14ac:dyDescent="0.45">
+      <c r="B54" s="80" t="s">
+        <v>174</v>
+      </c>
+      <c r="C54" s="110" t="s">
+        <v>177</v>
+      </c>
+      <c r="D54" s="97"/>
+      <c r="E54" s="97"/>
+      <c r="F54" s="97"/>
+      <c r="G54" s="97"/>
+      <c r="H54" s="97"/>
+    </row>
+    <row r="55" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B55" s="80" t="s">
+        <v>175</v>
+      </c>
+      <c r="C55" s="110"/>
+      <c r="D55" s="97"/>
+      <c r="E55" s="97"/>
+      <c r="F55" s="97"/>
+      <c r="G55" s="97"/>
+      <c r="H55" s="97"/>
+    </row>
+    <row r="56" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B56" s="80" t="s">
+        <v>176</v>
+      </c>
+      <c r="C56" s="110"/>
+      <c r="D56" s="97"/>
+      <c r="E56" s="97"/>
+      <c r="F56" s="97"/>
+      <c r="G56" s="97"/>
+      <c r="H56" s="97"/>
+    </row>
+    <row r="57" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B57" s="80" t="s">
+        <v>178</v>
+      </c>
+      <c r="C57" s="110"/>
+      <c r="D57" s="97"/>
+      <c r="E57" s="97"/>
+      <c r="F57" s="97"/>
+      <c r="G57" s="97"/>
+      <c r="H57" s="97"/>
+    </row>
+    <row r="58" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B58" s="80" t="s">
+        <v>179</v>
+      </c>
+      <c r="C58" s="110"/>
+      <c r="D58" s="97"/>
+      <c r="E58" s="97"/>
+      <c r="F58" s="97"/>
+      <c r="G58" s="97"/>
+      <c r="H58" s="97"/>
+    </row>
+    <row r="59" spans="1:9" s="47" customFormat="1" ht="36" x14ac:dyDescent="0.45">
+      <c r="A59" s="115" t="s">
         <v>173</v>
       </c>
-      <c r="B53" s="72"/>
-      <c r="C53" s="112" t="s">
+      <c r="B59" s="71"/>
+      <c r="C59" s="111" t="s">
         <v>146</v>
       </c>
-      <c r="D53" s="47"/>
-      <c r="E53" s="47"/>
-      <c r="F53" s="47"/>
-      <c r="G53" s="47"/>
-      <c r="H53" s="47"/>
-      <c r="I53" s="47"/>
-    </row>
-    <row r="54" spans="1:9" s="51" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
-      <c r="A54" s="64"/>
-      <c r="B54" s="82" t="s">
+      <c r="D59" s="46"/>
+      <c r="E59" s="46"/>
+      <c r="F59" s="46"/>
+      <c r="G59" s="46"/>
+      <c r="H59" s="46"/>
+      <c r="I59" s="46"/>
+    </row>
+    <row r="60" spans="1:9" s="50" customFormat="1" ht="72" x14ac:dyDescent="0.45">
+      <c r="A60" s="63"/>
+      <c r="B60" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="C54" s="113" t="s">
+      <c r="C60" s="112" t="s">
         <v>147</v>
       </c>
-      <c r="D54" s="99"/>
-      <c r="E54" s="49"/>
-      <c r="F54" s="49"/>
-      <c r="G54" s="49"/>
-      <c r="H54" s="49"/>
-      <c r="I54" s="50"/>
-    </row>
-    <row r="55" spans="1:9" s="51" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A55" s="64"/>
-      <c r="B55" s="83" t="s">
+      <c r="D60" s="98"/>
+      <c r="E60" s="48"/>
+      <c r="F60" s="48"/>
+      <c r="G60" s="48"/>
+      <c r="H60" s="48"/>
+      <c r="I60" s="49"/>
+    </row>
+    <row r="61" spans="1:9" s="50" customFormat="1" ht="48" x14ac:dyDescent="0.45">
+      <c r="A61" s="63"/>
+      <c r="B61" s="82" t="s">
         <v>91</v>
       </c>
-      <c r="C55" s="113" t="s">
+      <c r="C61" s="112" t="s">
         <v>148</v>
       </c>
-      <c r="D55" s="99"/>
-      <c r="E55" s="49"/>
-      <c r="F55" s="49"/>
-      <c r="G55" s="49"/>
-      <c r="H55" s="49"/>
-      <c r="I55" s="50"/>
-    </row>
-    <row r="56" spans="1:9" s="51" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A56" s="64"/>
-      <c r="B56" s="82" t="s">
+      <c r="D61" s="98"/>
+      <c r="E61" s="48"/>
+      <c r="F61" s="48"/>
+      <c r="G61" s="48"/>
+      <c r="H61" s="48"/>
+      <c r="I61" s="49"/>
+    </row>
+    <row r="62" spans="1:9" s="50" customFormat="1" ht="36" x14ac:dyDescent="0.45">
+      <c r="A62" s="63"/>
+      <c r="B62" s="81" t="s">
         <v>92</v>
       </c>
-      <c r="C56" s="113" t="s">
+      <c r="C62" s="112" t="s">
         <v>149</v>
       </c>
-      <c r="D56" s="99"/>
-      <c r="E56" s="49"/>
-      <c r="F56" s="49"/>
-      <c r="G56" s="49"/>
-      <c r="H56" s="49"/>
-      <c r="I56" s="50"/>
-    </row>
-    <row r="57" spans="1:9" s="51" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A57" s="64"/>
-      <c r="B57" s="82" t="s">
+      <c r="D62" s="98"/>
+      <c r="E62" s="48"/>
+      <c r="F62" s="48"/>
+      <c r="G62" s="48"/>
+      <c r="H62" s="48"/>
+      <c r="I62" s="49"/>
+    </row>
+    <row r="63" spans="1:9" s="50" customFormat="1" ht="36" x14ac:dyDescent="0.45">
+      <c r="A63" s="63"/>
+      <c r="B63" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="C57" s="113" t="s">
+      <c r="C63" s="112" t="s">
         <v>150</v>
       </c>
-      <c r="D57" s="99"/>
-      <c r="E57" s="49"/>
-      <c r="F57" s="49"/>
-      <c r="G57" s="49"/>
-      <c r="H57" s="49"/>
-      <c r="I57" s="50"/>
-    </row>
-    <row r="58" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A58" s="64"/>
-      <c r="B58" s="82" t="s">
+      <c r="D63" s="98"/>
+      <c r="E63" s="48"/>
+      <c r="F63" s="48"/>
+      <c r="G63" s="48"/>
+      <c r="H63" s="48"/>
+      <c r="I63" s="49"/>
+    </row>
+    <row r="64" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A64" s="63"/>
+      <c r="B64" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="C58" s="113"/>
-      <c r="D58" s="99"/>
-      <c r="E58" s="49"/>
-      <c r="F58" s="49"/>
-      <c r="G58" s="49"/>
-      <c r="H58" s="49"/>
-      <c r="I58" s="50"/>
-    </row>
-    <row r="59" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A59" s="64"/>
-      <c r="B59" s="82" t="s">
+      <c r="C64" s="112"/>
+      <c r="D64" s="98"/>
+      <c r="E64" s="48"/>
+      <c r="F64" s="48"/>
+      <c r="G64" s="48"/>
+      <c r="H64" s="48"/>
+      <c r="I64" s="49"/>
+    </row>
+    <row r="65" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A65" s="63"/>
+      <c r="B65" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="C59" s="113"/>
-      <c r="D59" s="99"/>
-      <c r="E59" s="49"/>
-      <c r="F59" s="49"/>
-      <c r="G59" s="49"/>
-      <c r="H59" s="49"/>
-      <c r="I59" s="50"/>
-    </row>
-    <row r="60" spans="1:9" s="51" customFormat="1" ht="39.6" x14ac:dyDescent="0.5">
-      <c r="A60" s="64"/>
-      <c r="B60" s="84" t="s">
+      <c r="C65" s="112"/>
+      <c r="D65" s="98"/>
+      <c r="E65" s="48"/>
+      <c r="F65" s="48"/>
+      <c r="G65" s="48"/>
+      <c r="H65" s="48"/>
+      <c r="I65" s="49"/>
+    </row>
+    <row r="66" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A66" s="63"/>
+      <c r="B66" s="83" t="s">
         <v>36</v>
       </c>
-      <c r="C60" s="113"/>
-      <c r="D60" s="99"/>
-      <c r="E60" s="49"/>
-      <c r="F60" s="49"/>
-      <c r="G60" s="49"/>
-      <c r="H60" s="49"/>
-      <c r="I60" s="50"/>
-    </row>
-    <row r="61" spans="1:9" s="51" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
-      <c r="A61" s="64"/>
-      <c r="B61" s="84" t="s">
+      <c r="C66" s="112"/>
+      <c r="D66" s="98"/>
+      <c r="E66" s="48"/>
+      <c r="F66" s="48"/>
+      <c r="G66" s="48"/>
+      <c r="H66" s="48"/>
+      <c r="I66" s="49"/>
+    </row>
+    <row r="67" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A67" s="63"/>
+      <c r="B67" s="83" t="s">
         <v>37</v>
       </c>
-      <c r="C61" s="113"/>
-      <c r="D61" s="99"/>
-      <c r="E61" s="49"/>
-      <c r="F61" s="49"/>
-      <c r="G61" s="49"/>
-      <c r="H61" s="49"/>
-      <c r="I61" s="50"/>
-    </row>
-    <row r="62" spans="1:9" s="51" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
-      <c r="A62" s="64"/>
-      <c r="B62" s="82" t="s">
+      <c r="C67" s="112"/>
+      <c r="D67" s="98"/>
+      <c r="E67" s="48"/>
+      <c r="F67" s="48"/>
+      <c r="G67" s="48"/>
+      <c r="H67" s="48"/>
+      <c r="I67" s="49"/>
+    </row>
+    <row r="68" spans="1:9" s="50" customFormat="1" ht="72" x14ac:dyDescent="0.45">
+      <c r="A68" s="63"/>
+      <c r="B68" s="81" t="s">
         <v>94</v>
       </c>
-      <c r="C62" s="113" t="s">
+      <c r="C68" s="112" t="s">
         <v>151</v>
       </c>
-      <c r="D62" s="99"/>
-      <c r="E62" s="49"/>
-      <c r="F62" s="49"/>
-      <c r="G62" s="49"/>
-      <c r="H62" s="49"/>
-      <c r="I62" s="50"/>
-    </row>
-    <row r="63" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A63" s="64"/>
-      <c r="B63" s="82" t="s">
+      <c r="D68" s="98"/>
+      <c r="E68" s="48"/>
+      <c r="F68" s="48"/>
+      <c r="G68" s="48"/>
+      <c r="H68" s="48"/>
+      <c r="I68" s="49"/>
+    </row>
+    <row r="69" spans="1:9" s="50" customFormat="1" ht="24" x14ac:dyDescent="0.45">
+      <c r="A69" s="63"/>
+      <c r="B69" s="81" t="s">
         <v>95</v>
       </c>
-      <c r="C63" s="113" t="s">
+      <c r="C69" s="112" t="s">
         <v>162</v>
       </c>
-      <c r="D63" s="99"/>
-      <c r="E63" s="49"/>
-      <c r="F63" s="49"/>
-      <c r="G63" s="49"/>
-      <c r="H63" s="49"/>
-      <c r="I63" s="50"/>
+      <c r="D69" s="98"/>
+      <c r="E69" s="48"/>
+      <c r="F69" s="48"/>
+      <c r="G69" s="48"/>
+      <c r="H69" s="48"/>
+      <c r="I69" s="49"/>
     </row>
   </sheetData>
   <sheetProtection deleteColumns="0" selectLockedCells="1"/>
@@ -2678,7 +2766,7 @@
           <x14:formula1>
             <xm:f>'Drop Down List Values'!$M$2:$M$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D63:H63</xm:sqref>
+          <xm:sqref>D69:H69</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{33A578CF-33CA-4B41-B2C5-7541E5042FC9}">
           <x14:formula1>
@@ -2712,24 +2800,24 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="62" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="49.21875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="49.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -2770,7 +2858,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -2811,7 +2899,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>49</v>
       </c>
@@ -2852,7 +2940,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>168</v>
       </c>
@@ -2893,7 +2981,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -2925,7 +3013,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -2945,7 +3033,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>52</v>
       </c>
@@ -3276,17 +3364,17 @@
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69E3EF86-6C9E-4C22-A476-13DA012C68C5}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b541edd5-2552-480e-ada6-0e2c8d317108"/>
+    <ds:schemaRef ds:uri="3146657c-56f4-4c0a-bb9c-a675121ac670"/>
+    <ds:schemaRef ds:uri="780ae317-08c5-4e10-af93-dd385a8384a9"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="780ae317-08c5-4e10-af93-dd385a8384a9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="3146657c-56f4-4c0a-bb9c-a675121ac670"/>
-    <ds:schemaRef ds:uri="b541edd5-2552-480e-ada6-0e2c8d317108"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Major datetime management workflow added. Fixed up the xlsx templates to provide suggested formatting in the excel sheets themselves.
</commit_message>
<xml_diff>
--- a/MDI-To-EDRS-Template.xlsx
+++ b/MDI-To-EDRS-Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20403"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20405"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mriley7\workspace\raven-import-and-submit-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F43D857-94EB-472C-B98C-8C7156000CAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C671669-30A5-4663-937D-603704E65E52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8490" xr2:uid="{7A50F290-1C75-487E-9806-F93553E4E7CC}"/>
   </bookViews>
@@ -689,8 +689,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="167" formatCode="000\-00\-0000"/>
+    <numFmt numFmtId="168" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="170" formatCode="[$-409]h:mm:ss\ AM/PM;@"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -977,7 +980,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -1018,10 +1021,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="14" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -1060,14 +1059,6 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -1108,10 +1099,6 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
@@ -1119,15 +1106,7 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="14" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -1229,10 +1208,6 @@
     <xf numFmtId="0" fontId="7" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="14" fontId="3" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -1253,10 +1228,6 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
@@ -1265,19 +1236,7 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="14" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -1361,6 +1320,54 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="14" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="14" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1700,28 +1707,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54CD1DC7-E143-4CF5-BEA9-4DABBAFFC7B0}">
   <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="22.5" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" style="52" customWidth="1"/>
-    <col min="2" max="2" width="64.42578125" style="64" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" style="72" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" style="46" customWidth="1"/>
+    <col min="2" max="2" width="64.42578125" style="58" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" style="66" customWidth="1"/>
     <col min="4" max="8" width="32.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="58" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="72" t="s">
+      <c r="C1" s="66" t="s">
         <v>27</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -1744,27 +1751,27 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="36.75" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C2" s="72" t="s">
+      <c r="C2" s="66" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="120" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="46" t="s">
         <v>169</v>
       </c>
-      <c r="B3" s="120" t="s">
+      <c r="B3" s="109" t="s">
         <v>171</v>
       </c>
-      <c r="C3" s="121" t="s">
+      <c r="C3" s="110" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="4" customFormat="1" ht="36.75" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="99" t="s">
+      <c r="B4" s="59"/>
+      <c r="C4" s="88" t="s">
         <v>101</v>
       </c>
       <c r="D4" s="3"/>
@@ -1775,41 +1782,41 @@
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.45">
-      <c r="A5" s="54"/>
-      <c r="B5" s="117" t="s">
+      <c r="A5" s="48"/>
+      <c r="B5" s="106" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="100" t="s">
+      <c r="C5" s="89" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
       <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:9" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.45">
-      <c r="A6" s="54"/>
-      <c r="B6" s="118" t="s">
+      <c r="A6" s="48"/>
+      <c r="B6" s="107" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="100" t="s">
+      <c r="C6" s="89" t="s">
         <v>103</v>
       </c>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="51"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
       <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:9" s="8" customFormat="1" ht="36" x14ac:dyDescent="0.45">
-      <c r="A7" s="55" t="s">
+      <c r="A7" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="66"/>
-      <c r="C7" s="101" t="s">
+      <c r="B7" s="60"/>
+      <c r="C7" s="90" t="s">
         <v>105</v>
       </c>
       <c r="D7" s="7"/>
@@ -1820,14 +1827,14 @@
       <c r="I7" s="7"/>
     </row>
     <row r="8" spans="1:9" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.45">
-      <c r="A8" s="56"/>
-      <c r="B8" s="73" t="s">
+      <c r="A8" s="50"/>
+      <c r="B8" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="102" t="s">
+      <c r="C8" s="91" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="14"/>
+      <c r="D8" s="13"/>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
@@ -1835,14 +1842,14 @@
       <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:9" s="11" customFormat="1" ht="60" x14ac:dyDescent="0.45">
-      <c r="A9" s="56"/>
-      <c r="B9" s="73" t="s">
+      <c r="A9" s="50"/>
+      <c r="B9" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="102" t="s">
+      <c r="C9" s="91" t="s">
         <v>108</v>
       </c>
-      <c r="D9" s="14"/>
+      <c r="D9" s="13"/>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
@@ -1850,14 +1857,14 @@
       <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:9" s="11" customFormat="1" ht="24" x14ac:dyDescent="0.45">
-      <c r="A10" s="56"/>
-      <c r="B10" s="73" t="s">
+      <c r="A10" s="50"/>
+      <c r="B10" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="102" t="s">
+      <c r="C10" s="91" t="s">
         <v>107</v>
       </c>
-      <c r="D10" s="14"/>
+      <c r="D10" s="13"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
@@ -1865,14 +1872,14 @@
       <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9" s="11" customFormat="1" ht="36" x14ac:dyDescent="0.45">
-      <c r="A11" s="56"/>
-      <c r="B11" s="74" t="s">
+      <c r="A11" s="50"/>
+      <c r="B11" s="68" t="s">
         <v>76</v>
       </c>
-      <c r="C11" s="102" t="s">
+      <c r="C11" s="91" t="s">
         <v>106</v>
       </c>
-      <c r="D11" s="14"/>
+      <c r="D11" s="13"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
@@ -1880,29 +1887,29 @@
       <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:9" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.45">
-      <c r="A12" s="56"/>
-      <c r="B12" s="73" t="s">
+      <c r="A12" s="50"/>
+      <c r="B12" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="102" t="s">
+      <c r="C12" s="91" t="s">
         <v>155</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
+      <c r="D12" s="112"/>
+      <c r="E12" s="113"/>
+      <c r="F12" s="113"/>
+      <c r="G12" s="113"/>
+      <c r="H12" s="113"/>
       <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.45">
-      <c r="A13" s="56"/>
-      <c r="B13" s="73" t="s">
+      <c r="A13" s="50"/>
+      <c r="B13" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="102" t="s">
+      <c r="C13" s="91" t="s">
         <v>109</v>
       </c>
-      <c r="D13" s="14"/>
+      <c r="D13" s="13"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
@@ -1910,27 +1917,27 @@
       <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.45">
-      <c r="A14" s="56"/>
-      <c r="B14" s="73" t="s">
+      <c r="A14" s="50"/>
+      <c r="B14" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="102" t="s">
+      <c r="C14" s="91" t="s">
         <v>110</v>
       </c>
-      <c r="D14" s="84"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
+      <c r="D14" s="114"/>
+      <c r="E14" s="115"/>
+      <c r="F14" s="115"/>
+      <c r="G14" s="115"/>
+      <c r="H14" s="115"/>
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="56"/>
-      <c r="B15" s="73" t="s">
+      <c r="A15" s="50"/>
+      <c r="B15" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="102"/>
-      <c r="D15" s="14"/>
+      <c r="C15" s="91"/>
+      <c r="D15" s="13"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
@@ -1938,27 +1945,27 @@
       <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:9" s="11" customFormat="1" ht="24" x14ac:dyDescent="0.45">
-      <c r="A16" s="56"/>
-      <c r="B16" s="73" t="s">
+      <c r="A16" s="50"/>
+      <c r="B16" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="102" t="s">
+      <c r="C16" s="91" t="s">
         <v>111</v>
       </c>
-      <c r="D16" s="85"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
       <c r="H16" s="9"/>
       <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="56"/>
-      <c r="B17" s="73" t="s">
+      <c r="A17" s="50"/>
+      <c r="B17" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="102"/>
-      <c r="D17" s="14"/>
+      <c r="C17" s="91"/>
+      <c r="D17" s="13"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
@@ -1966,12 +1973,12 @@
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="56"/>
-      <c r="B18" s="73" t="s">
+      <c r="A18" s="50"/>
+      <c r="B18" s="67" t="s">
         <v>99</v>
       </c>
-      <c r="C18" s="102"/>
-      <c r="D18" s="14"/>
+      <c r="C18" s="91"/>
+      <c r="D18" s="13"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
@@ -1979,12 +1986,12 @@
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="56"/>
-      <c r="B19" s="75" t="s">
+      <c r="A19" s="50"/>
+      <c r="B19" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="102"/>
-      <c r="D19" s="14"/>
+      <c r="C19" s="91"/>
+      <c r="D19" s="13"/>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
@@ -1992,12 +1999,12 @@
       <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="56"/>
-      <c r="B20" s="73" t="s">
+      <c r="A20" s="50"/>
+      <c r="B20" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="102"/>
-      <c r="D20" s="14"/>
+      <c r="C20" s="91"/>
+      <c r="D20" s="13"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
@@ -2005,707 +2012,707 @@
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="56"/>
-      <c r="B21" s="73" t="s">
+      <c r="A21" s="50"/>
+      <c r="B21" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="102"/>
-      <c r="D21" s="14"/>
+      <c r="C21" s="91"/>
+      <c r="D21" s="13"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
       <c r="I21" s="10"/>
     </row>
-    <row r="22" spans="1:9" s="16" customFormat="1" ht="84" x14ac:dyDescent="0.45">
-      <c r="A22" s="113" t="s">
+    <row r="22" spans="1:9" s="15" customFormat="1" ht="84" x14ac:dyDescent="0.45">
+      <c r="A22" s="102" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="67"/>
-      <c r="C22" s="103" t="s">
+      <c r="B22" s="61"/>
+      <c r="C22" s="92" t="s">
         <v>112</v>
       </c>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-    </row>
-    <row r="23" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="57"/>
-      <c r="B23" s="119" t="s">
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+    </row>
+    <row r="23" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="51"/>
+      <c r="B23" s="108" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="104" t="s">
+      <c r="C23" s="93" t="s">
         <v>113</v>
       </c>
-      <c r="D23" s="86"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="18"/>
-    </row>
-    <row r="24" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="57"/>
-      <c r="B24" s="119" t="s">
+      <c r="D23" s="79"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="17"/>
+    </row>
+    <row r="24" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="51"/>
+      <c r="B24" s="108" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="104" t="s">
+      <c r="C24" s="93" t="s">
         <v>114</v>
       </c>
-      <c r="D24" s="87"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="18"/>
-    </row>
-    <row r="25" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="57"/>
-      <c r="B25" s="119" t="s">
+      <c r="D24" s="80"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="17"/>
+    </row>
+    <row r="25" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="51"/>
+      <c r="B25" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="104" t="s">
+      <c r="C25" s="93" t="s">
         <v>115</v>
       </c>
-      <c r="D25" s="88"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="18"/>
-    </row>
-    <row r="26" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="57"/>
-      <c r="B26" s="119" t="s">
+      <c r="D25" s="81"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="17"/>
+    </row>
+    <row r="26" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="51"/>
+      <c r="B26" s="108" t="s">
         <v>98</v>
       </c>
-      <c r="C26" s="104" t="s">
+      <c r="C26" s="93" t="s">
         <v>116</v>
       </c>
-      <c r="D26" s="88"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="18"/>
-    </row>
-    <row r="27" spans="1:9" s="19" customFormat="1" ht="48" x14ac:dyDescent="0.45">
-      <c r="A27" s="57"/>
-      <c r="B27" s="119" t="s">
+      <c r="D26" s="81"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="17"/>
+    </row>
+    <row r="27" spans="1:9" s="18" customFormat="1" ht="48" x14ac:dyDescent="0.45">
+      <c r="A27" s="51"/>
+      <c r="B27" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="104" t="s">
+      <c r="C27" s="93" t="s">
         <v>117</v>
       </c>
-      <c r="D27" s="88"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="18"/>
-    </row>
-    <row r="28" spans="1:9" s="19" customFormat="1" ht="48" x14ac:dyDescent="0.45">
-      <c r="A28" s="57"/>
-      <c r="B28" s="119" t="s">
+      <c r="D27" s="81"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="17"/>
+    </row>
+    <row r="28" spans="1:9" s="18" customFormat="1" ht="48" x14ac:dyDescent="0.45">
+      <c r="A28" s="51"/>
+      <c r="B28" s="108" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="104" t="s">
+      <c r="C28" s="93" t="s">
         <v>118</v>
       </c>
-      <c r="D28" s="88"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="18"/>
-    </row>
-    <row r="29" spans="1:9" s="19" customFormat="1" ht="48" x14ac:dyDescent="0.45">
-      <c r="A29" s="57"/>
-      <c r="B29" s="119" t="s">
+      <c r="D28" s="81"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="17"/>
+    </row>
+    <row r="29" spans="1:9" s="18" customFormat="1" ht="48" x14ac:dyDescent="0.45">
+      <c r="A29" s="51"/>
+      <c r="B29" s="108" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="104" t="s">
+      <c r="C29" s="93" t="s">
         <v>119</v>
       </c>
-      <c r="D29" s="88"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="18"/>
-    </row>
-    <row r="30" spans="1:9" s="19" customFormat="1" ht="48" x14ac:dyDescent="0.45">
-      <c r="A30" s="57"/>
-      <c r="B30" s="119" t="s">
+      <c r="D29" s="81"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="17"/>
+    </row>
+    <row r="30" spans="1:9" s="18" customFormat="1" ht="48" x14ac:dyDescent="0.45">
+      <c r="A30" s="51"/>
+      <c r="B30" s="108" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="104" t="s">
+      <c r="C30" s="93" t="s">
         <v>120</v>
       </c>
-      <c r="D30" s="86"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="18"/>
-    </row>
-    <row r="31" spans="1:9" s="19" customFormat="1" ht="48" x14ac:dyDescent="0.45">
-      <c r="A31" s="57"/>
-      <c r="B31" s="119" t="s">
+      <c r="D30" s="79"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="17"/>
+    </row>
+    <row r="31" spans="1:9" s="18" customFormat="1" ht="48" x14ac:dyDescent="0.45">
+      <c r="A31" s="51"/>
+      <c r="B31" s="108" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="104" t="s">
+      <c r="C31" s="93" t="s">
         <v>121</v>
       </c>
-      <c r="D31" s="89"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="18"/>
-    </row>
-    <row r="32" spans="1:9" s="19" customFormat="1" ht="24" x14ac:dyDescent="0.45">
-      <c r="A32" s="57"/>
-      <c r="B32" s="76" t="s">
+      <c r="D31" s="82"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="17"/>
+    </row>
+    <row r="32" spans="1:9" s="18" customFormat="1" ht="24" x14ac:dyDescent="0.45">
+      <c r="A32" s="51"/>
+      <c r="B32" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="C32" s="104" t="s">
+      <c r="C32" s="93" t="s">
         <v>122</v>
       </c>
-      <c r="D32" s="89"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="18"/>
-    </row>
-    <row r="33" spans="1:9" s="19" customFormat="1" ht="60" x14ac:dyDescent="0.45">
-      <c r="A33" s="57"/>
-      <c r="B33" s="76" t="s">
+      <c r="D32" s="82"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="17"/>
+    </row>
+    <row r="33" spans="1:9" s="18" customFormat="1" ht="60" x14ac:dyDescent="0.45">
+      <c r="A33" s="51"/>
+      <c r="B33" s="70" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="104" t="s">
+      <c r="C33" s="93" t="s">
         <v>123</v>
       </c>
-      <c r="D33" s="90"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="23"/>
-      <c r="H33" s="23"/>
-      <c r="I33" s="18"/>
-    </row>
-    <row r="34" spans="1:9" s="19" customFormat="1" ht="84" x14ac:dyDescent="0.45">
-      <c r="A34" s="57"/>
-      <c r="B34" s="76" t="s">
+      <c r="D33" s="116"/>
+      <c r="E33" s="117"/>
+      <c r="F33" s="117"/>
+      <c r="G33" s="117"/>
+      <c r="H33" s="117"/>
+      <c r="I33" s="17"/>
+    </row>
+    <row r="34" spans="1:9" s="18" customFormat="1" ht="84" x14ac:dyDescent="0.45">
+      <c r="A34" s="51"/>
+      <c r="B34" s="70" t="s">
         <v>83</v>
       </c>
-      <c r="C34" s="104" t="s">
+      <c r="C34" s="93" t="s">
         <v>124</v>
       </c>
-      <c r="D34" s="89"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="24"/>
-      <c r="I34" s="18"/>
-    </row>
-    <row r="35" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="58"/>
-      <c r="B35" s="76" t="s">
+      <c r="D34" s="118"/>
+      <c r="E34" s="119"/>
+      <c r="F34" s="119"/>
+      <c r="G34" s="119"/>
+      <c r="H34" s="119"/>
+      <c r="I34" s="17"/>
+    </row>
+    <row r="35" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="52"/>
+      <c r="B35" s="70" t="s">
         <v>82</v>
       </c>
-      <c r="C35" s="104" t="s">
+      <c r="C35" s="93" t="s">
         <v>125</v>
       </c>
-      <c r="D35" s="88"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="25"/>
-    </row>
-    <row r="36" spans="1:9" s="19" customFormat="1" ht="36" x14ac:dyDescent="0.45">
-      <c r="A36" s="57"/>
-      <c r="B36" s="76" t="s">
+      <c r="D35" s="81"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="22"/>
+    </row>
+    <row r="36" spans="1:9" s="18" customFormat="1" ht="36" x14ac:dyDescent="0.45">
+      <c r="A36" s="51"/>
+      <c r="B36" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="C36" s="104" t="s">
+      <c r="C36" s="93" t="s">
         <v>126</v>
       </c>
-      <c r="D36" s="89"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="22"/>
-      <c r="I36" s="18"/>
-    </row>
-    <row r="37" spans="1:9" s="19" customFormat="1" ht="36" x14ac:dyDescent="0.45">
-      <c r="A37" s="57"/>
-      <c r="B37" s="76" t="s">
+      <c r="D36" s="82"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="17"/>
+    </row>
+    <row r="37" spans="1:9" s="18" customFormat="1" ht="36" x14ac:dyDescent="0.45">
+      <c r="A37" s="51"/>
+      <c r="B37" s="70" t="s">
         <v>43</v>
       </c>
-      <c r="C37" s="104" t="s">
+      <c r="C37" s="93" t="s">
         <v>127</v>
       </c>
-      <c r="D37" s="89"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
-      <c r="I37" s="18"/>
-    </row>
-    <row r="38" spans="1:9" s="28" customFormat="1" ht="84" x14ac:dyDescent="0.45">
-      <c r="A38" s="114" t="s">
+      <c r="D37" s="82"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="17"/>
+    </row>
+    <row r="38" spans="1:9" s="25" customFormat="1" ht="84" x14ac:dyDescent="0.45">
+      <c r="A38" s="103" t="s">
         <v>30</v>
       </c>
-      <c r="B38" s="68"/>
-      <c r="C38" s="105" t="s">
+      <c r="B38" s="62"/>
+      <c r="C38" s="94" t="s">
         <v>143</v>
       </c>
-      <c r="D38" s="27"/>
-      <c r="E38" s="27"/>
-      <c r="F38" s="27"/>
-      <c r="G38" s="27"/>
-      <c r="H38" s="27"/>
-      <c r="I38" s="27"/>
-    </row>
-    <row r="39" spans="1:9" s="31" customFormat="1" ht="24" x14ac:dyDescent="0.45">
-      <c r="A39" s="59"/>
-      <c r="B39" s="77" t="s">
+      <c r="D38" s="24"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="24"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="24"/>
+    </row>
+    <row r="39" spans="1:9" s="28" customFormat="1" ht="24" x14ac:dyDescent="0.45">
+      <c r="A39" s="53"/>
+      <c r="B39" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="106" t="s">
+      <c r="C39" s="95" t="s">
         <v>128</v>
       </c>
-      <c r="D39" s="91"/>
-      <c r="E39" s="29"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="29"/>
-      <c r="H39" s="29"/>
-      <c r="I39" s="30"/>
-    </row>
-    <row r="40" spans="1:9" s="31" customFormat="1" ht="24" x14ac:dyDescent="0.45">
-      <c r="A40" s="59"/>
-      <c r="B40" s="78" t="s">
+      <c r="D39" s="83"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="26"/>
+      <c r="H39" s="26"/>
+      <c r="I39" s="27"/>
+    </row>
+    <row r="40" spans="1:9" s="28" customFormat="1" ht="24" x14ac:dyDescent="0.45">
+      <c r="A40" s="53"/>
+      <c r="B40" s="72" t="s">
         <v>96</v>
       </c>
-      <c r="C40" s="106" t="s">
+      <c r="C40" s="95" t="s">
         <v>166</v>
       </c>
-      <c r="D40" s="91"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="32"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="32"/>
-      <c r="I40" s="30"/>
-    </row>
-    <row r="41" spans="1:9" s="31" customFormat="1" ht="36" x14ac:dyDescent="0.45">
-      <c r="A41" s="59"/>
-      <c r="B41" s="77" t="s">
+      <c r="D40" s="83"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="27"/>
+    </row>
+    <row r="41" spans="1:9" s="28" customFormat="1" ht="36" x14ac:dyDescent="0.45">
+      <c r="A41" s="53"/>
+      <c r="B41" s="71" t="s">
         <v>77</v>
       </c>
-      <c r="C41" s="106" t="s">
+      <c r="C41" s="95" t="s">
         <v>129</v>
       </c>
-      <c r="D41" s="91"/>
-      <c r="E41" s="91"/>
-      <c r="F41" s="91"/>
-      <c r="G41" s="91"/>
-      <c r="H41" s="91"/>
-      <c r="I41" s="30"/>
-    </row>
-    <row r="42" spans="1:9" s="31" customFormat="1" ht="36" x14ac:dyDescent="0.45">
-      <c r="A42" s="59"/>
-      <c r="B42" s="116" t="s">
+      <c r="D41" s="83"/>
+      <c r="E41" s="83"/>
+      <c r="F41" s="83"/>
+      <c r="G41" s="83"/>
+      <c r="H41" s="83"/>
+      <c r="I41" s="27"/>
+    </row>
+    <row r="42" spans="1:9" s="28" customFormat="1" ht="36" x14ac:dyDescent="0.45">
+      <c r="A42" s="53"/>
+      <c r="B42" s="105" t="s">
         <v>1</v>
       </c>
-      <c r="C42" s="106" t="s">
+      <c r="C42" s="95" t="s">
         <v>130</v>
       </c>
-      <c r="D42" s="91"/>
-      <c r="E42" s="29"/>
-      <c r="F42" s="29"/>
-      <c r="G42" s="29"/>
-      <c r="H42" s="29"/>
-      <c r="I42" s="30"/>
-    </row>
-    <row r="43" spans="1:9" s="35" customFormat="1" ht="60" x14ac:dyDescent="0.45">
-      <c r="A43" s="122" t="s">
+      <c r="D42" s="83"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26"/>
+      <c r="G42" s="26"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="27"/>
+    </row>
+    <row r="43" spans="1:9" s="32" customFormat="1" ht="60" x14ac:dyDescent="0.45">
+      <c r="A43" s="111" t="s">
         <v>172</v>
       </c>
-      <c r="B43" s="69"/>
-      <c r="C43" s="107" t="s">
+      <c r="B43" s="63"/>
+      <c r="C43" s="96" t="s">
         <v>144</v>
       </c>
-      <c r="D43" s="92"/>
-      <c r="E43" s="33"/>
-      <c r="F43" s="33"/>
-      <c r="G43" s="33"/>
-      <c r="H43" s="33"/>
-      <c r="I43" s="34"/>
-    </row>
-    <row r="44" spans="1:9" s="38" customFormat="1" ht="48" x14ac:dyDescent="0.45">
-      <c r="A44" s="60"/>
-      <c r="B44" s="79" t="s">
+      <c r="D43" s="84"/>
+      <c r="E43" s="30"/>
+      <c r="F43" s="30"/>
+      <c r="G43" s="30"/>
+      <c r="H43" s="30"/>
+      <c r="I43" s="31"/>
+    </row>
+    <row r="44" spans="1:9" s="34" customFormat="1" ht="48" x14ac:dyDescent="0.45">
+      <c r="A44" s="54"/>
+      <c r="B44" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="C44" s="108" t="s">
+      <c r="C44" s="97" t="s">
         <v>131</v>
       </c>
-      <c r="D44" s="93"/>
-      <c r="E44" s="36"/>
-      <c r="F44" s="36"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="37"/>
-    </row>
-    <row r="45" spans="1:9" s="38" customFormat="1" ht="84" x14ac:dyDescent="0.45">
-      <c r="A45" s="60"/>
-      <c r="B45" s="79" t="s">
+      <c r="D44" s="120"/>
+      <c r="E44" s="121"/>
+      <c r="F44" s="121"/>
+      <c r="G44" s="121"/>
+      <c r="H44" s="121"/>
+      <c r="I44" s="33"/>
+    </row>
+    <row r="45" spans="1:9" s="34" customFormat="1" ht="84" x14ac:dyDescent="0.45">
+      <c r="A45" s="54"/>
+      <c r="B45" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="C45" s="108" t="s">
+      <c r="C45" s="97" t="s">
         <v>132</v>
       </c>
-      <c r="D45" s="94"/>
-      <c r="E45" s="39"/>
-      <c r="F45" s="39"/>
-      <c r="G45" s="39"/>
-      <c r="H45" s="39"/>
-      <c r="I45" s="37"/>
-    </row>
-    <row r="46" spans="1:9" s="38" customFormat="1" ht="36" x14ac:dyDescent="0.45">
-      <c r="A46" s="60"/>
-      <c r="B46" s="79" t="s">
+      <c r="D45" s="122"/>
+      <c r="E45" s="123"/>
+      <c r="F45" s="123"/>
+      <c r="G45" s="123"/>
+      <c r="H45" s="123"/>
+      <c r="I45" s="33"/>
+    </row>
+    <row r="46" spans="1:9" s="34" customFormat="1" ht="36" x14ac:dyDescent="0.45">
+      <c r="A46" s="54"/>
+      <c r="B46" s="73" t="s">
         <v>78</v>
       </c>
-      <c r="C46" s="108" t="s">
+      <c r="C46" s="97" t="s">
         <v>137</v>
       </c>
-      <c r="D46" s="95"/>
-      <c r="E46" s="40"/>
-      <c r="F46" s="40"/>
-      <c r="G46" s="40"/>
-      <c r="H46" s="40"/>
-      <c r="I46" s="37"/>
-    </row>
-    <row r="47" spans="1:9" s="38" customFormat="1" ht="60" x14ac:dyDescent="0.45">
-      <c r="A47" s="60"/>
-      <c r="B47" s="79" t="s">
+      <c r="D46" s="85"/>
+      <c r="E46" s="35"/>
+      <c r="F46" s="35"/>
+      <c r="G46" s="35"/>
+      <c r="H46" s="35"/>
+      <c r="I46" s="33"/>
+    </row>
+    <row r="47" spans="1:9" s="34" customFormat="1" ht="60" x14ac:dyDescent="0.45">
+      <c r="A47" s="54"/>
+      <c r="B47" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="C47" s="108" t="s">
+      <c r="C47" s="97" t="s">
         <v>138</v>
       </c>
-      <c r="D47" s="96"/>
-      <c r="E47" s="41"/>
-      <c r="F47" s="41"/>
-      <c r="G47" s="41"/>
-      <c r="H47" s="41"/>
-      <c r="I47" s="37"/>
-    </row>
-    <row r="48" spans="1:9" s="38" customFormat="1" ht="96" x14ac:dyDescent="0.45">
-      <c r="A48" s="60"/>
-      <c r="B48" s="79" t="s">
+      <c r="D47" s="120"/>
+      <c r="E47" s="121"/>
+      <c r="F47" s="121"/>
+      <c r="G47" s="121"/>
+      <c r="H47" s="121"/>
+      <c r="I47" s="33"/>
+    </row>
+    <row r="48" spans="1:9" s="34" customFormat="1" ht="96" x14ac:dyDescent="0.45">
+      <c r="A48" s="54"/>
+      <c r="B48" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="C48" s="108" t="s">
+      <c r="C48" s="97" t="s">
         <v>139</v>
       </c>
-      <c r="D48" s="94"/>
-      <c r="E48" s="39"/>
-      <c r="F48" s="39"/>
-      <c r="G48" s="39"/>
-      <c r="H48" s="39"/>
-      <c r="I48" s="37"/>
-    </row>
-    <row r="49" spans="1:9" s="38" customFormat="1" ht="36" x14ac:dyDescent="0.45">
-      <c r="A49" s="60"/>
-      <c r="B49" s="79" t="s">
+      <c r="D48" s="122"/>
+      <c r="E48" s="123"/>
+      <c r="F48" s="123"/>
+      <c r="G48" s="123"/>
+      <c r="H48" s="123"/>
+      <c r="I48" s="33"/>
+    </row>
+    <row r="49" spans="1:9" s="34" customFormat="1" ht="36" x14ac:dyDescent="0.45">
+      <c r="A49" s="54"/>
+      <c r="B49" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="C49" s="108" t="s">
+      <c r="C49" s="97" t="s">
         <v>140</v>
       </c>
-      <c r="D49" s="95"/>
-      <c r="E49" s="40"/>
-      <c r="F49" s="40"/>
-      <c r="G49" s="40"/>
-      <c r="H49" s="40"/>
-      <c r="I49" s="37"/>
-    </row>
-    <row r="50" spans="1:9" s="43" customFormat="1" ht="24" x14ac:dyDescent="0.45">
-      <c r="A50" s="61" t="s">
+      <c r="D49" s="85"/>
+      <c r="E49" s="35"/>
+      <c r="F49" s="35"/>
+      <c r="G49" s="35"/>
+      <c r="H49" s="35"/>
+      <c r="I49" s="33"/>
+    </row>
+    <row r="50" spans="1:9" s="37" customFormat="1" ht="24" x14ac:dyDescent="0.45">
+      <c r="A50" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="B50" s="70"/>
-      <c r="C50" s="109" t="s">
+      <c r="B50" s="64"/>
+      <c r="C50" s="98" t="s">
         <v>145</v>
       </c>
-      <c r="D50" s="42"/>
-      <c r="E50" s="42"/>
-      <c r="F50" s="42"/>
-      <c r="G50" s="42"/>
-      <c r="H50" s="42"/>
-      <c r="I50" s="42"/>
-    </row>
-    <row r="51" spans="1:9" s="45" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="62"/>
-      <c r="B51" s="80" t="s">
+      <c r="D50" s="36"/>
+      <c r="E50" s="36"/>
+      <c r="F50" s="36"/>
+      <c r="G50" s="36"/>
+      <c r="H50" s="36"/>
+      <c r="I50" s="36"/>
+    </row>
+    <row r="51" spans="1:9" s="39" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A51" s="56"/>
+      <c r="B51" s="74" t="s">
         <v>45</v>
       </c>
-      <c r="C51" s="110" t="s">
+      <c r="C51" s="99" t="s">
         <v>141</v>
       </c>
-      <c r="D51" s="97"/>
-      <c r="E51" s="97"/>
-      <c r="F51" s="97"/>
-      <c r="G51" s="97"/>
-      <c r="H51" s="97"/>
-      <c r="I51" s="44"/>
-    </row>
-    <row r="52" spans="1:9" s="62" customFormat="1" ht="36" x14ac:dyDescent="0.45">
-      <c r="B52" s="80" t="s">
+      <c r="D51" s="86"/>
+      <c r="E51" s="86"/>
+      <c r="F51" s="86"/>
+      <c r="G51" s="86"/>
+      <c r="H51" s="86"/>
+      <c r="I51" s="38"/>
+    </row>
+    <row r="52" spans="1:9" s="56" customFormat="1" ht="36" x14ac:dyDescent="0.45">
+      <c r="B52" s="74" t="s">
         <v>81</v>
       </c>
-      <c r="C52" s="110" t="s">
+      <c r="C52" s="99" t="s">
         <v>142</v>
       </c>
-      <c r="D52" s="97"/>
-      <c r="E52" s="97"/>
-      <c r="F52" s="97"/>
-      <c r="G52" s="97"/>
-      <c r="H52" s="97"/>
-    </row>
-    <row r="53" spans="1:9" s="62" customFormat="1" ht="24" x14ac:dyDescent="0.45">
-      <c r="B53" s="80" t="s">
+      <c r="D52" s="86"/>
+      <c r="E52" s="86"/>
+      <c r="F52" s="86"/>
+      <c r="G52" s="86"/>
+      <c r="H52" s="86"/>
+    </row>
+    <row r="53" spans="1:9" s="56" customFormat="1" ht="24" x14ac:dyDescent="0.45">
+      <c r="B53" s="74" t="s">
         <v>180</v>
       </c>
-      <c r="C53" s="110" t="s">
+      <c r="C53" s="99" t="s">
         <v>181</v>
       </c>
-      <c r="D53" s="97"/>
-      <c r="E53" s="97"/>
-      <c r="F53" s="97"/>
-      <c r="G53" s="97"/>
-      <c r="H53" s="97"/>
-    </row>
-    <row r="54" spans="1:9" s="62" customFormat="1" ht="24" x14ac:dyDescent="0.45">
-      <c r="B54" s="80" t="s">
+      <c r="D53" s="86"/>
+      <c r="E53" s="86"/>
+      <c r="F53" s="86"/>
+      <c r="G53" s="86"/>
+      <c r="H53" s="86"/>
+    </row>
+    <row r="54" spans="1:9" s="56" customFormat="1" ht="24" x14ac:dyDescent="0.45">
+      <c r="B54" s="74" t="s">
         <v>174</v>
       </c>
-      <c r="C54" s="110" t="s">
+      <c r="C54" s="99" t="s">
         <v>177</v>
       </c>
-      <c r="D54" s="97"/>
-      <c r="E54" s="97"/>
-      <c r="F54" s="97"/>
-      <c r="G54" s="97"/>
-      <c r="H54" s="97"/>
-    </row>
-    <row r="55" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B55" s="80" t="s">
+      <c r="D54" s="86"/>
+      <c r="E54" s="86"/>
+      <c r="F54" s="86"/>
+      <c r="G54" s="86"/>
+      <c r="H54" s="86"/>
+    </row>
+    <row r="55" spans="1:9" s="56" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B55" s="74" t="s">
         <v>175</v>
       </c>
-      <c r="C55" s="110"/>
-      <c r="D55" s="97"/>
-      <c r="E55" s="97"/>
-      <c r="F55" s="97"/>
-      <c r="G55" s="97"/>
-      <c r="H55" s="97"/>
-    </row>
-    <row r="56" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B56" s="80" t="s">
+      <c r="C55" s="99"/>
+      <c r="D55" s="86"/>
+      <c r="E55" s="86"/>
+      <c r="F55" s="86"/>
+      <c r="G55" s="86"/>
+      <c r="H55" s="86"/>
+    </row>
+    <row r="56" spans="1:9" s="56" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B56" s="74" t="s">
         <v>176</v>
       </c>
-      <c r="C56" s="110"/>
-      <c r="D56" s="97"/>
-      <c r="E56" s="97"/>
-      <c r="F56" s="97"/>
-      <c r="G56" s="97"/>
-      <c r="H56" s="97"/>
-    </row>
-    <row r="57" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B57" s="80" t="s">
+      <c r="C56" s="99"/>
+      <c r="D56" s="86"/>
+      <c r="E56" s="86"/>
+      <c r="F56" s="86"/>
+      <c r="G56" s="86"/>
+      <c r="H56" s="86"/>
+    </row>
+    <row r="57" spans="1:9" s="56" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B57" s="74" t="s">
         <v>178</v>
       </c>
-      <c r="C57" s="110"/>
-      <c r="D57" s="97"/>
-      <c r="E57" s="97"/>
-      <c r="F57" s="97"/>
-      <c r="G57" s="97"/>
-      <c r="H57" s="97"/>
-    </row>
-    <row r="58" spans="1:9" s="62" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B58" s="80" t="s">
+      <c r="C57" s="99"/>
+      <c r="D57" s="86"/>
+      <c r="E57" s="86"/>
+      <c r="F57" s="86"/>
+      <c r="G57" s="86"/>
+      <c r="H57" s="86"/>
+    </row>
+    <row r="58" spans="1:9" s="56" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B58" s="74" t="s">
         <v>179</v>
       </c>
-      <c r="C58" s="110"/>
-      <c r="D58" s="97"/>
-      <c r="E58" s="97"/>
-      <c r="F58" s="97"/>
-      <c r="G58" s="97"/>
-      <c r="H58" s="97"/>
-    </row>
-    <row r="59" spans="1:9" s="47" customFormat="1" ht="36" x14ac:dyDescent="0.45">
-      <c r="A59" s="115" t="s">
+      <c r="C58" s="99"/>
+      <c r="D58" s="86"/>
+      <c r="E58" s="86"/>
+      <c r="F58" s="86"/>
+      <c r="G58" s="86"/>
+      <c r="H58" s="86"/>
+    </row>
+    <row r="59" spans="1:9" s="41" customFormat="1" ht="36" x14ac:dyDescent="0.45">
+      <c r="A59" s="104" t="s">
         <v>173</v>
       </c>
-      <c r="B59" s="71"/>
-      <c r="C59" s="111" t="s">
+      <c r="B59" s="65"/>
+      <c r="C59" s="100" t="s">
         <v>146</v>
       </c>
-      <c r="D59" s="46"/>
-      <c r="E59" s="46"/>
-      <c r="F59" s="46"/>
-      <c r="G59" s="46"/>
-      <c r="H59" s="46"/>
-      <c r="I59" s="46"/>
-    </row>
-    <row r="60" spans="1:9" s="50" customFormat="1" ht="72" x14ac:dyDescent="0.45">
-      <c r="A60" s="63"/>
-      <c r="B60" s="81" t="s">
+      <c r="D59" s="40"/>
+      <c r="E59" s="40"/>
+      <c r="F59" s="40"/>
+      <c r="G59" s="40"/>
+      <c r="H59" s="40"/>
+      <c r="I59" s="40"/>
+    </row>
+    <row r="60" spans="1:9" s="44" customFormat="1" ht="72" x14ac:dyDescent="0.45">
+      <c r="A60" s="57"/>
+      <c r="B60" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="C60" s="112" t="s">
+      <c r="C60" s="101" t="s">
         <v>147</v>
       </c>
-      <c r="D60" s="98"/>
-      <c r="E60" s="48"/>
-      <c r="F60" s="48"/>
-      <c r="G60" s="48"/>
-      <c r="H60" s="48"/>
-      <c r="I60" s="49"/>
-    </row>
-    <row r="61" spans="1:9" s="50" customFormat="1" ht="48" x14ac:dyDescent="0.45">
-      <c r="A61" s="63"/>
-      <c r="B61" s="82" t="s">
+      <c r="D60" s="87"/>
+      <c r="E60" s="42"/>
+      <c r="F60" s="42"/>
+      <c r="G60" s="42"/>
+      <c r="H60" s="42"/>
+      <c r="I60" s="43"/>
+    </row>
+    <row r="61" spans="1:9" s="44" customFormat="1" ht="48" x14ac:dyDescent="0.45">
+      <c r="A61" s="57"/>
+      <c r="B61" s="76" t="s">
         <v>91</v>
       </c>
-      <c r="C61" s="112" t="s">
+      <c r="C61" s="101" t="s">
         <v>148</v>
       </c>
-      <c r="D61" s="98"/>
-      <c r="E61" s="48"/>
-      <c r="F61" s="48"/>
-      <c r="G61" s="48"/>
-      <c r="H61" s="48"/>
-      <c r="I61" s="49"/>
-    </row>
-    <row r="62" spans="1:9" s="50" customFormat="1" ht="36" x14ac:dyDescent="0.45">
-      <c r="A62" s="63"/>
-      <c r="B62" s="81" t="s">
+      <c r="D61" s="87"/>
+      <c r="E61" s="42"/>
+      <c r="F61" s="42"/>
+      <c r="G61" s="42"/>
+      <c r="H61" s="42"/>
+      <c r="I61" s="43"/>
+    </row>
+    <row r="62" spans="1:9" s="44" customFormat="1" ht="36" x14ac:dyDescent="0.45">
+      <c r="A62" s="57"/>
+      <c r="B62" s="75" t="s">
         <v>92</v>
       </c>
-      <c r="C62" s="112" t="s">
+      <c r="C62" s="101" t="s">
         <v>149</v>
       </c>
-      <c r="D62" s="98"/>
-      <c r="E62" s="48"/>
-      <c r="F62" s="48"/>
-      <c r="G62" s="48"/>
-      <c r="H62" s="48"/>
-      <c r="I62" s="49"/>
-    </row>
-    <row r="63" spans="1:9" s="50" customFormat="1" ht="36" x14ac:dyDescent="0.45">
-      <c r="A63" s="63"/>
-      <c r="B63" s="81" t="s">
+      <c r="D62" s="87"/>
+      <c r="E62" s="42"/>
+      <c r="F62" s="42"/>
+      <c r="G62" s="42"/>
+      <c r="H62" s="42"/>
+      <c r="I62" s="43"/>
+    </row>
+    <row r="63" spans="1:9" s="44" customFormat="1" ht="36" x14ac:dyDescent="0.45">
+      <c r="A63" s="57"/>
+      <c r="B63" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="C63" s="112" t="s">
+      <c r="C63" s="101" t="s">
         <v>150</v>
       </c>
-      <c r="D63" s="98"/>
-      <c r="E63" s="48"/>
-      <c r="F63" s="48"/>
-      <c r="G63" s="48"/>
-      <c r="H63" s="48"/>
-      <c r="I63" s="49"/>
-    </row>
-    <row r="64" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A64" s="63"/>
-      <c r="B64" s="81" t="s">
+      <c r="D63" s="87"/>
+      <c r="E63" s="42"/>
+      <c r="F63" s="42"/>
+      <c r="G63" s="42"/>
+      <c r="H63" s="42"/>
+      <c r="I63" s="43"/>
+    </row>
+    <row r="64" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A64" s="57"/>
+      <c r="B64" s="75" t="s">
         <v>34</v>
       </c>
-      <c r="C64" s="112"/>
-      <c r="D64" s="98"/>
-      <c r="E64" s="48"/>
-      <c r="F64" s="48"/>
-      <c r="G64" s="48"/>
-      <c r="H64" s="48"/>
-      <c r="I64" s="49"/>
-    </row>
-    <row r="65" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A65" s="63"/>
-      <c r="B65" s="81" t="s">
+      <c r="C64" s="101"/>
+      <c r="D64" s="87"/>
+      <c r="E64" s="42"/>
+      <c r="F64" s="42"/>
+      <c r="G64" s="42"/>
+      <c r="H64" s="42"/>
+      <c r="I64" s="43"/>
+    </row>
+    <row r="65" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A65" s="57"/>
+      <c r="B65" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="C65" s="112"/>
-      <c r="D65" s="98"/>
-      <c r="E65" s="48"/>
-      <c r="F65" s="48"/>
-      <c r="G65" s="48"/>
-      <c r="H65" s="48"/>
-      <c r="I65" s="49"/>
-    </row>
-    <row r="66" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A66" s="63"/>
-      <c r="B66" s="83" t="s">
+      <c r="C65" s="101"/>
+      <c r="D65" s="87"/>
+      <c r="E65" s="42"/>
+      <c r="F65" s="42"/>
+      <c r="G65" s="42"/>
+      <c r="H65" s="42"/>
+      <c r="I65" s="43"/>
+    </row>
+    <row r="66" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A66" s="57"/>
+      <c r="B66" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="C66" s="112"/>
-      <c r="D66" s="98"/>
-      <c r="E66" s="48"/>
-      <c r="F66" s="48"/>
-      <c r="G66" s="48"/>
-      <c r="H66" s="48"/>
-      <c r="I66" s="49"/>
-    </row>
-    <row r="67" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A67" s="63"/>
-      <c r="B67" s="83" t="s">
+      <c r="C66" s="101"/>
+      <c r="D66" s="87"/>
+      <c r="E66" s="42"/>
+      <c r="F66" s="42"/>
+      <c r="G66" s="42"/>
+      <c r="H66" s="42"/>
+      <c r="I66" s="43"/>
+    </row>
+    <row r="67" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A67" s="57"/>
+      <c r="B67" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="C67" s="112"/>
-      <c r="D67" s="98"/>
-      <c r="E67" s="48"/>
-      <c r="F67" s="48"/>
-      <c r="G67" s="48"/>
-      <c r="H67" s="48"/>
-      <c r="I67" s="49"/>
-    </row>
-    <row r="68" spans="1:9" s="50" customFormat="1" ht="72" x14ac:dyDescent="0.45">
-      <c r="A68" s="63"/>
-      <c r="B68" s="81" t="s">
+      <c r="C67" s="101"/>
+      <c r="D67" s="87"/>
+      <c r="E67" s="42"/>
+      <c r="F67" s="42"/>
+      <c r="G67" s="42"/>
+      <c r="H67" s="42"/>
+      <c r="I67" s="43"/>
+    </row>
+    <row r="68" spans="1:9" s="44" customFormat="1" ht="72" x14ac:dyDescent="0.45">
+      <c r="A68" s="57"/>
+      <c r="B68" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="C68" s="112" t="s">
+      <c r="C68" s="101" t="s">
         <v>151</v>
       </c>
-      <c r="D68" s="98"/>
-      <c r="E68" s="48"/>
-      <c r="F68" s="48"/>
-      <c r="G68" s="48"/>
-      <c r="H68" s="48"/>
-      <c r="I68" s="49"/>
-    </row>
-    <row r="69" spans="1:9" s="50" customFormat="1" ht="24" x14ac:dyDescent="0.45">
-      <c r="A69" s="63"/>
-      <c r="B69" s="81" t="s">
+      <c r="D68" s="87"/>
+      <c r="E68" s="42"/>
+      <c r="F68" s="42"/>
+      <c r="G68" s="42"/>
+      <c r="H68" s="42"/>
+      <c r="I68" s="43"/>
+    </row>
+    <row r="69" spans="1:9" s="44" customFormat="1" ht="24" x14ac:dyDescent="0.45">
+      <c r="A69" s="57"/>
+      <c r="B69" s="75" t="s">
         <v>95</v>
       </c>
-      <c r="C69" s="112" t="s">
+      <c r="C69" s="101" t="s">
         <v>162</v>
       </c>
-      <c r="D69" s="98"/>
-      <c r="E69" s="48"/>
-      <c r="F69" s="48"/>
-      <c r="G69" s="48"/>
-      <c r="H69" s="48"/>
-      <c r="I69" s="49"/>
+      <c r="D69" s="87"/>
+      <c r="E69" s="42"/>
+      <c r="F69" s="42"/>
+      <c r="G69" s="42"/>
+      <c r="H69" s="42"/>
+      <c r="I69" s="43"/>
     </row>
   </sheetData>
   <sheetProtection deleteColumns="0" selectLockedCells="1"/>
@@ -3054,65 +3061,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="b541edd5-2552-480e-ada6-0e2c8d317108">YVWEJ5DVYS2U-421999773-68</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="b541edd5-2552-480e-ada6-0e2c8d317108">
+      <Url>https://cdcpartners.sharepoint.com/sites/NCHS/nvssmodcop/_layouts/15/DocIdRedir.aspx?ID=YVWEJ5DVYS2U-421999773-68</Url>
+      <Description>YVWEJ5DVYS2U-421999773-68</Description>
+    </_dlc_DocIdUrl>
+    <ShareFileCreator xmlns="780ae317-08c5-4e10-af93-dd385a8384a9" xsi:nil="true"/>
+    <ShareFileCreated xmlns="780ae317-08c5-4e10-af93-dd385a8384a9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D4902BA52C7D94A994657A564808B2B" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e4455a60d2ff5f5fcd8815d6d89b5b66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b541edd5-2552-480e-ada6-0e2c8d317108" xmlns:ns3="780ae317-08c5-4e10-af93-dd385a8384a9" xmlns:ns4="3146657c-56f4-4c0a-bb9c-a675121ac670" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d1d01ecd782f081d5d944fa263943fc4" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="b541edd5-2552-480e-ada6-0e2c8d317108"/>
@@ -3311,37 +3273,84 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="b541edd5-2552-480e-ada6-0e2c8d317108">YVWEJ5DVYS2U-421999773-68</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="b541edd5-2552-480e-ada6-0e2c8d317108">
-      <Url>https://cdcpartners.sharepoint.com/sites/NCHS/nvssmodcop/_layouts/15/DocIdRedir.aspx?ID=YVWEJ5DVYS2U-421999773-68</Url>
-      <Description>YVWEJ5DVYS2U-421999773-68</Description>
-    </_dlc_DocIdUrl>
-    <ShareFileCreator xmlns="780ae317-08c5-4e10-af93-dd385a8384a9" xsi:nil="true"/>
-    <ShareFileCreated xmlns="780ae317-08c5-4e10-af93-dd385a8384a9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{448710E8-BE9E-4C9E-A40A-0AC1DAE48E99}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69E3EF86-6C9E-4C22-A476-13DA012C68C5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b541edd5-2552-480e-ada6-0e2c8d317108"/>
+    <ds:schemaRef ds:uri="3146657c-56f4-4c0a-bb9c-a675121ac670"/>
+    <ds:schemaRef ds:uri="780ae317-08c5-4e10-af93-dd385a8384a9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF0D7A6D-D78F-4048-9348-0B4289842B11}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0980278E-2A79-4F44-8623-FE545C304BE1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3361,20 +3370,18 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF0D7A6D-D78F-4048-9348-0B4289842B11}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69E3EF86-6C9E-4C22-A476-13DA012C68C5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{448710E8-BE9E-4C9E-A40A-0AC1DAE48E99}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="b541edd5-2552-480e-ada6-0e2c8d317108"/>
-    <ds:schemaRef ds:uri="3146657c-56f4-4c0a-bb9c-a675121ac670"/>
-    <ds:schemaRef ds:uri="780ae317-08c5-4e10-af93-dd385a8384a9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added Certifier identifier and system to import sheet. Fixed VRDR to 5.2.1. Fixed pregnancy valueset.
</commit_message>
<xml_diff>
--- a/MDI-To-EDRS-Template.xlsx
+++ b/MDI-To-EDRS-Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20405"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20412"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mriley7\workspace\raven-import-and-submit-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C671669-30A5-4663-937D-603704E65E52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7898B5E6-88BE-47E0-B5A5-E92A8B713263}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8490" xr2:uid="{7A50F290-1C75-487E-9806-F93553E4E7CC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8196" xr2:uid="{7A50F290-1C75-487E-9806-F93553E4E7CC}"/>
   </bookViews>
   <sheets>
     <sheet name="MDI RAVEN Input Schema" sheetId="4" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="178">
   <si>
     <t>Manner of Death</t>
   </si>
@@ -124,9 +124,6 @@
     <t>Cause And Manner of Death</t>
   </si>
   <si>
-    <t>Medical Examiner Name</t>
-  </si>
-  <si>
     <t>Medical Examiner Office: Street</t>
   </si>
   <si>
@@ -299,12 +296,6 @@
   </si>
   <si>
     <t>Death in nursing home or long term care facility</t>
-  </si>
-  <si>
-    <t>Medical Examiner Phone Number</t>
-  </si>
-  <si>
-    <t>Medical Examiner License Number</t>
   </si>
   <si>
     <t>End of Cases</t>
@@ -530,25 +521,6 @@
     <t>This section describes the autopsy findings, if an autopsy occurred.</t>
   </si>
   <si>
-    <t>This section describes the primary Chief Medical Examiner or Coroner associated to the case.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name of the Medical Examiner.
-Accepted Formats:
-&lt;First Name&gt; &lt;Last Name&gt;
-&lt;First Name&gt; &lt;Middle Initial&gt; &lt;Last Name&gt;
-&lt;First Name&gt; &lt;Middle Name&gt; &lt;Last Name&gt;
-</t>
-  </si>
-  <si>
-    <t>Phone number of the office of the Medical Examiner, or primary contact number
-Accepted Formats:
-###-###-####</t>
-  </si>
-  <si>
-    <t>Medical Examiner License Number associated to the juridiction in which the case is owned.</t>
-  </si>
-  <si>
     <t>Primary Address of the medical examiner's office or primary address. Multiple lines are supported.</t>
   </si>
   <si>
@@ -576,9 +548,6 @@
   </si>
   <si>
     <t>Pregnant</t>
-  </si>
-  <si>
-    <t>Not pregnant within past year</t>
   </si>
   <si>
     <t>Pregnant at time of death</t>
@@ -652,48 +621,58 @@
     </r>
   </si>
   <si>
-    <t>INVALID</t>
-  </si>
-  <si>
     <t>Death Pronouncement</t>
   </si>
   <si>
-    <t>Death Certifier</t>
+    <t>Autopsy Performed Office Name</t>
+  </si>
+  <si>
+    <t>Name of the office in which the autopsy took place</t>
   </si>
   <si>
     <t>Autopsy Performed Location: Street</t>
   </si>
   <si>
+    <t>Primary Address of the autopsy location. Multiple lines are supported.</t>
+  </si>
+  <si>
     <t>Autopsy Performed Location: City</t>
   </si>
   <si>
     <t>Autopsy Performed Location: County</t>
   </si>
   <si>
-    <t>Primary Address of the autopsy location. Multiple lines are supported.</t>
-  </si>
-  <si>
     <t>Autopsy Performed Location: State, U.S. Territory or Canadian Province</t>
   </si>
   <si>
     <t>Autopsy Performed Location: Postal Code</t>
   </si>
   <si>
-    <t>Autopsy Performed Office Name</t>
-  </si>
-  <si>
-    <t>Name of the office in which the autopsy took place</t>
+    <t>Certifier Identifier</t>
+  </si>
+  <si>
+    <t>Certifier Identifier System</t>
+  </si>
+  <si>
+    <t>URN system that describes the type of identifier.
+Default: urn:mdi:raven:provideridentifier</t>
+  </si>
+  <si>
+    <t>Unique identifier assigned to the certifying medication examiner or coroner. This could include a medical license number, board certification number, or other official professional ID relevant to the jurisdiction</t>
+  </si>
+  <si>
+    <t>Not pregnant within the past year</t>
+  </si>
+  <si>
+    <t>XXX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
-    <numFmt numFmtId="167" formatCode="000\-00\-0000"/>
-    <numFmt numFmtId="168" formatCode="mm/dd/yy;@"/>
-    <numFmt numFmtId="170" formatCode="[$-409]h:mm:ss\ AM/PM;@"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -980,7 +959,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -1021,6 +1000,10 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="14" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -1059,6 +1042,14 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -1099,6 +1090,10 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
@@ -1106,10 +1101,18 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="14" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
@@ -1117,15 +1120,15 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyProtection="1">
@@ -1171,7 +1174,6 @@
     <xf numFmtId="0" fontId="7" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1202,12 +1204,13 @@
     <xf numFmtId="0" fontId="7" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="14" fontId="3" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -1228,6 +1231,10 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
@@ -1236,7 +1243,19 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="14" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -1285,9 +1304,6 @@
     <xf numFmtId="0" fontId="9" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1297,9 +1313,6 @@
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1321,53 +1334,62 @@
     <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="14" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="14" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1402,10 +1424,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1705,74 +1723,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54CD1DC7-E143-4CF5-BEA9-4DABBAFFC7B0}">
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="22.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="21" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" style="46" customWidth="1"/>
-    <col min="2" max="2" width="64.42578125" style="58" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" style="66" customWidth="1"/>
-    <col min="4" max="8" width="32.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="27.33203125" style="52" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" style="64" customWidth="1"/>
+    <col min="3" max="3" width="38.44140625" style="71" customWidth="1"/>
+    <col min="4" max="8" width="32.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.5">
+      <c r="A1" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="64" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="71" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="23.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C2" s="71" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="66" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="36.75" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C2" s="66" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="120" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="46" t="s">
-        <v>169</v>
-      </c>
-      <c r="B3" s="109" t="s">
-        <v>171</v>
-      </c>
-      <c r="C3" s="110" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="4" customFormat="1" ht="36.75" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="47" t="s">
+    </row>
+    <row r="3" spans="1:9" ht="109.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="52" t="s">
+        <v>161</v>
+      </c>
+      <c r="B3" s="116" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" s="117" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="4" customFormat="1" ht="34.799999999999997" thickTop="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="59"/>
-      <c r="C4" s="88" t="s">
-        <v>101</v>
+      <c r="B4" s="65"/>
+      <c r="C4" s="97" t="s">
+        <v>98</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -1781,43 +1799,43 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.45">
-      <c r="A5" s="48"/>
-      <c r="B5" s="106" t="s">
+    <row r="5" spans="1:9" s="6" customFormat="1" ht="29.4" x14ac:dyDescent="0.5">
+      <c r="A5" s="54"/>
+      <c r="B5" s="113" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="98" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" s="6" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A6" s="54"/>
+      <c r="B6" s="114" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="89" t="s">
+      <c r="C6" s="98" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" s="8" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A7" s="55" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="66"/>
+      <c r="C7" s="99" t="s">
         <v>102</v>
-      </c>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="5"/>
-    </row>
-    <row r="6" spans="1:9" s="6" customFormat="1" ht="48" x14ac:dyDescent="0.45">
-      <c r="A6" s="48"/>
-      <c r="B6" s="107" t="s">
-        <v>80</v>
-      </c>
-      <c r="C6" s="89" t="s">
-        <v>103</v>
-      </c>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="5"/>
-    </row>
-    <row r="7" spans="1:9" s="8" customFormat="1" ht="36" x14ac:dyDescent="0.45">
-      <c r="A7" s="49" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="60"/>
-      <c r="C7" s="90" t="s">
-        <v>105</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
@@ -1826,893 +1844,877 @@
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:9" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.45">
-      <c r="A8" s="50"/>
-      <c r="B8" s="67" t="s">
+    <row r="8" spans="1:9" s="11" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
+      <c r="A8" s="56"/>
+      <c r="B8" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="91" t="s">
-        <v>104</v>
-      </c>
-      <c r="D8" s="13"/>
+      <c r="C8" s="100" t="s">
+        <v>101</v>
+      </c>
+      <c r="D8" s="14"/>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
       <c r="I8" s="10"/>
     </row>
-    <row r="9" spans="1:9" s="11" customFormat="1" ht="60" x14ac:dyDescent="0.45">
-      <c r="A9" s="50"/>
-      <c r="B9" s="67" t="s">
+    <row r="9" spans="1:9" s="11" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A9" s="56"/>
+      <c r="B9" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="91" t="s">
-        <v>108</v>
-      </c>
-      <c r="D9" s="13"/>
+      <c r="C9" s="100" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9" s="14"/>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
       <c r="I9" s="10"/>
     </row>
-    <row r="10" spans="1:9" s="11" customFormat="1" ht="24" x14ac:dyDescent="0.45">
-      <c r="A10" s="50"/>
-      <c r="B10" s="67" t="s">
+    <row r="10" spans="1:9" s="11" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A10" s="56"/>
+      <c r="B10" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="91" t="s">
-        <v>107</v>
-      </c>
-      <c r="D10" s="13"/>
+      <c r="C10" s="100" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="14"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
       <c r="I10" s="10"/>
     </row>
-    <row r="11" spans="1:9" s="11" customFormat="1" ht="36" x14ac:dyDescent="0.45">
-      <c r="A11" s="50"/>
-      <c r="B11" s="68" t="s">
-        <v>76</v>
-      </c>
-      <c r="C11" s="91" t="s">
-        <v>106</v>
-      </c>
-      <c r="D11" s="13"/>
+    <row r="11" spans="1:9" s="11" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A11" s="56"/>
+      <c r="B11" s="73" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="100" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11" s="14"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
       <c r="I11" s="10"/>
     </row>
-    <row r="12" spans="1:9" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.45">
-      <c r="A12" s="50"/>
-      <c r="B12" s="67" t="s">
+    <row r="12" spans="1:9" s="11" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A12" s="56"/>
+      <c r="B12" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="91" t="s">
-        <v>155</v>
-      </c>
-      <c r="D12" s="112"/>
-      <c r="E12" s="113"/>
-      <c r="F12" s="113"/>
-      <c r="G12" s="113"/>
-      <c r="H12" s="113"/>
+      <c r="C12" s="100" t="s">
+        <v>148</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
       <c r="I12" s="10"/>
     </row>
-    <row r="13" spans="1:9" s="11" customFormat="1" ht="72" x14ac:dyDescent="0.45">
-      <c r="A13" s="50"/>
-      <c r="B13" s="67" t="s">
+    <row r="13" spans="1:9" s="11" customFormat="1" ht="57" x14ac:dyDescent="0.5">
+      <c r="A13" s="56"/>
+      <c r="B13" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="91" t="s">
-        <v>109</v>
-      </c>
-      <c r="D13" s="13"/>
+      <c r="C13" s="100" t="s">
+        <v>106</v>
+      </c>
+      <c r="D13" s="14"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="I13" s="10"/>
     </row>
-    <row r="14" spans="1:9" s="11" customFormat="1" ht="48" x14ac:dyDescent="0.45">
-      <c r="A14" s="50"/>
-      <c r="B14" s="67" t="s">
+    <row r="14" spans="1:9" s="11" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A14" s="56"/>
+      <c r="B14" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="91" t="s">
-        <v>110</v>
-      </c>
-      <c r="D14" s="114"/>
-      <c r="E14" s="115"/>
-      <c r="F14" s="115"/>
-      <c r="G14" s="115"/>
-      <c r="H14" s="115"/>
+      <c r="C14" s="100" t="s">
+        <v>107</v>
+      </c>
+      <c r="D14" s="82"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
       <c r="I14" s="10"/>
     </row>
-    <row r="15" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="50"/>
-      <c r="B15" s="67" t="s">
+    <row r="15" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="56"/>
+      <c r="B15" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="91"/>
-      <c r="D15" s="13"/>
+      <c r="C15" s="100"/>
+      <c r="D15" s="14"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
       <c r="I15" s="10"/>
     </row>
-    <row r="16" spans="1:9" s="11" customFormat="1" ht="24" x14ac:dyDescent="0.45">
-      <c r="A16" s="50"/>
-      <c r="B16" s="67" t="s">
+    <row r="16" spans="1:9" s="11" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A16" s="56"/>
+      <c r="B16" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="91" t="s">
-        <v>111</v>
-      </c>
-      <c r="D16" s="78"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
+      <c r="C16" s="100" t="s">
+        <v>108</v>
+      </c>
+      <c r="D16" s="83"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="9"/>
       <c r="H16" s="9"/>
       <c r="I16" s="10"/>
     </row>
-    <row r="17" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="50"/>
-      <c r="B17" s="67" t="s">
+    <row r="17" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="56"/>
+      <c r="B17" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="91"/>
-      <c r="D17" s="13"/>
+      <c r="C17" s="100"/>
+      <c r="D17" s="14"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
       <c r="I17" s="10"/>
     </row>
-    <row r="18" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="50"/>
-      <c r="B18" s="67" t="s">
-        <v>99</v>
-      </c>
-      <c r="C18" s="91"/>
-      <c r="D18" s="13"/>
+    <row r="18" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="56"/>
+      <c r="B18" s="72" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18" s="100"/>
+      <c r="D18" s="14"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
       <c r="I18" s="10"/>
     </row>
-    <row r="19" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="50"/>
-      <c r="B19" s="69" t="s">
+    <row r="19" spans="1:9" s="11" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
+      <c r="A19" s="56"/>
+      <c r="B19" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="91"/>
-      <c r="D19" s="13"/>
+      <c r="C19" s="100"/>
+      <c r="D19" s="14"/>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
       <c r="I19" s="10"/>
     </row>
-    <row r="20" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="50"/>
-      <c r="B20" s="67" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="91"/>
-      <c r="D20" s="13"/>
+    <row r="20" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A20" s="56"/>
+      <c r="B20" s="72" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="100"/>
+      <c r="D20" s="14"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
       <c r="I20" s="10"/>
     </row>
-    <row r="21" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="50"/>
-      <c r="B21" s="67" t="s">
+    <row r="21" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A21" s="56"/>
+      <c r="B21" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="91"/>
-      <c r="D21" s="13"/>
+      <c r="C21" s="100"/>
+      <c r="D21" s="14"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
       <c r="I21" s="10"/>
     </row>
-    <row r="22" spans="1:9" s="15" customFormat="1" ht="84" x14ac:dyDescent="0.45">
-      <c r="A22" s="102" t="s">
+    <row r="22" spans="1:9" s="16" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
+      <c r="A22" s="110" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="61"/>
-      <c r="C22" s="92" t="s">
+      <c r="B22" s="67"/>
+      <c r="C22" s="101" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+    </row>
+    <row r="23" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A23" s="57"/>
+      <c r="B23" s="115" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="102" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" s="119"/>
+      <c r="E23" s="120"/>
+      <c r="F23" s="120"/>
+      <c r="G23" s="120"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="18"/>
+    </row>
+    <row r="24" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A24" s="57"/>
+      <c r="B24" s="115" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="102" t="s">
+        <v>111</v>
+      </c>
+      <c r="D24" s="85"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="121"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="18"/>
+    </row>
+    <row r="25" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A25" s="57"/>
+      <c r="B25" s="115" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="102" t="s">
         <v>112</v>
       </c>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-    </row>
-    <row r="23" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="51"/>
-      <c r="B23" s="108" t="s">
-        <v>2</v>
-      </c>
-      <c r="C23" s="93" t="s">
+      <c r="D25" s="86"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="18"/>
+    </row>
+    <row r="26" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A26" s="57"/>
+      <c r="B26" s="115" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" s="102" t="s">
         <v>113</v>
       </c>
-      <c r="D23" s="79"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="17"/>
-    </row>
-    <row r="24" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="51"/>
-      <c r="B24" s="108" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="93" t="s">
+      <c r="D26" s="86"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="18"/>
+    </row>
+    <row r="27" spans="1:9" s="19" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A27" s="57"/>
+      <c r="B27" s="115" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="102" t="s">
         <v>114</v>
       </c>
-      <c r="D24" s="80"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="17"/>
-    </row>
-    <row r="25" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="51"/>
-      <c r="B25" s="108" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="93" t="s">
+      <c r="D27" s="86"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="18"/>
+    </row>
+    <row r="28" spans="1:9" s="19" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A28" s="57"/>
+      <c r="B28" s="115" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="102" t="s">
         <v>115</v>
       </c>
-      <c r="D25" s="81"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="17"/>
-    </row>
-    <row r="26" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="51"/>
-      <c r="B26" s="108" t="s">
-        <v>98</v>
-      </c>
-      <c r="C26" s="93" t="s">
+      <c r="D28" s="86"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="18"/>
+    </row>
+    <row r="29" spans="1:9" s="19" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A29" s="57"/>
+      <c r="B29" s="115" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="102" t="s">
         <v>116</v>
       </c>
-      <c r="D26" s="81"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="17"/>
-    </row>
-    <row r="27" spans="1:9" s="18" customFormat="1" ht="48" x14ac:dyDescent="0.45">
-      <c r="A27" s="51"/>
-      <c r="B27" s="108" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="93" t="s">
+      <c r="D29" s="86"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="18"/>
+    </row>
+    <row r="30" spans="1:9" s="19" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A30" s="57"/>
+      <c r="B30" s="115" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="102" t="s">
         <v>117</v>
       </c>
-      <c r="D27" s="81"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="17"/>
-    </row>
-    <row r="28" spans="1:9" s="18" customFormat="1" ht="48" x14ac:dyDescent="0.45">
-      <c r="A28" s="51"/>
-      <c r="B28" s="108" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="93" t="s">
+      <c r="D30" s="84"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="18"/>
+    </row>
+    <row r="31" spans="1:9" s="19" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A31" s="57"/>
+      <c r="B31" s="115" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="102" t="s">
         <v>118</v>
       </c>
-      <c r="D28" s="81"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="17"/>
-    </row>
-    <row r="29" spans="1:9" s="18" customFormat="1" ht="48" x14ac:dyDescent="0.45">
-      <c r="A29" s="51"/>
-      <c r="B29" s="108" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="93" t="s">
+      <c r="D31" s="86"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="18"/>
+    </row>
+    <row r="32" spans="1:9" s="19" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A32" s="57"/>
+      <c r="B32" s="75" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="102" t="s">
         <v>119</v>
       </c>
-      <c r="D29" s="81"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="17"/>
-    </row>
-    <row r="30" spans="1:9" s="18" customFormat="1" ht="48" x14ac:dyDescent="0.45">
-      <c r="A30" s="51"/>
-      <c r="B30" s="108" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="93" t="s">
+      <c r="D32" s="87"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="18"/>
+    </row>
+    <row r="33" spans="1:9" s="19" customFormat="1" ht="57" x14ac:dyDescent="0.5">
+      <c r="A33" s="57"/>
+      <c r="B33" s="75" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="102" t="s">
         <v>120</v>
       </c>
-      <c r="D30" s="79"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="17"/>
-    </row>
-    <row r="31" spans="1:9" s="18" customFormat="1" ht="48" x14ac:dyDescent="0.45">
-      <c r="A31" s="51"/>
-      <c r="B31" s="108" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" s="93" t="s">
+      <c r="D33" s="88"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="18"/>
+    </row>
+    <row r="34" spans="1:9" s="19" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
+      <c r="A34" s="57"/>
+      <c r="B34" s="75" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" s="102" t="s">
         <v>121</v>
       </c>
-      <c r="D31" s="82"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="17"/>
-    </row>
-    <row r="32" spans="1:9" s="18" customFormat="1" ht="24" x14ac:dyDescent="0.45">
-      <c r="A32" s="51"/>
-      <c r="B32" s="70" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" s="93" t="s">
+      <c r="D34" s="122"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="123"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="18"/>
+    </row>
+    <row r="35" spans="1:9" s="26" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A35" s="58"/>
+      <c r="B35" s="75" t="s">
+        <v>81</v>
+      </c>
+      <c r="C35" s="102" t="s">
         <v>122</v>
       </c>
-      <c r="D32" s="82"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="17"/>
-    </row>
-    <row r="33" spans="1:9" s="18" customFormat="1" ht="60" x14ac:dyDescent="0.45">
-      <c r="A33" s="51"/>
-      <c r="B33" s="70" t="s">
+      <c r="D35" s="86"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="25"/>
+    </row>
+    <row r="36" spans="1:9" s="19" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A36" s="57"/>
+      <c r="B36" s="75" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="93" t="s">
+      <c r="C36" s="102" t="s">
         <v>123</v>
       </c>
-      <c r="D33" s="116"/>
-      <c r="E33" s="117"/>
-      <c r="F33" s="117"/>
-      <c r="G33" s="117"/>
-      <c r="H33" s="117"/>
-      <c r="I33" s="17"/>
-    </row>
-    <row r="34" spans="1:9" s="18" customFormat="1" ht="84" x14ac:dyDescent="0.45">
-      <c r="A34" s="51"/>
-      <c r="B34" s="70" t="s">
-        <v>83</v>
-      </c>
-      <c r="C34" s="93" t="s">
+      <c r="D36" s="87"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="18"/>
+    </row>
+    <row r="37" spans="1:9" s="19" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A37" s="57"/>
+      <c r="B37" s="75" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" s="102" t="s">
         <v>124</v>
       </c>
-      <c r="D34" s="118"/>
-      <c r="E34" s="119"/>
-      <c r="F34" s="119"/>
-      <c r="G34" s="119"/>
-      <c r="H34" s="119"/>
-      <c r="I34" s="17"/>
-    </row>
-    <row r="35" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="52"/>
-      <c r="B35" s="70" t="s">
-        <v>82</v>
-      </c>
-      <c r="C35" s="93" t="s">
+      <c r="D37" s="87"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="18"/>
+    </row>
+    <row r="38" spans="1:9" s="28" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
+      <c r="A38" s="111" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="68"/>
+      <c r="C38" s="103" t="s">
+        <v>140</v>
+      </c>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="27"/>
+    </row>
+    <row r="39" spans="1:9" s="31" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A39" s="59"/>
+      <c r="B39" s="76" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" s="104" t="s">
         <v>125</v>
       </c>
-      <c r="D35" s="81"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="20"/>
-      <c r="I35" s="22"/>
-    </row>
-    <row r="36" spans="1:9" s="18" customFormat="1" ht="36" x14ac:dyDescent="0.45">
-      <c r="A36" s="51"/>
-      <c r="B36" s="70" t="s">
-        <v>42</v>
-      </c>
-      <c r="C36" s="93" t="s">
+      <c r="D39" s="89"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="29"/>
+      <c r="G39" s="29"/>
+      <c r="H39" s="29"/>
+      <c r="I39" s="30"/>
+    </row>
+    <row r="40" spans="1:9" s="31" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A40" s="59"/>
+      <c r="B40" s="77" t="s">
+        <v>93</v>
+      </c>
+      <c r="C40" s="104" t="s">
+        <v>158</v>
+      </c>
+      <c r="D40" s="89"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="32"/>
+      <c r="I40" s="30"/>
+    </row>
+    <row r="41" spans="1:9" s="31" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A41" s="59"/>
+      <c r="B41" s="76" t="s">
+        <v>76</v>
+      </c>
+      <c r="C41" s="104" t="s">
         <v>126</v>
       </c>
-      <c r="D36" s="82"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="21"/>
-      <c r="I36" s="17"/>
-    </row>
-    <row r="37" spans="1:9" s="18" customFormat="1" ht="36" x14ac:dyDescent="0.45">
-      <c r="A37" s="51"/>
-      <c r="B37" s="70" t="s">
+      <c r="D41" s="89"/>
+      <c r="E41" s="89"/>
+      <c r="F41" s="89"/>
+      <c r="G41" s="89"/>
+      <c r="H41" s="89"/>
+      <c r="I41" s="30"/>
+    </row>
+    <row r="42" spans="1:9" s="31" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A42" s="59"/>
+      <c r="B42" s="112" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="104" t="s">
+        <v>127</v>
+      </c>
+      <c r="D42" s="89"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="29"/>
+      <c r="G42" s="29"/>
+      <c r="H42" s="29"/>
+      <c r="I42" s="30"/>
+    </row>
+    <row r="43" spans="1:9" s="35" customFormat="1" ht="57" x14ac:dyDescent="0.5">
+      <c r="A43" s="118" t="s">
+        <v>163</v>
+      </c>
+      <c r="B43" s="69"/>
+      <c r="C43" s="105" t="s">
+        <v>141</v>
+      </c>
+      <c r="D43" s="90"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="33"/>
+      <c r="G43" s="33"/>
+      <c r="H43" s="33"/>
+      <c r="I43" s="34"/>
+    </row>
+    <row r="44" spans="1:9" s="38" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A44" s="60"/>
+      <c r="B44" s="78" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" s="106" t="s">
+        <v>128</v>
+      </c>
+      <c r="D44" s="91"/>
+      <c r="E44" s="36"/>
+      <c r="F44" s="36"/>
+      <c r="G44" s="36"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="37"/>
+    </row>
+    <row r="45" spans="1:9" s="38" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
+      <c r="A45" s="60"/>
+      <c r="B45" s="78" t="s">
+        <v>22</v>
+      </c>
+      <c r="C45" s="106" t="s">
+        <v>129</v>
+      </c>
+      <c r="D45" s="92"/>
+      <c r="E45" s="39"/>
+      <c r="F45" s="39"/>
+      <c r="G45" s="39"/>
+      <c r="H45" s="39"/>
+      <c r="I45" s="37"/>
+    </row>
+    <row r="46" spans="1:9" s="38" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A46" s="60"/>
+      <c r="B46" s="78" t="s">
+        <v>77</v>
+      </c>
+      <c r="C46" s="106" t="s">
+        <v>134</v>
+      </c>
+      <c r="D46" s="93"/>
+      <c r="E46" s="40"/>
+      <c r="F46" s="40"/>
+      <c r="G46" s="40"/>
+      <c r="H46" s="40"/>
+      <c r="I46" s="37"/>
+    </row>
+    <row r="47" spans="1:9" s="38" customFormat="1" ht="57" x14ac:dyDescent="0.5">
+      <c r="A47" s="60"/>
+      <c r="B47" s="78" t="s">
+        <v>23</v>
+      </c>
+      <c r="C47" s="106" t="s">
+        <v>135</v>
+      </c>
+      <c r="D47" s="94"/>
+      <c r="E47" s="41"/>
+      <c r="F47" s="41"/>
+      <c r="G47" s="41"/>
+      <c r="H47" s="41"/>
+      <c r="I47" s="37"/>
+    </row>
+    <row r="48" spans="1:9" s="38" customFormat="1" ht="91.2" x14ac:dyDescent="0.5">
+      <c r="A48" s="60"/>
+      <c r="B48" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="C48" s="106" t="s">
+        <v>136</v>
+      </c>
+      <c r="D48" s="92"/>
+      <c r="E48" s="39"/>
+      <c r="F48" s="39"/>
+      <c r="G48" s="39"/>
+      <c r="H48" s="39"/>
+      <c r="I48" s="37"/>
+    </row>
+    <row r="49" spans="1:9" s="38" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A49" s="60"/>
+      <c r="B49" s="78" t="s">
+        <v>39</v>
+      </c>
+      <c r="C49" s="106" t="s">
+        <v>137</v>
+      </c>
+      <c r="D49" s="40"/>
+      <c r="E49" s="40"/>
+      <c r="F49" s="40"/>
+      <c r="G49" s="40"/>
+      <c r="H49" s="40"/>
+      <c r="I49" s="37"/>
+    </row>
+    <row r="50" spans="1:9" s="43" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A50" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="C37" s="93" t="s">
-        <v>127</v>
-      </c>
-      <c r="D37" s="82"/>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
-      <c r="G37" s="21"/>
-      <c r="H37" s="21"/>
-      <c r="I37" s="17"/>
-    </row>
-    <row r="38" spans="1:9" s="25" customFormat="1" ht="84" x14ac:dyDescent="0.45">
-      <c r="A38" s="103" t="s">
-        <v>30</v>
-      </c>
-      <c r="B38" s="62"/>
-      <c r="C38" s="94" t="s">
+      <c r="B50" s="70"/>
+      <c r="C50" s="107" t="s">
+        <v>142</v>
+      </c>
+      <c r="D50" s="42"/>
+      <c r="E50" s="42"/>
+      <c r="F50" s="42"/>
+      <c r="G50" s="42"/>
+      <c r="H50" s="42"/>
+      <c r="I50" s="42"/>
+    </row>
+    <row r="51" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A51" s="62"/>
+      <c r="B51" s="79" t="s">
+        <v>44</v>
+      </c>
+      <c r="C51" s="108" t="s">
+        <v>138</v>
+      </c>
+      <c r="D51" s="95"/>
+      <c r="E51" s="44"/>
+      <c r="F51" s="44"/>
+      <c r="G51" s="44"/>
+      <c r="H51" s="44"/>
+      <c r="I51" s="45"/>
+    </row>
+    <row r="52" spans="1:9" s="46" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A52" s="62"/>
+      <c r="B52" s="79" t="s">
+        <v>80</v>
+      </c>
+      <c r="C52" s="108" t="s">
+        <v>139</v>
+      </c>
+      <c r="D52" s="95"/>
+      <c r="E52" s="44"/>
+      <c r="F52" s="44"/>
+      <c r="G52" s="44"/>
+      <c r="H52" s="44"/>
+      <c r="I52" s="45"/>
+    </row>
+    <row r="53" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A53" s="127"/>
+      <c r="B53" s="129" t="s">
+        <v>164</v>
+      </c>
+      <c r="C53" s="132" t="s">
+        <v>165</v>
+      </c>
+      <c r="D53" s="130"/>
+      <c r="E53" s="130"/>
+      <c r="F53" s="130"/>
+      <c r="G53" s="130"/>
+      <c r="H53" s="130"/>
+      <c r="I53" s="127"/>
+    </row>
+    <row r="54" spans="1:9" s="47" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A54" s="127"/>
+      <c r="B54" s="129" t="s">
+        <v>166</v>
+      </c>
+      <c r="C54" s="132" t="s">
+        <v>167</v>
+      </c>
+      <c r="D54" s="130"/>
+      <c r="E54" s="130"/>
+      <c r="F54" s="130"/>
+      <c r="G54" s="130"/>
+      <c r="H54" s="130"/>
+      <c r="I54" s="127"/>
+    </row>
+    <row r="55" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A55" s="127"/>
+      <c r="B55" s="129" t="s">
+        <v>168</v>
+      </c>
+      <c r="C55" s="132"/>
+      <c r="D55" s="130"/>
+      <c r="E55" s="130"/>
+      <c r="F55" s="130"/>
+      <c r="G55" s="130"/>
+      <c r="H55" s="130"/>
+      <c r="I55" s="127"/>
+    </row>
+    <row r="56" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A56" s="127"/>
+      <c r="B56" s="129" t="s">
+        <v>169</v>
+      </c>
+      <c r="C56" s="132"/>
+      <c r="D56" s="130"/>
+      <c r="E56" s="130"/>
+      <c r="F56" s="130"/>
+      <c r="G56" s="130"/>
+      <c r="H56" s="130"/>
+      <c r="I56" s="127"/>
+    </row>
+    <row r="57" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A57" s="127"/>
+      <c r="B57" s="129" t="s">
+        <v>170</v>
+      </c>
+      <c r="C57" s="132"/>
+      <c r="D57" s="130"/>
+      <c r="E57" s="130"/>
+      <c r="F57" s="130"/>
+      <c r="G57" s="130"/>
+      <c r="H57" s="130"/>
+      <c r="I57" s="127"/>
+    </row>
+    <row r="58" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A58" s="127"/>
+      <c r="B58" s="129" t="s">
+        <v>171</v>
+      </c>
+      <c r="C58" s="132"/>
+      <c r="D58" s="130"/>
+      <c r="E58" s="130"/>
+      <c r="F58" s="130"/>
+      <c r="G58" s="130"/>
+      <c r="H58" s="130"/>
+      <c r="I58" s="127"/>
+    </row>
+    <row r="59" spans="1:9" s="126" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A59" s="128"/>
+      <c r="B59" s="133" t="s">
+        <v>32</v>
+      </c>
+      <c r="C59" s="135" t="s">
         <v>143</v>
       </c>
-      <c r="D38" s="24"/>
-      <c r="E38" s="24"/>
-      <c r="F38" s="24"/>
-      <c r="G38" s="24"/>
-      <c r="H38" s="24"/>
-      <c r="I38" s="24"/>
-    </row>
-    <row r="39" spans="1:9" s="28" customFormat="1" ht="24" x14ac:dyDescent="0.45">
-      <c r="A39" s="53"/>
-      <c r="B39" s="71" t="s">
-        <v>39</v>
-      </c>
-      <c r="C39" s="95" t="s">
-        <v>128</v>
-      </c>
-      <c r="D39" s="83"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="26"/>
-      <c r="H39" s="26"/>
-      <c r="I39" s="27"/>
-    </row>
-    <row r="40" spans="1:9" s="28" customFormat="1" ht="24" x14ac:dyDescent="0.45">
-      <c r="A40" s="53"/>
-      <c r="B40" s="72" t="s">
-        <v>96</v>
-      </c>
-      <c r="C40" s="95" t="s">
-        <v>166</v>
-      </c>
-      <c r="D40" s="83"/>
-      <c r="E40" s="26"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="26"/>
-      <c r="H40" s="29"/>
-      <c r="I40" s="27"/>
-    </row>
-    <row r="41" spans="1:9" s="28" customFormat="1" ht="36" x14ac:dyDescent="0.45">
-      <c r="A41" s="53"/>
-      <c r="B41" s="71" t="s">
-        <v>77</v>
-      </c>
-      <c r="C41" s="95" t="s">
-        <v>129</v>
-      </c>
-      <c r="D41" s="83"/>
-      <c r="E41" s="83"/>
-      <c r="F41" s="83"/>
-      <c r="G41" s="83"/>
-      <c r="H41" s="83"/>
-      <c r="I41" s="27"/>
-    </row>
-    <row r="42" spans="1:9" s="28" customFormat="1" ht="36" x14ac:dyDescent="0.45">
-      <c r="A42" s="53"/>
-      <c r="B42" s="105" t="s">
-        <v>1</v>
-      </c>
-      <c r="C42" s="95" t="s">
-        <v>130</v>
-      </c>
-      <c r="D42" s="83"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="26"/>
-      <c r="H42" s="26"/>
-      <c r="I42" s="27"/>
-    </row>
-    <row r="43" spans="1:9" s="32" customFormat="1" ht="60" x14ac:dyDescent="0.45">
-      <c r="A43" s="111" t="s">
+      <c r="D59" s="131"/>
+      <c r="E59" s="134"/>
+      <c r="F59" s="134"/>
+      <c r="G59" s="134"/>
+      <c r="H59" s="124"/>
+      <c r="I59" s="125"/>
+    </row>
+    <row r="60" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A60" s="63"/>
+      <c r="B60" s="80" t="s">
+        <v>33</v>
+      </c>
+      <c r="C60" s="109"/>
+      <c r="D60" s="96"/>
+      <c r="E60" s="48"/>
+      <c r="F60" s="48"/>
+      <c r="G60" s="48"/>
+      <c r="H60" s="48"/>
+      <c r="I60" s="49"/>
+    </row>
+    <row r="61" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A61" s="63"/>
+      <c r="B61" s="80" t="s">
+        <v>34</v>
+      </c>
+      <c r="C61" s="109"/>
+      <c r="D61" s="96"/>
+      <c r="E61" s="48"/>
+      <c r="F61" s="48"/>
+      <c r="G61" s="48"/>
+      <c r="H61" s="48"/>
+      <c r="I61" s="49"/>
+    </row>
+    <row r="62" spans="1:9" s="50" customFormat="1" ht="39.6" x14ac:dyDescent="0.5">
+      <c r="A62" s="63"/>
+      <c r="B62" s="81" t="s">
+        <v>35</v>
+      </c>
+      <c r="C62" s="109"/>
+      <c r="D62" s="96"/>
+      <c r="E62" s="48"/>
+      <c r="F62" s="48"/>
+      <c r="G62" s="48"/>
+      <c r="H62" s="48"/>
+      <c r="I62" s="49"/>
+    </row>
+    <row r="63" spans="1:9" s="50" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
+      <c r="A63" s="63"/>
+      <c r="B63" s="81" t="s">
+        <v>36</v>
+      </c>
+      <c r="C63" s="109"/>
+      <c r="D63" s="96"/>
+      <c r="E63" s="48"/>
+      <c r="F63" s="48"/>
+      <c r="G63" s="48"/>
+      <c r="H63" s="48"/>
+      <c r="I63" s="49"/>
+    </row>
+    <row r="64" spans="1:9" s="50" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
+      <c r="A64" s="63"/>
+      <c r="B64" s="80" t="s">
+        <v>91</v>
+      </c>
+      <c r="C64" s="109" t="s">
+        <v>144</v>
+      </c>
+      <c r="D64" s="96"/>
+      <c r="E64" s="48"/>
+      <c r="F64" s="48"/>
+      <c r="G64" s="48"/>
+      <c r="H64" s="48"/>
+      <c r="I64" s="49"/>
+    </row>
+    <row r="65" spans="1:9" s="126" customFormat="1" ht="57" x14ac:dyDescent="0.5">
+      <c r="A65" s="128"/>
+      <c r="B65" s="133" t="s">
         <v>172</v>
       </c>
-      <c r="B43" s="63"/>
-      <c r="C43" s="96" t="s">
-        <v>144</v>
-      </c>
-      <c r="D43" s="84"/>
-      <c r="E43" s="30"/>
-      <c r="F43" s="30"/>
-      <c r="G43" s="30"/>
-      <c r="H43" s="30"/>
-      <c r="I43" s="31"/>
-    </row>
-    <row r="44" spans="1:9" s="34" customFormat="1" ht="48" x14ac:dyDescent="0.45">
-      <c r="A44" s="54"/>
-      <c r="B44" s="73" t="s">
-        <v>21</v>
-      </c>
-      <c r="C44" s="97" t="s">
-        <v>131</v>
-      </c>
-      <c r="D44" s="120"/>
-      <c r="E44" s="121"/>
-      <c r="F44" s="121"/>
-      <c r="G44" s="121"/>
-      <c r="H44" s="121"/>
-      <c r="I44" s="33"/>
-    </row>
-    <row r="45" spans="1:9" s="34" customFormat="1" ht="84" x14ac:dyDescent="0.45">
-      <c r="A45" s="54"/>
-      <c r="B45" s="73" t="s">
-        <v>22</v>
-      </c>
-      <c r="C45" s="97" t="s">
-        <v>132</v>
-      </c>
-      <c r="D45" s="122"/>
-      <c r="E45" s="123"/>
-      <c r="F45" s="123"/>
-      <c r="G45" s="123"/>
-      <c r="H45" s="123"/>
-      <c r="I45" s="33"/>
-    </row>
-    <row r="46" spans="1:9" s="34" customFormat="1" ht="36" x14ac:dyDescent="0.45">
-      <c r="A46" s="54"/>
-      <c r="B46" s="73" t="s">
-        <v>78</v>
-      </c>
-      <c r="C46" s="97" t="s">
-        <v>137</v>
-      </c>
-      <c r="D46" s="85"/>
-      <c r="E46" s="35"/>
-      <c r="F46" s="35"/>
-      <c r="G46" s="35"/>
-      <c r="H46" s="35"/>
-      <c r="I46" s="33"/>
-    </row>
-    <row r="47" spans="1:9" s="34" customFormat="1" ht="60" x14ac:dyDescent="0.45">
-      <c r="A47" s="54"/>
-      <c r="B47" s="73" t="s">
-        <v>23</v>
-      </c>
-      <c r="C47" s="97" t="s">
-        <v>138</v>
-      </c>
-      <c r="D47" s="120"/>
-      <c r="E47" s="121"/>
-      <c r="F47" s="121"/>
-      <c r="G47" s="121"/>
-      <c r="H47" s="121"/>
-      <c r="I47" s="33"/>
-    </row>
-    <row r="48" spans="1:9" s="34" customFormat="1" ht="96" x14ac:dyDescent="0.45">
-      <c r="A48" s="54"/>
-      <c r="B48" s="73" t="s">
-        <v>24</v>
-      </c>
-      <c r="C48" s="97" t="s">
-        <v>139</v>
-      </c>
-      <c r="D48" s="122"/>
-      <c r="E48" s="123"/>
-      <c r="F48" s="123"/>
-      <c r="G48" s="123"/>
-      <c r="H48" s="123"/>
-      <c r="I48" s="33"/>
-    </row>
-    <row r="49" spans="1:9" s="34" customFormat="1" ht="36" x14ac:dyDescent="0.45">
-      <c r="A49" s="54"/>
-      <c r="B49" s="73" t="s">
-        <v>40</v>
-      </c>
-      <c r="C49" s="97" t="s">
-        <v>140</v>
-      </c>
-      <c r="D49" s="85"/>
-      <c r="E49" s="35"/>
-      <c r="F49" s="35"/>
-      <c r="G49" s="35"/>
-      <c r="H49" s="35"/>
-      <c r="I49" s="33"/>
-    </row>
-    <row r="50" spans="1:9" s="37" customFormat="1" ht="24" x14ac:dyDescent="0.45">
-      <c r="A50" s="55" t="s">
-        <v>44</v>
-      </c>
-      <c r="B50" s="64"/>
-      <c r="C50" s="98" t="s">
-        <v>145</v>
-      </c>
-      <c r="D50" s="36"/>
-      <c r="E50" s="36"/>
-      <c r="F50" s="36"/>
-      <c r="G50" s="36"/>
-      <c r="H50" s="36"/>
-      <c r="I50" s="36"/>
-    </row>
-    <row r="51" spans="1:9" s="39" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="56"/>
-      <c r="B51" s="74" t="s">
-        <v>45</v>
-      </c>
-      <c r="C51" s="99" t="s">
-        <v>141</v>
-      </c>
-      <c r="D51" s="86"/>
-      <c r="E51" s="86"/>
-      <c r="F51" s="86"/>
-      <c r="G51" s="86"/>
-      <c r="H51" s="86"/>
-      <c r="I51" s="38"/>
-    </row>
-    <row r="52" spans="1:9" s="56" customFormat="1" ht="36" x14ac:dyDescent="0.45">
-      <c r="B52" s="74" t="s">
-        <v>81</v>
-      </c>
-      <c r="C52" s="99" t="s">
-        <v>142</v>
-      </c>
-      <c r="D52" s="86"/>
-      <c r="E52" s="86"/>
-      <c r="F52" s="86"/>
-      <c r="G52" s="86"/>
-      <c r="H52" s="86"/>
-    </row>
-    <row r="53" spans="1:9" s="56" customFormat="1" ht="24" x14ac:dyDescent="0.45">
-      <c r="B53" s="74" t="s">
-        <v>180</v>
-      </c>
-      <c r="C53" s="99" t="s">
-        <v>181</v>
-      </c>
-      <c r="D53" s="86"/>
-      <c r="E53" s="86"/>
-      <c r="F53" s="86"/>
-      <c r="G53" s="86"/>
-      <c r="H53" s="86"/>
-    </row>
-    <row r="54" spans="1:9" s="56" customFormat="1" ht="24" x14ac:dyDescent="0.45">
-      <c r="B54" s="74" t="s">
+      <c r="C65" s="135" t="s">
+        <v>175</v>
+      </c>
+      <c r="D65" s="134"/>
+      <c r="E65" s="124"/>
+      <c r="F65" s="124"/>
+      <c r="G65" s="124"/>
+      <c r="H65" s="124"/>
+      <c r="I65" s="125"/>
+    </row>
+    <row r="66" spans="1:9" s="126" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A66" s="128"/>
+      <c r="B66" s="133" t="s">
+        <v>173</v>
+      </c>
+      <c r="C66" s="135" t="s">
         <v>174</v>
       </c>
-      <c r="C54" s="99" t="s">
-        <v>177</v>
-      </c>
-      <c r="D54" s="86"/>
-      <c r="E54" s="86"/>
-      <c r="F54" s="86"/>
-      <c r="G54" s="86"/>
-      <c r="H54" s="86"/>
-    </row>
-    <row r="55" spans="1:9" s="56" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B55" s="74" t="s">
-        <v>175</v>
-      </c>
-      <c r="C55" s="99"/>
-      <c r="D55" s="86"/>
-      <c r="E55" s="86"/>
-      <c r="F55" s="86"/>
-      <c r="G55" s="86"/>
-      <c r="H55" s="86"/>
-    </row>
-    <row r="56" spans="1:9" s="56" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B56" s="74" t="s">
-        <v>176</v>
-      </c>
-      <c r="C56" s="99"/>
-      <c r="D56" s="86"/>
-      <c r="E56" s="86"/>
-      <c r="F56" s="86"/>
-      <c r="G56" s="86"/>
-      <c r="H56" s="86"/>
-    </row>
-    <row r="57" spans="1:9" s="56" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B57" s="74" t="s">
-        <v>178</v>
-      </c>
-      <c r="C57" s="99"/>
-      <c r="D57" s="86"/>
-      <c r="E57" s="86"/>
-      <c r="F57" s="86"/>
-      <c r="G57" s="86"/>
-      <c r="H57" s="86"/>
-    </row>
-    <row r="58" spans="1:9" s="56" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B58" s="74" t="s">
-        <v>179</v>
-      </c>
-      <c r="C58" s="99"/>
-      <c r="D58" s="86"/>
-      <c r="E58" s="86"/>
-      <c r="F58" s="86"/>
-      <c r="G58" s="86"/>
-      <c r="H58" s="86"/>
-    </row>
-    <row r="59" spans="1:9" s="41" customFormat="1" ht="36" x14ac:dyDescent="0.45">
-      <c r="A59" s="104" t="s">
-        <v>173</v>
-      </c>
-      <c r="B59" s="65"/>
-      <c r="C59" s="100" t="s">
-        <v>146</v>
-      </c>
-      <c r="D59" s="40"/>
-      <c r="E59" s="40"/>
-      <c r="F59" s="40"/>
-      <c r="G59" s="40"/>
-      <c r="H59" s="40"/>
-      <c r="I59" s="40"/>
-    </row>
-    <row r="60" spans="1:9" s="44" customFormat="1" ht="72" x14ac:dyDescent="0.45">
-      <c r="A60" s="57"/>
-      <c r="B60" s="75" t="s">
-        <v>32</v>
-      </c>
-      <c r="C60" s="101" t="s">
-        <v>147</v>
-      </c>
-      <c r="D60" s="87"/>
-      <c r="E60" s="42"/>
-      <c r="F60" s="42"/>
-      <c r="G60" s="42"/>
-      <c r="H60" s="42"/>
-      <c r="I60" s="43"/>
-    </row>
-    <row r="61" spans="1:9" s="44" customFormat="1" ht="48" x14ac:dyDescent="0.45">
-      <c r="A61" s="57"/>
-      <c r="B61" s="76" t="s">
-        <v>91</v>
-      </c>
-      <c r="C61" s="101" t="s">
-        <v>148</v>
-      </c>
-      <c r="D61" s="87"/>
-      <c r="E61" s="42"/>
-      <c r="F61" s="42"/>
-      <c r="G61" s="42"/>
-      <c r="H61" s="42"/>
-      <c r="I61" s="43"/>
-    </row>
-    <row r="62" spans="1:9" s="44" customFormat="1" ht="36" x14ac:dyDescent="0.45">
-      <c r="A62" s="57"/>
-      <c r="B62" s="75" t="s">
+      <c r="D66" s="134"/>
+      <c r="E66" s="124"/>
+      <c r="F66" s="124"/>
+      <c r="G66" s="124"/>
+      <c r="H66" s="124"/>
+      <c r="I66" s="125"/>
+    </row>
+    <row r="67" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A67" s="63"/>
+      <c r="B67" s="80" t="s">
         <v>92</v>
       </c>
-      <c r="C62" s="101" t="s">
-        <v>149</v>
-      </c>
-      <c r="D62" s="87"/>
-      <c r="E62" s="42"/>
-      <c r="F62" s="42"/>
-      <c r="G62" s="42"/>
-      <c r="H62" s="42"/>
-      <c r="I62" s="43"/>
-    </row>
-    <row r="63" spans="1:9" s="44" customFormat="1" ht="36" x14ac:dyDescent="0.45">
-      <c r="A63" s="57"/>
-      <c r="B63" s="75" t="s">
-        <v>33</v>
-      </c>
-      <c r="C63" s="101" t="s">
-        <v>150</v>
-      </c>
-      <c r="D63" s="87"/>
-      <c r="E63" s="42"/>
-      <c r="F63" s="42"/>
-      <c r="G63" s="42"/>
-      <c r="H63" s="42"/>
-      <c r="I63" s="43"/>
-    </row>
-    <row r="64" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A64" s="57"/>
-      <c r="B64" s="75" t="s">
-        <v>34</v>
-      </c>
-      <c r="C64" s="101"/>
-      <c r="D64" s="87"/>
-      <c r="E64" s="42"/>
-      <c r="F64" s="42"/>
-      <c r="G64" s="42"/>
-      <c r="H64" s="42"/>
-      <c r="I64" s="43"/>
-    </row>
-    <row r="65" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A65" s="57"/>
-      <c r="B65" s="75" t="s">
-        <v>35</v>
-      </c>
-      <c r="C65" s="101"/>
-      <c r="D65" s="87"/>
-      <c r="E65" s="42"/>
-      <c r="F65" s="42"/>
-      <c r="G65" s="42"/>
-      <c r="H65" s="42"/>
-      <c r="I65" s="43"/>
-    </row>
-    <row r="66" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A66" s="57"/>
-      <c r="B66" s="77" t="s">
-        <v>36</v>
-      </c>
-      <c r="C66" s="101"/>
-      <c r="D66" s="87"/>
-      <c r="E66" s="42"/>
-      <c r="F66" s="42"/>
-      <c r="G66" s="42"/>
-      <c r="H66" s="42"/>
-      <c r="I66" s="43"/>
-    </row>
-    <row r="67" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A67" s="57"/>
-      <c r="B67" s="77" t="s">
-        <v>37</v>
-      </c>
-      <c r="C67" s="101"/>
-      <c r="D67" s="87"/>
-      <c r="E67" s="42"/>
-      <c r="F67" s="42"/>
-      <c r="G67" s="42"/>
-      <c r="H67" s="42"/>
-      <c r="I67" s="43"/>
-    </row>
-    <row r="68" spans="1:9" s="44" customFormat="1" ht="72" x14ac:dyDescent="0.45">
-      <c r="A68" s="57"/>
-      <c r="B68" s="75" t="s">
-        <v>94</v>
-      </c>
-      <c r="C68" s="101" t="s">
-        <v>151</v>
-      </c>
-      <c r="D68" s="87"/>
-      <c r="E68" s="42"/>
-      <c r="F68" s="42"/>
-      <c r="G68" s="42"/>
-      <c r="H68" s="42"/>
-      <c r="I68" s="43"/>
-    </row>
-    <row r="69" spans="1:9" s="44" customFormat="1" ht="24" x14ac:dyDescent="0.45">
-      <c r="A69" s="57"/>
-      <c r="B69" s="75" t="s">
-        <v>95</v>
-      </c>
-      <c r="C69" s="101" t="s">
-        <v>162</v>
-      </c>
-      <c r="D69" s="87"/>
-      <c r="E69" s="42"/>
-      <c r="F69" s="42"/>
-      <c r="G69" s="42"/>
-      <c r="H69" s="42"/>
-      <c r="I69" s="43"/>
+      <c r="C67" s="109" t="s">
+        <v>154</v>
+      </c>
+      <c r="D67" s="96"/>
+      <c r="E67" s="48"/>
+      <c r="F67" s="48"/>
+      <c r="G67" s="48"/>
+      <c r="H67" s="48"/>
+      <c r="I67" s="49"/>
     </row>
   </sheetData>
   <sheetProtection deleteColumns="0" selectLockedCells="1"/>
@@ -2720,66 +2722,60 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="12">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0D2213F9-2AC5-4DB3-AF11-582BD913AFC1}">
-          <x14:formula1>
-            <xm:f>'Drop Down List Values'!$A$2:$A$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>D9</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="13">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2560A1C6-3FEA-4452-84E2-D4BC7FEE35BC}">
           <x14:formula1>
             <xm:f>'Drop Down List Values'!$B$2:$B$5</xm:f>
           </x14:formula1>
-          <xm:sqref>D10:H10</xm:sqref>
+          <xm:sqref>H10</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6714C258-4BD2-45CC-BA09-55489A06314D}">
           <x14:formula1>
             <xm:f>'Drop Down List Values'!$C$2:$C$5</xm:f>
           </x14:formula1>
-          <xm:sqref>D11:H11</xm:sqref>
+          <xm:sqref>H11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6EE5A822-FD38-4314-981B-8ED84EDD69EC}">
           <x14:formula1>
             <xm:f>'Drop Down List Values'!$E$2:$E$7</xm:f>
           </x14:formula1>
-          <xm:sqref>D32:H32</xm:sqref>
+          <xm:sqref>H32</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DC01C7B9-BA05-42AD-B9A9-F2FD4557F0F1}">
           <x14:formula1>
             <xm:f>'Drop Down List Values'!$F$2:$F$5</xm:f>
           </x14:formula1>
-          <xm:sqref>D36:H36</xm:sqref>
+          <xm:sqref>H36</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7CC0EF60-AEB4-4234-B37C-4A02B7E2DE3B}">
           <x14:formula1>
             <xm:f>'Drop Down List Values'!$G$2:$G$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D37:H37</xm:sqref>
+          <xm:sqref>H37</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D99AC123-497D-47BE-A346-1D3330E13BAC}">
           <x14:formula1>
             <xm:f>'Drop Down List Values'!$I$2:$I$6</xm:f>
           </x14:formula1>
-          <xm:sqref>D42:H42</xm:sqref>
+          <xm:sqref>H42</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2388147A-1FAB-42AF-9190-67DEDF83A4EA}">
           <x14:formula1>
             <xm:f>'Drop Down List Values'!$J$2:$J$7</xm:f>
           </x14:formula1>
-          <xm:sqref>D49:H49</xm:sqref>
+          <xm:sqref>H49</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{093E1169-867D-4A32-AC3C-DC58C26E3C39}">
           <x14:formula1>
             <xm:f>'Drop Down List Values'!$M$2:$M$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D69:H69</xm:sqref>
+          <xm:sqref>H67</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{33A578CF-33CA-4B41-B2C5-7541E5042FC9}">
           <x14:formula1>
             <xm:f>'Drop Down List Values'!$A$2:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>E9:H9</xm:sqref>
+          <xm:sqref>H9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{77990685-A35A-4CD2-A1C0-E931CAE699E2}">
           <x14:formula1>
@@ -2787,11 +2783,23 @@
           </x14:formula1>
           <xm:sqref>D41:H41</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E0C755F2-6856-4118-9F77-76F8475243FA}">
+          <x14:formula1>
+            <xm:f>'Drop Down List Values'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>D9 D10:G11 D32:G32 D36:G37 D49:G49 D67:G67 D46:G46 D42:G42</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{42CF6A8A-0F3A-4568-B9E2-BCEDE7FAF2A2}">
+          <x14:formula1>
+            <xm:f>'Drop Down List Values'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>E9:G9</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{38BD6F45-E1D6-4C47-97BB-112AE837004E}">
           <x14:formula1>
-            <xm:f>'Drop Down List Values'!K2:K4</xm:f>
+            <xm:f>'Drop Down List Values'!O2:O4</xm:f>
           </x14:formula1>
-          <xm:sqref>D46:H46</xm:sqref>
+          <xm:sqref>H46</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2803,28 +2811,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7F8BFBD-18C1-4ED5-A02E-9841686C259E}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="62" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="49.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="49.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -2832,19 +2840,19 @@
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H1" t="s">
         <v>25</v>
@@ -2853,205 +2861,205 @@
         <v>1</v>
       </c>
       <c r="J1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K1" t="s">
+        <v>130</v>
+      </c>
+      <c r="L1" t="s">
+        <v>149</v>
+      </c>
+      <c r="M1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J2" t="s">
+        <v>88</v>
+      </c>
+      <c r="K2" t="s">
+        <v>131</v>
+      </c>
+      <c r="L2" t="s">
+        <v>176</v>
+      </c>
+      <c r="M2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" t="s">
+        <v>68</v>
+      </c>
+      <c r="J3" t="s">
         <v>84</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K3" t="s">
+        <v>132</v>
+      </c>
+      <c r="L3" t="s">
+        <v>150</v>
+      </c>
+      <c r="M3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J4" t="s">
+        <v>85</v>
+      </c>
+      <c r="K4" t="s">
         <v>133</v>
       </c>
-      <c r="L1" t="s">
-        <v>156</v>
-      </c>
-      <c r="M1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="L4" t="s">
+        <v>151</v>
+      </c>
+      <c r="M4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
         <v>53</v>
       </c>
-      <c r="C2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H2" t="s">
-        <v>68</v>
-      </c>
-      <c r="I2" t="s">
-        <v>68</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="C5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" t="s">
+        <v>51</v>
+      </c>
+      <c r="J5" t="s">
+        <v>86</v>
+      </c>
+      <c r="L5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I6" t="s">
+        <v>74</v>
+      </c>
+      <c r="J6" t="s">
+        <v>87</v>
+      </c>
+      <c r="L6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" t="s">
+        <v>65</v>
+      </c>
+      <c r="J7" t="s">
         <v>89</v>
       </c>
-      <c r="K2" t="s">
-        <v>134</v>
-      </c>
-      <c r="L2" t="s">
-        <v>157</v>
-      </c>
-      <c r="M2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="L7" t="s">
         <v>69</v>
-      </c>
-      <c r="G3" t="s">
-        <v>72</v>
-      </c>
-      <c r="H3" t="s">
-        <v>69</v>
-      </c>
-      <c r="I3" t="s">
-        <v>69</v>
-      </c>
-      <c r="J3" t="s">
-        <v>85</v>
-      </c>
-      <c r="K3" t="s">
-        <v>135</v>
-      </c>
-      <c r="L3" t="s">
-        <v>158</v>
-      </c>
-      <c r="M3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F4" t="s">
-        <v>52</v>
-      </c>
-      <c r="G4" t="s">
-        <v>73</v>
-      </c>
-      <c r="H4" t="s">
-        <v>52</v>
-      </c>
-      <c r="I4" t="s">
-        <v>74</v>
-      </c>
-      <c r="J4" t="s">
-        <v>86</v>
-      </c>
-      <c r="K4" t="s">
-        <v>136</v>
-      </c>
-      <c r="L4" t="s">
-        <v>159</v>
-      </c>
-      <c r="M4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" t="s">
-        <v>70</v>
-      </c>
-      <c r="H5" t="s">
-        <v>70</v>
-      </c>
-      <c r="I5" t="s">
-        <v>52</v>
-      </c>
-      <c r="J5" t="s">
-        <v>87</v>
-      </c>
-      <c r="L5" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" t="s">
-        <v>65</v>
-      </c>
-      <c r="I6" t="s">
-        <v>75</v>
-      </c>
-      <c r="J6" t="s">
-        <v>88</v>
-      </c>
-      <c r="L6" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" t="s">
-        <v>66</v>
-      </c>
-      <c r="J7" t="s">
-        <v>90</v>
-      </c>
-      <c r="L7" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -3335,17 +3343,17 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69E3EF86-6C9E-4C22-A476-13DA012C68C5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="b541edd5-2552-480e-ada6-0e2c8d317108"/>
     <ds:schemaRef ds:uri="3146657c-56f4-4c0a-bb9c-a675121ac670"/>
     <ds:schemaRef ds:uri="780ae317-08c5-4e10-af93-dd385a8384a9"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="b541edd5-2552-480e-ada6-0e2c8d317108"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>